<commit_message>
updated with first jsonata codes in
</commit_message>
<xml_diff>
--- a/Maps/sdtm_mapping_paths.xlsx
+++ b/Maps/sdtm_mapping_paths.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL032\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\SDTM_mapper\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E270DB-1A17-4916-A518-07F2B848A589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6588ED97-C8A4-40ED-B8AC-C302C38C8CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-11955" yWindow="-21720" windowWidth="51840" windowHeight="21120" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="471">
   <si>
     <t>Class</t>
   </si>
@@ -1281,15 +1281,9 @@
     <t>Study Minimum Age + Unit Study Population</t>
   </si>
   <si>
-    <t>Study Minimum Age + Unit Study Cohort</t>
-  </si>
-  <si>
     <t>Study Maximum Age + Unit Study Population</t>
   </si>
   <si>
-    <t>Study Maximum Age + Unit Study Cohort</t>
-  </si>
-  <si>
     <t>Biospecimen retention contains DNA indicator</t>
   </si>
   <si>
@@ -1332,9 +1326,6 @@
     <t>Sponsor Name - Organization</t>
   </si>
   <si>
-    <t>Sponsor Name - Person</t>
-  </si>
-  <si>
     <t>Single Site Eu State Trial Indicator</t>
   </si>
   <si>
@@ -1414,13 +1405,300 @@
   </si>
   <si>
     <t>JSONATA</t>
+  </si>
+  <si>
+    <r>
+      <t>$exists</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>study</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>versions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>studyDesigns</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>characteristics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"C98704"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>])</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ? "Y" : ""</t>
+    </r>
+  </si>
+  <si>
+    <t>$min([study.versions.studyDesigns.population.plannedAge.minValue.value,study.versions.studyDesigns.population.cohorts.plannedAge.minValue.value]) &amp; " " &amp; 
+study.versions.studyDesigns.population.plannedAge.minValue.unit.standardCode.decode &amp; " " &amp; study.versions.studyDesigns.population.cohorts.plannedAge.minValue.unit.standardCode.decode</t>
+  </si>
+  <si>
+    <t>$max([study.versions.studyDesigns.population.plannedAge.maxValue.value,study.versions.studyDesigns.population.cohorts.plannedAge.maxValue.value]) &amp; " " &amp; 
+study.versions.studyDesigns.population.plannedAge.maxValue.unit.standardCode.decode &amp; " " &amp; study.versions.studyDesigns.population.cohorts.plannedAge.maxValue.unit.standardCode.decode</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.biospecimenRetentions.includesDNA</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.biospecimenRetentions.isRetained</t>
+  </si>
+  <si>
+    <t>study.versions.titles[type.code="C207616"].text</t>
+  </si>
+  <si>
+    <t>study.study.versions.studyDesigns.studyPhase.standardCode.decode</t>
+  </si>
+  <si>
+    <t>study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0];</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C98388"].model.decode</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.indications.label</t>
+  </si>
+  <si>
+    <r>
+      <t>$count</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>study</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>versions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>studyDesigns</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>arms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.blindingSchema.standardCode.decode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">study.versions.studyDesigns.population.plannedEnrollmentNumber.value </t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.objectives[level.code="C85826"].text</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.objectives[level.code="C85827"].text</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.objectives[level.code="C163559"].text</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions.type.decode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1476,8 +1754,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFA00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1505,6 +1810,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1612,7 +1923,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1699,6 +2010,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1711,8 +2025,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2033,34 +2353,34 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B7" s="17"/>
     </row>
@@ -2069,7 +2389,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="31" x14ac:dyDescent="0.35">
@@ -2077,7 +2397,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -2085,7 +2405,7 @@
         <v>79</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="31" x14ac:dyDescent="0.35">
@@ -2093,7 +2413,7 @@
         <v>56</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -2101,7 +2421,7 @@
         <v>58</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -2109,7 +2429,7 @@
         <v>57</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -2117,7 +2437,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -2125,29 +2445,29 @@
         <v>60</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B18" s="17"/>
     </row>
     <row r="20" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -2177,26 +2497,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="33" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -2723,26 +3043,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="33" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -2905,7 +3225,7 @@
         <v>389</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>391</v>
@@ -2951,7 +3271,7 @@
         <v>389</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>391</v>
@@ -3137,26 +3457,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="33" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -3652,26 +3972,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="33" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -4103,26 +4423,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="33" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -4542,7 +4862,7 @@
         <v>389</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="N13" s="5" t="s">
         <v>391</v>
@@ -4567,10 +4887,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DEA66B-9A3B-A542-95A2-9E48A8B13E1D}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="182" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="182" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4581,7 +4901,7 @@
     <col min="4" max="4" width="28.6328125" customWidth="1"/>
     <col min="5" max="5" width="33.81640625" customWidth="1"/>
     <col min="6" max="6" width="32.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.54296875" customWidth="1"/>
+    <col min="7" max="7" width="85.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
@@ -4603,8 +4923,8 @@
       <c r="F1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="34" t="s">
-        <v>456</v>
+      <c r="G1" s="30" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -4622,8 +4942,11 @@
       <c r="F2" s="14" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="G2" s="35" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>185</v>
       </c>
@@ -4638,184 +4961,200 @@
       <c r="F3" s="14" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="G3" s="35" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>185</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="14" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="G4" s="35" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
+        <v>192</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>194</v>
+      </c>
       <c r="F5" s="14" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="G5" s="35" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
+        <v>197</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>198</v>
+      </c>
       <c r="F6" s="14" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="G6" s="35" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>193</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>193</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>193</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>193</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>193</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>215</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
       <c r="F12" s="14" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>193</v>
@@ -4824,34 +5163,38 @@
         <v>219</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
+        <v>228</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>219</v>
+      </c>
       <c r="F14" s="14" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>193</v>
@@ -4860,18 +5203,18 @@
         <v>219</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>193</v>
@@ -4880,256 +5223,274 @@
         <v>219</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>219</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
       <c r="F17" s="14" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="E18" s="15" t="s">
-        <v>219</v>
-      </c>
+      <c r="E18" s="15"/>
       <c r="F18" s="14" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>193</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>421</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="14" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+        <v>247</v>
+      </c>
+      <c r="G22" s="36" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
+        <v>252</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>219</v>
+      </c>
       <c r="F23" s="14" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>250</v>
+      </c>
+      <c r="G23" s="35" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
-      <c r="F24" s="14" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F24" s="13" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>252</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>219</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
       <c r="F25" s="14" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
-      <c r="F26" s="13" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="F26" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="G26" s="35" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
       <c r="F27" s="14" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
       <c r="F28" s="14" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
+        <v>271</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>274</v>
+      </c>
       <c r="F29" s="14" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+      <c r="G29" s="37" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
+        <v>277</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>274</v>
+      </c>
       <c r="F30" s="14" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>278</v>
+      </c>
+      <c r="G30" s="37" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>273</v>
@@ -5138,122 +5499,125 @@
         <v>274</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>282</v>
+      </c>
+      <c r="G31" s="37" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>277</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>273</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>274</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
       <c r="F32" s="14" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>281</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>273</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>274</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
       <c r="F33" s="14" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
       <c r="F34" s="14" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="15" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
       <c r="F35" s="14" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="15" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>291</v>
-      </c>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
+        <v>297</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>299</v>
+      </c>
       <c r="F36" s="14" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
+        <v>302</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>299</v>
+      </c>
       <c r="F37" s="14" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="15" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>298</v>
@@ -5262,438 +5626,397 @@
         <v>299</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="15" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>298</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="D39" s="15"/>
       <c r="E39" s="15" t="s">
-        <v>299</v>
+        <v>219</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="15" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="E40" s="15" t="s">
-        <v>299</v>
-      </c>
+        <v>311</v>
+      </c>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
       <c r="F40" s="14" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A41" s="15" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="G41" s="35" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="F41" s="14" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>310</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
       <c r="F42" s="14" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="20"/>
       <c r="F43" s="14" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="14" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>329</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>330</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A47" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="14" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A49" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="19" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>316</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>317</v>
-      </c>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="14" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="15" t="s">
-        <v>322</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>323</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>324</v>
-      </c>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="14" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="15" t="s">
-        <v>326</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>327</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>328</v>
-      </c>
-      <c r="D47" s="20" t="s">
+      <c r="G49" s="36" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A50" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="D50" s="20" t="s">
         <v>329</v>
       </c>
-      <c r="E47" s="20" t="s">
-        <v>330</v>
-      </c>
-      <c r="F47" s="14" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="15" t="s">
-        <v>331</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>332</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>333</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="F48" s="14" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A49" s="15" t="s">
-        <v>334</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>335</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>336</v>
-      </c>
-      <c r="D49" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="E49" s="20" t="s">
-        <v>337</v>
-      </c>
-      <c r="F49" s="14" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="15" t="s">
-        <v>338</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>339</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>340</v>
-      </c>
-      <c r="D50" s="20"/>
       <c r="E50" s="20"/>
       <c r="F50" s="14" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="15" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="20"/>
-      <c r="F51" s="19" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="F51" s="14" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="15" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="20"/>
-      <c r="F52" s="19" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="F52" s="14" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A53" s="15" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>346</v>
-      </c>
-      <c r="D53" s="20" t="s">
-        <v>329</v>
-      </c>
+        <v>356</v>
+      </c>
+      <c r="D53" s="20"/>
       <c r="E53" s="20"/>
       <c r="F53" s="14" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>357</v>
+      </c>
+      <c r="G53" s="35" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="15" t="s">
-        <v>347</v>
+        <v>358</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>348</v>
+        <v>359</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>349</v>
-      </c>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
+        <v>360</v>
+      </c>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
       <c r="F54" s="14" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="15" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>351</v>
+        <v>363</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>352</v>
-      </c>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
+        <v>364</v>
+      </c>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
       <c r="F55" s="14" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="15" t="s">
-        <v>354</v>
+        <v>365</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>355</v>
+        <v>366</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>356</v>
-      </c>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
+        <v>367</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>369</v>
+      </c>
+      <c r="E56" s="15"/>
       <c r="F56" s="14" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="15" t="s">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>360</v>
+        <v>372</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57" s="15"/>
       <c r="F57" s="14" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+        <v>373</v>
+      </c>
+      <c r="G57" s="35" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="15" t="s">
-        <v>362</v>
+        <v>374</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>363</v>
+        <v>375</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
       <c r="F58" s="14" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>377</v>
+      </c>
+      <c r="G58" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="15" t="s">
-        <v>365</v>
+        <v>378</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>366</v>
+        <v>379</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>367</v>
+        <v>380</v>
       </c>
       <c r="D59" s="15" t="s">
         <v>369</v>
       </c>
-      <c r="E59" s="15"/>
+      <c r="E59" s="15" t="s">
+        <v>219</v>
+      </c>
       <c r="F59" s="14" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="15" t="s">
-        <v>370</v>
+        <v>382</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>371</v>
+        <v>383</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>372</v>
+        <v>384</v>
       </c>
       <c r="D60" s="15"/>
       <c r="E60" s="15"/>
       <c r="F60" s="14" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A61" s="15" t="s">
-        <v>374</v>
-      </c>
-      <c r="B61" s="15" t="s">
-        <v>375</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>376</v>
-      </c>
-      <c r="D61" s="15"/>
-      <c r="E61" s="15"/>
-      <c r="F61" s="14" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="15" t="s">
-        <v>378</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>379</v>
-      </c>
-      <c r="C62" s="15" t="s">
-        <v>380</v>
-      </c>
-      <c r="D62" s="15" t="s">
-        <v>369</v>
-      </c>
-      <c r="E62" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="F62" s="14" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" s="15" t="s">
-        <v>382</v>
-      </c>
-      <c r="B63" s="15" t="s">
-        <v>383</v>
-      </c>
-      <c r="C63" s="15" t="s">
-        <v>384</v>
-      </c>
-      <c r="D63" s="15"/>
-      <c r="E63" s="15"/>
-      <c r="F63" s="14" t="s">
         <v>385</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added commas to code for testing
</commit_message>
<xml_diff>
--- a/Maps/sdtm_mapping_paths.xlsx
+++ b/Maps/sdtm_mapping_paths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\SDTM_mapper\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6588ED97-C8A4-40ED-B8AC-C302C38C8CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EDE078-5246-49F7-95FD-4183013F0D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11955" yWindow="-21720" windowWidth="51840" windowHeight="21120" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6285" yWindow="-16830" windowWidth="27840" windowHeight="14760" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -1923,7 +1923,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2013,6 +2013,15 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2025,13 +2034,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2497,26 +2500,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="34" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -3043,26 +3046,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="34" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -3457,26 +3460,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="34" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -3972,26 +3975,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="34" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -4423,26 +4426,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="34" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -4889,8 +4892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DEA66B-9A3B-A542-95A2-9E48A8B13E1D}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="182" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="182" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4942,7 +4945,7 @@
       <c r="F2" s="14" t="s">
         <v>410</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="38" t="s">
         <v>454</v>
       </c>
     </row>
@@ -4961,7 +4964,7 @@
       <c r="F3" s="14" t="s">
         <v>411</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="38" t="s">
         <v>455</v>
       </c>
     </row>
@@ -4980,7 +4983,7 @@
       <c r="F4" s="14" t="s">
         <v>412</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="31" t="s">
         <v>456</v>
       </c>
     </row>
@@ -5003,7 +5006,7 @@
       <c r="F5" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="31" t="s">
         <v>457</v>
       </c>
     </row>
@@ -5026,7 +5029,7 @@
       <c r="F6" s="14" t="s">
         <v>414</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="31" t="s">
         <v>458</v>
       </c>
     </row>
@@ -5307,7 +5310,7 @@
       <c r="F21" s="14" t="s">
         <v>421</v>
       </c>
-      <c r="G21" s="35" t="s">
+      <c r="G21" s="31" t="s">
         <v>463</v>
       </c>
     </row>
@@ -5326,7 +5329,7 @@
       <c r="F22" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="G22" s="36" t="s">
+      <c r="G22" s="32" t="s">
         <v>462</v>
       </c>
     </row>
@@ -5349,7 +5352,7 @@
       <c r="F23" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="G23" s="35" t="s">
+      <c r="G23" s="31" t="s">
         <v>470</v>
       </c>
     </row>
@@ -5400,7 +5403,7 @@
       <c r="F26" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="G26" s="35" t="s">
+      <c r="G26" s="31" t="s">
         <v>464</v>
       </c>
     </row>
@@ -5455,7 +5458,7 @@
       <c r="F29" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="G29" s="37" t="s">
+      <c r="G29" s="33" t="s">
         <v>469</v>
       </c>
     </row>
@@ -5478,7 +5481,7 @@
       <c r="F30" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="G30" s="37" t="s">
+      <c r="G30" s="33" t="s">
         <v>467</v>
       </c>
     </row>
@@ -5501,7 +5504,7 @@
       <c r="F31" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="G31" s="37" t="s">
+      <c r="G31" s="33" t="s">
         <v>468</v>
       </c>
     </row>
@@ -5678,7 +5681,7 @@
       <c r="F41" s="14" t="s">
         <v>424</v>
       </c>
-      <c r="G41" s="35" t="s">
+      <c r="G41" s="31" t="s">
         <v>466</v>
       </c>
     </row>
@@ -5823,7 +5826,7 @@
       <c r="F49" s="19" t="s">
         <v>426</v>
       </c>
-      <c r="G49" s="36" t="s">
+      <c r="G49" s="32" t="s">
         <v>461</v>
       </c>
     </row>
@@ -5892,7 +5895,7 @@
       <c r="F53" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="G53" s="35" t="s">
+      <c r="G53" s="31" t="s">
         <v>465</v>
       </c>
     </row>
@@ -5961,7 +5964,7 @@
       <c r="F57" s="14" t="s">
         <v>373</v>
       </c>
-      <c r="G57" s="35" t="s">
+      <c r="G57" s="31" t="s">
         <v>459</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update mapping for testing
</commit_message>
<xml_diff>
--- a/Maps/sdtm_mapping_paths.xlsx
+++ b/Maps/sdtm_mapping_paths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\SDTM_mapper\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EDE078-5246-49F7-95FD-4183013F0D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0757A6D-F9F1-4285-849F-88F1B2AD2CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6285" yWindow="-16830" windowWidth="27840" windowHeight="14760" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6360" yWindow="-16350" windowWidth="30300" windowHeight="11235" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="472">
   <si>
     <t>Class</t>
   </si>
@@ -1552,10 +1552,6 @@
     </r>
   </si>
   <si>
-    <t>$min([study.versions.studyDesigns.population.plannedAge.minValue.value,study.versions.studyDesigns.population.cohorts.plannedAge.minValue.value]) &amp; " " &amp; 
-study.versions.studyDesigns.population.plannedAge.minValue.unit.standardCode.decode &amp; " " &amp; study.versions.studyDesigns.population.cohorts.plannedAge.minValue.unit.standardCode.decode</t>
-  </si>
-  <si>
     <t>$max([study.versions.studyDesigns.population.plannedAge.maxValue.value,study.versions.studyDesigns.population.cohorts.plannedAge.maxValue.value]) &amp; " " &amp; 
 study.versions.studyDesigns.population.plannedAge.maxValue.unit.standardCode.decode &amp; " " &amp; study.versions.studyDesigns.population.cohorts.plannedAge.maxValue.unit.standardCode.decode</t>
   </si>
@@ -1692,6 +1688,13 @@
   </si>
   <si>
     <t>study.versions.studyInterventions.type.decode</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>("$min([study.versions.studyDesigns.population.plannedAge.minValue.value,study.versions.studyDesigns.population.cohorts.plannedAge.minValue.value]) &amp; " " &amp; 
+study.versions.studyDesigns.population.plannedAge.minValue.unit.standardCode.decode &amp; " " &amp; study.versions.studyDesigns.population.cohorts.plannedAge.minValue.unit.standardCode.decode")</t>
   </si>
 </sst>
 </file>
@@ -2022,6 +2025,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2033,9 +2039,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2500,26 +2503,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="37" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -3046,26 +3049,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="37" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -3460,26 +3463,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="37" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -3975,26 +3978,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="37" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -4426,26 +4429,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="37" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -4893,7 +4896,7 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="182" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4905,6 +4908,7 @@
     <col min="5" max="5" width="33.81640625" customWidth="1"/>
     <col min="6" max="6" width="32.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="85.54296875" customWidth="1"/>
+    <col min="8" max="8" width="52.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
@@ -4945,7 +4949,7 @@
       <c r="F2" s="14" t="s">
         <v>410</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="34" t="s">
         <v>454</v>
       </c>
     </row>
@@ -4964,8 +4968,8 @@
       <c r="F3" s="14" t="s">
         <v>411</v>
       </c>
-      <c r="G3" s="38" t="s">
-        <v>455</v>
+      <c r="G3" s="34" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="58" x14ac:dyDescent="0.35">
@@ -4984,7 +4988,7 @@
         <v>412</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="58" x14ac:dyDescent="0.35">
@@ -5007,7 +5011,7 @@
         <v>413</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
@@ -5030,7 +5034,7 @@
         <v>414</v>
       </c>
       <c r="G6" s="31" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -5051,6 +5055,9 @@
       </c>
       <c r="F7" s="14" t="s">
         <v>415</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -5311,7 +5318,7 @@
         <v>421</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -5330,7 +5337,7 @@
         <v>247</v>
       </c>
       <c r="G22" s="32" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -5353,7 +5360,7 @@
         <v>250</v>
       </c>
       <c r="G23" s="31" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -5404,7 +5411,7 @@
         <v>262</v>
       </c>
       <c r="G26" s="31" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -5459,7 +5466,7 @@
         <v>272</v>
       </c>
       <c r="G29" s="33" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -5482,7 +5489,7 @@
         <v>278</v>
       </c>
       <c r="G30" s="33" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -5505,7 +5512,7 @@
         <v>282</v>
       </c>
       <c r="G31" s="33" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -5682,7 +5689,7 @@
         <v>424</v>
       </c>
       <c r="G41" s="31" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -5827,7 +5834,7 @@
         <v>426</v>
       </c>
       <c r="G49" s="32" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -5896,7 +5903,7 @@
         <v>357</v>
       </c>
       <c r="G53" s="31" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
@@ -5965,7 +5972,7 @@
         <v>373</v>
       </c>
       <c r="G57" s="31" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -5984,7 +5991,7 @@
         <v>377</v>
       </c>
       <c r="G58" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
row 3 again corrected
</commit_message>
<xml_diff>
--- a/Maps/sdtm_mapping_paths.xlsx
+++ b/Maps/sdtm_mapping_paths.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\SDTM_mapper\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF815108-A3EE-4142-BAC1-0163E2909E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5217ED70-5068-4199-AE4E-161E6E2ACBE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1694,7 +1694,7 @@
   </si>
   <si>
     <t>$min([study.versions.studyDesigns.population.plannedAge.minValue.value,study.versions.studyDesigns.population.cohorts.plannedAge.minValue.value]) &amp; " " &amp; 
-study.versions.studyDesigns.population.plannedAge.minValue.unit.standardCode.decode &amp; " " &amp; study.versions.studyDesigns.population.cohorts.plannedAge.minValue.unit.standardCode.decode"</t>
+study.versions.studyDesigns.population.plannedAge.minValue.unit.standardCode.decode &amp; " " &amp; study.versions.studyDesigns.population.cohorts.plannedAge.minValue.unit.standardCode.decode</t>
   </si>
 </sst>
 </file>
@@ -4896,7 +4896,7 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="182" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added more jsonata mappings
</commit_message>
<xml_diff>
--- a/Maps/sdtm_mapping_paths.xlsx
+++ b/Maps/sdtm_mapping_paths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\SDTM_mapper\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951C7312-F680-4361-967A-62938176B3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20B6780-8A36-456B-B0B7-BC55D5FD391B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38040" yWindow="-10920" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12030" yWindow="-21600" windowWidth="30435" windowHeight="20985" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,9 @@
     <sheet name="TS" sheetId="7" r:id="rId6"/>
     <sheet name="TS Parameters" sheetId="10" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'TS Parameters'!$A$1:$G$60</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="483">
   <si>
     <t>Class</t>
   </si>
@@ -504,18 +507,12 @@
     <t>Subcategory is not mandatory. If beneficial, we advice to store it in the EligibilityCriterion notes according to an internal codelist used for the purpose.</t>
   </si>
   <si>
-    <t>Set to "TS"</t>
-  </si>
-  <si>
     <t>TSSEQ</t>
   </si>
   <si>
     <t>Sequence Number</t>
   </si>
   <si>
-    <t xml:space="preserve">Will be mapped per trial summary parameter </t>
-  </si>
-  <si>
     <t>TSGRPID</t>
   </si>
   <si>
@@ -543,9 +540,6 @@
     <t>Result Qualifier</t>
   </si>
   <si>
-    <t>Will be mapped per trial summary parameter. When the mapping resolved to Yes or No values, then the corresponding CDISC CT codes need to be used; TSVAL="Y" and TSVALCD="C49488" or TSVAL="N" and TSVALCD="C49487" </t>
-  </si>
-  <si>
     <t>TSVALNF</t>
   </si>
   <si>
@@ -564,30 +558,12 @@
     <t>Name of Reference Terminology</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>codeSystem</t>
-  </si>
-  <si>
-    <t>code/@codeSystem</t>
-  </si>
-  <si>
-    <t>Align path to the corresponding code or decode mapped for the specific code item it refers to.</t>
-  </si>
-  <si>
     <t>TSVCDVER</t>
   </si>
   <si>
     <t>Version of the Reference Terminology</t>
   </si>
   <si>
-    <t>codeSystemVersion</t>
-  </si>
-  <si>
-    <t>code/@codeSystemVersion</t>
-  </si>
-  <si>
     <t xml:space="preserve">TSSEQ </t>
   </si>
   <si>
@@ -687,9 +663,6 @@
     <t>C98715</t>
   </si>
   <si>
-    <t>Mimimum Response Duration</t>
-  </si>
-  <si>
     <t>If applicable, combine with the corresponding intervention variables by a common unique TSGRPID</t>
   </si>
   <si>
@@ -1288,9 +1261,6 @@
   </si>
   <si>
     <t>Biospecimen retention indicator</t>
-  </si>
-  <si>
-    <t>(International) Non Proprietary Comparator Drug Name</t>
   </si>
   <si>
     <t>Background treatment</t>
@@ -1678,12 +1648,6 @@
     <t xml:space="preserve">study.versions.studyDesigns.population.plannedEnrollmentNumber.value </t>
   </si>
   <si>
-    <t>study.versions.studyInterventions.type.decode</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>$min([study.versions.studyDesigns.population.plannedAge.minValue.value,study.versions.studyDesigns.population.cohorts.plannedAge.minValue.value]) &amp; " " &amp; 
 study.versions.studyDesigns.population.plannedAge.minValue.unit.standardCode.decode &amp; " " &amp; study.versions.studyDesigns.population.cohorts.plannedAge.minValue.unit.standardCode.decode</t>
   </si>
@@ -1716,6 +1680,58 @@
   </si>
   <si>
     <t>study.versions.studyDesigns.objectives[level.code="C163559"].{id: objectives.endpoint.text}</t>
+  </si>
+  <si>
+    <t>study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0];
+studyIdentifiers[scopeId=$sponsorIdVal].text;)</t>
+  </si>
+  <si>
+    <t>Fixed content</t>
+  </si>
+  <si>
+    <t>"TS"</t>
+  </si>
+  <si>
+    <t>..code.codeSystem</t>
+  </si>
+  <si>
+    <t>..code.codeSystemVersion</t>
+  </si>
+  <si>
+    <t>Minimum Response Duration</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions.{id: minimumResponseDuration.value &amp; " " &amp; minimumResponseDuration.unit.standardCode.decode}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions[role.code="C165822"].{id: label}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions[role.code="C41161"].{id: label}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: type.decode}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.duration.quantity.value &amp; " " &amp; administrations.duration.quantity.unit.standardCode.decode}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: role[code="C753"].decode ? role[code="C753"].decode : role[code="C68609"].decode}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.administrableProduct.administrableDoseForm.standardCode.decode}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.dose.value}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.dose.unit.standardCode.decode}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.frequency.standardCode.decode}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions[role.code="C68609"].{id: label}</t>
   </si>
 </sst>
 </file>
@@ -2028,12 +2044,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2043,12 +2053,10 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2061,7 +2069,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2381,34 +2395,34 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>451</v>
+        <v>440</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>448</v>
+        <v>437</v>
       </c>
       <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>447</v>
+        <v>436</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="B7" s="17"/>
     </row>
@@ -2417,7 +2431,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="31" x14ac:dyDescent="0.35">
@@ -2425,7 +2439,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -2433,7 +2447,7 @@
         <v>79</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="31" x14ac:dyDescent="0.35">
@@ -2441,7 +2455,7 @@
         <v>56</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -2449,7 +2463,7 @@
         <v>58</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -2457,7 +2471,7 @@
         <v>57</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -2465,7 +2479,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -2473,29 +2487,29 @@
         <v>60</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
       <c r="B18" s="17"/>
     </row>
     <row r="20" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -2525,26 +2539,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="38" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -2700,19 +2714,19 @@
         <v>68</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="O5" s="8" t="s">
         <v>66</v>
@@ -2746,19 +2760,19 @@
         <v>69</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="O6" s="8" t="s">
         <v>66</v>
@@ -2795,16 +2809,16 @@
         <v>77</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="O7" s="8" t="s">
         <v>66</v>
@@ -2840,19 +2854,19 @@
         <v>72</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="O8" s="8" t="s">
         <v>66</v>
@@ -2888,19 +2902,19 @@
         <v>73</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="O9" s="8" t="s">
         <v>66</v>
@@ -2966,16 +2980,16 @@
         <v>74</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="L11" s="7" t="s">
         <v>78</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="O11" s="8" t="s">
         <v>66</v>
@@ -3011,19 +3025,19 @@
         <v>75</v>
       </c>
       <c r="J12" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="M12" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="K12" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>399</v>
-      </c>
       <c r="N12" s="7" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="O12" s="8" t="s">
         <v>66</v>
@@ -3071,26 +3085,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="38" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -3244,19 +3258,19 @@
         <v>72</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>66</v>
@@ -3290,19 +3304,19 @@
         <v>73</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="O6" s="4" t="s">
         <v>66</v>
@@ -3336,19 +3350,19 @@
         <v>100</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="O7" s="4" t="s">
         <v>66</v>
@@ -3382,19 +3396,19 @@
         <v>101</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="O8" s="4" t="s">
         <v>66</v>
@@ -3431,16 +3445,16 @@
         <v>103</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="O9" s="4" t="s">
         <v>66</v>
@@ -3485,26 +3499,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="38" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -3662,16 +3676,16 @@
         <v>128</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>105</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>66</v>
@@ -3707,19 +3721,19 @@
         <v>123</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>108</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>66</v>
@@ -3755,19 +3769,19 @@
         <v>124</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>110</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="O7" s="6" t="s">
         <v>66</v>
@@ -3803,19 +3817,19 @@
         <v>68</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="O8" s="6" t="s">
         <v>66</v>
@@ -3851,19 +3865,19 @@
         <v>69</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="O9" s="6" t="s">
         <v>66</v>
@@ -3899,19 +3913,19 @@
         <v>125</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M10" s="6" t="s">
         <v>116</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="O10" s="6" t="s">
         <v>66</v>
@@ -3947,19 +3961,19 @@
         <v>126</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>118</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="O11" s="6" t="s">
         <v>66</v>
@@ -4000,26 +4014,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="38" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -4171,22 +4185,22 @@
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="12" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>131</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>66</v>
@@ -4219,22 +4233,22 @@
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="12" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>133</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="O6" s="4" t="s">
         <v>66</v>
@@ -4267,22 +4281,22 @@
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="12" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>135</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="O7" s="4" t="s">
         <v>66</v>
@@ -4315,22 +4329,22 @@
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="12" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>152</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>137</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="O8" s="4" t="s">
         <v>66</v>
@@ -4398,13 +4412,13 @@
         <v>150</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>141</v>
@@ -4432,102 +4446,80 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF8120D-B51B-094C-AABA-CA55EB26DD5D}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="14.6328125" style="16" customWidth="1"/>
-    <col min="6" max="7" width="21.453125" style="16" customWidth="1"/>
-    <col min="8" max="8" width="39" style="16" customWidth="1"/>
-    <col min="9" max="10" width="21.453125" style="16" customWidth="1"/>
-    <col min="11" max="12" width="32.6328125" style="16" customWidth="1"/>
-    <col min="13" max="15" width="21.453125" style="16" customWidth="1"/>
-    <col min="16" max="16" width="17.36328125" style="29" customWidth="1"/>
-    <col min="17" max="16384" width="8.6328125" style="16"/>
+    <col min="1" max="1" width="19.7265625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.6328125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="21.453125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="26.6328125" style="16" customWidth="1"/>
+    <col min="8" max="8" width="29.81640625" style="16" customWidth="1"/>
+    <col min="9" max="16384" width="8.6328125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-    </row>
-    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="N2" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="P2" s="24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G1" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>466</v>
+      </c>
+      <c r="H2" s="39"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>82</v>
@@ -4538,45 +4530,21 @@
       <c r="E3" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="P3" s="26" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="F3" s="5"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="9" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>84</v>
+        <v>153</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>85</v>
+        <v>154</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>8</v>
@@ -4584,51 +4552,31 @@
       <c r="E4" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="28"/>
-    </row>
-    <row r="5" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="F4" s="12"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="39"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="28"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="G5" s="38"/>
+      <c r="H5" s="39"/>
+    </row>
+    <row r="6" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>157</v>
       </c>
@@ -4639,26 +4587,16 @@
         <v>82</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>8</v>
+        <v>88</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="28"/>
-    </row>
-    <row r="7" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G6" s="38"/>
+      <c r="H6" s="39"/>
+    </row>
+    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>159</v>
       </c>
@@ -4669,26 +4607,16 @@
         <v>82</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>83</v>
       </c>
       <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="28"/>
-    </row>
-    <row r="8" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="G7" s="38"/>
+      <c r="H7" s="39"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>161</v>
       </c>
@@ -4699,216 +4627,104 @@
         <v>82</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>91</v>
+        <v>163</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="28"/>
-    </row>
-    <row r="9" spans="1:16" ht="87" x14ac:dyDescent="0.35">
+      <c r="G8" s="38"/>
+      <c r="H8" s="39"/>
+    </row>
+    <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>82</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12" t="s">
+      <c r="G9" s="38"/>
+      <c r="H9" s="39"/>
+    </row>
+    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="28"/>
-    </row>
-    <row r="10" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+      <c r="B10" s="9" t="s">
         <v>167</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>168</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>82</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="28"/>
-    </row>
-    <row r="11" spans="1:16" ht="87" x14ac:dyDescent="0.35">
+      <c r="G10" s="38"/>
+      <c r="H10" s="39"/>
+    </row>
+    <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>170</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>82</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="28"/>
-    </row>
-    <row r="12" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F11" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>469</v>
+      </c>
+      <c r="H11" s="39"/>
+    </row>
+    <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>171</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>172</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>82</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>389</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>391</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="P12" s="28"/>
-    </row>
-    <row r="13" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>389</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="M13" s="12" t="s">
-        <v>430</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>391</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="P13" s="28"/>
+        <v>419</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>470</v>
+      </c>
+      <c r="H12" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:P1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="I12" r:id="rId1" xr:uid="{D20F41AD-B0B1-D04B-BAE8-CE6916F58919}"/>
-    <hyperlink ref="I13" r:id="rId2" xr:uid="{4746AD37-6FEA-6440-AD2D-0A3AF707FA3C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4917,8 +4733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DEA66B-9A3B-A542-95A2-9E48A8B13E1D}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="182" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4935,1145 +4751,1171 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="30" t="s">
-        <v>453</v>
+      <c r="G1" s="28" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="14" t="s">
-        <v>410</v>
-      </c>
-      <c r="G2" s="34" t="s">
-        <v>454</v>
+        <v>400</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="14" t="s">
-        <v>411</v>
-      </c>
-      <c r="G3" s="34" t="s">
-        <v>468</v>
+        <v>401</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="G4" s="31" t="s">
-        <v>455</v>
+        <v>402</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>413</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>456</v>
+        <v>403</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>414</v>
-      </c>
-      <c r="G6" s="31" t="s">
-        <v>457</v>
+        <v>404</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D7" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>415</v>
-      </c>
-      <c r="G7" s="31" t="s">
-        <v>467</v>
+      <c r="F7" s="14"/>
+      <c r="G7" s="29" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>214</v>
+        <v>471</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>416</v>
+        <v>405</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="14" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>417</v>
+        <v>406</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>226</v>
+        <v>216</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>418</v>
+        <v>407</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>419</v>
+        <v>408</v>
+      </c>
+      <c r="G16" s="29" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="14" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="14" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="14" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="14" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="14" t="s">
-        <v>421</v>
-      </c>
-      <c r="G21" s="31" t="s">
-        <v>462</v>
+        <v>410</v>
+      </c>
+      <c r="G21" s="29" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="G22" s="32" t="s">
-        <v>461</v>
+        <v>237</v>
+      </c>
+      <c r="G22" s="30" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="G23" s="31" t="s">
-        <v>466</v>
+        <v>240</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="13" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
       <c r="F25" s="14" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
       <c r="F26" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="G26" s="31" t="s">
-        <v>463</v>
+        <v>252</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
       <c r="F27" s="14" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
       <c r="F28" s="14" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="G29" s="33" t="s">
-        <v>475</v>
+        <v>262</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="G30" s="33" t="s">
-        <v>473</v>
+        <v>268</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="G31" s="33" t="s">
-        <v>474</v>
+        <v>272</v>
+      </c>
+      <c r="G31" s="29" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
       <c r="F32" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="G32" s="39" t="s">
-        <v>469</v>
+        <v>273</v>
+      </c>
+      <c r="G32" s="32" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
       <c r="F33" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="G33" s="32" t="s">
-        <v>470</v>
+        <v>276</v>
+      </c>
+      <c r="G33" s="30" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
       <c r="F34" s="14" t="s">
-        <v>423</v>
-      </c>
-      <c r="G34" s="32" t="s">
-        <v>471</v>
+        <v>412</v>
+      </c>
+      <c r="G34" s="30" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="15" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
       <c r="F35" s="14" t="s">
-        <v>292</v>
-      </c>
-      <c r="G35" s="32" t="s">
-        <v>472</v>
+        <v>282</v>
+      </c>
+      <c r="G35" s="30" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="15" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>295</v>
-      </c>
-      <c r="G36" s="31" t="s">
-        <v>478</v>
+        <v>285</v>
+      </c>
+      <c r="G36" s="29" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="G37" s="31" t="s">
-        <v>476</v>
+        <v>290</v>
+      </c>
+      <c r="G37" s="29" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="15" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>303</v>
-      </c>
-      <c r="G38" s="31" t="s">
-        <v>477</v>
+        <v>293</v>
+      </c>
+      <c r="G38" s="29" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="15" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="15" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="15" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="20"/>
       <c r="F40" s="14" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A41" s="15" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="20"/>
       <c r="F41" s="14" t="s">
-        <v>424</v>
-      </c>
-      <c r="G41" s="31" t="s">
-        <v>465</v>
+        <v>413</v>
+      </c>
+      <c r="G41" s="29" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A42" s="15" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="20" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>425</v>
+        <v>414</v>
+      </c>
+      <c r="G42" s="30" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="20"/>
       <c r="F43" s="14" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="15" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="20"/>
       <c r="F44" s="14" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" s="15" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="15" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A47" s="15" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="15" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="20"/>
       <c r="F48" s="14" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="15" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
       <c r="F49" s="19" t="s">
-        <v>426</v>
-      </c>
-      <c r="G49" s="32" t="s">
-        <v>460</v>
+        <v>415</v>
+      </c>
+      <c r="G49" s="30" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="15" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="E50" s="20"/>
       <c r="F50" s="14" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="15" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="20"/>
       <c r="F51" s="14" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="15" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="20"/>
       <c r="F52" s="14" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A53" s="15" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="D53" s="20"/>
       <c r="E53" s="20"/>
       <c r="F53" s="14" t="s">
-        <v>357</v>
-      </c>
-      <c r="G53" s="31" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+        <v>347</v>
+      </c>
+      <c r="G53" s="29" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="15" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="15"/>
       <c r="F54" s="14" t="s">
-        <v>361</v>
+        <v>351</v>
+      </c>
+      <c r="G54" s="30" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="15" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="D55" s="15"/>
       <c r="E55" s="15"/>
       <c r="F55" s="14" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="15" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="E56" s="15"/>
       <c r="F56" s="14" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="15" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57" s="15"/>
       <c r="F57" s="14" t="s">
-        <v>373</v>
-      </c>
-      <c r="G57" s="31" t="s">
-        <v>458</v>
+        <v>363</v>
+      </c>
+      <c r="G57" s="29" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="15" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
       <c r="F58" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="G58" t="s">
-        <v>459</v>
+        <v>367</v>
+      </c>
+      <c r="G58" s="32" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="15" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>381</v>
+        <v>371</v>
+      </c>
+      <c r="G59" s="29" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="15" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="D60" s="15"/>
       <c r="E60" s="15"/>
       <c r="F60" s="14" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G60" xr:uid="{A2DEA66B-9A3B-A542-95A2-9E48A8B13E1D}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added TI jsonata mapping
</commit_message>
<xml_diff>
--- a/Maps/sdtm_mapping_paths.xlsx
+++ b/Maps/sdtm_mapping_paths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\SDTM_mapper\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFA8484-E5B1-4400-8F24-B347BA13E247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E189ADAB-3C48-4B40-99BF-48E6B02934AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9585" yWindow="-19275" windowWidth="24750" windowHeight="17490" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11385" yWindow="-18030" windowWidth="23910" windowHeight="16860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="540">
   <si>
     <t>Class</t>
   </si>
@@ -477,36 +477,6 @@
     <t>Grouping Qualifier</t>
   </si>
   <si>
-    <t>EligibilityCriterion</t>
-  </si>
-  <si>
-    <t>identifier</t>
-  </si>
-  <si>
-    <t>EligibilityCriterionItem</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>StudyVersion</t>
-  </si>
-  <si>
-    <t>versionIdentifier</t>
-  </si>
-  <si>
-    <t>StudyVersion/@versionIdentifier</t>
-  </si>
-  <si>
-    <t>Set to "TI"</t>
-  </si>
-  <si>
-    <t>Subcategory is not mandatory. If beneficial, we advice to store it in the EligibilityCriterion notes according to an internal codelist used for the purpose.</t>
-  </si>
-  <si>
     <t>TSSEQ</t>
   </si>
   <si>
@@ -1231,21 +1201,6 @@
   </si>
   <si>
     <t>Study Timeline</t>
-  </si>
-  <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@eligibilityCriteria/EligibilityCriterion/@identifier</t>
-  </si>
-  <si>
-    <t>Eligibility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StudyVersion/@studyDesigns/StudyDesign/@eligibilityCriteria/EligibilityCriterion/@text </t>
-  </si>
-  <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@eligibilityCriteria/EligibilityCriterion/@category/Code/@decode</t>
-  </si>
-  <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@eligibilityCriteria/EligibilityCriterion/@notes/CommentAnnotation/@codes/Code/@decode</t>
   </si>
   <si>
     <t>Adaptive Design Indicator</t>
@@ -1516,10 +1471,6 @@
     </r>
   </si>
   <si>
-    <t>$max([study.versions.studyDesigns.population.plannedAge.maxValue.value,study.versions.studyDesigns.population.cohorts.plannedAge.maxValue.value]) &amp; " " &amp; 
-study.versions.studyDesigns.population.plannedAge.maxValue.unit.standardCode.decode &amp; " " &amp; study.versions.studyDesigns.population.cohorts.plannedAge.maxValue.unit.standardCode.decode</t>
-  </si>
-  <si>
     <t>study.versions.studyDesigns.biospecimenRetentions.includesDNA</t>
   </si>
   <si>
@@ -1639,296 +1590,319 @@
     <t xml:space="preserve">study.versions.studyDesigns.population.plannedEnrollmentNumber.value </t>
   </si>
   <si>
+    <t>study.versions.studyDesigns[studyType.code="C16084"].model.decode</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C16084"].timePerspective.decode</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C16084"].populations.description</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C16084"].samplingMethod.decode</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.objectives[level.code="C85826"].{id: text}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.objectives[level.code="C85827"].{id: text}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.objectives[level.code="C163559"].{id: text}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.objectives[level.code="C85826"].{id: objectives.endpoint.text}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.objectives[level.code="C85827"].{id: objectives.endpoint.text}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.objectives[level.code="C163559"].{id: objectives.endpoint.text}</t>
+  </si>
+  <si>
+    <t>Fixed content</t>
+  </si>
+  <si>
+    <t>..code.codeSystem</t>
+  </si>
+  <si>
+    <t>..code.codeSystemVersion</t>
+  </si>
+  <si>
+    <t>Minimum Response Duration</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions.{id: minimumResponseDuration.value &amp; " " &amp; minimumResponseDuration.unit.standardCode.decode}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions[role.code="C165822"].{id: label}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions[role.code="C41161"].{id: label}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: type.decode}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.duration.quantity.value &amp; " " &amp; administrations.duration.quantity.unit.standardCode.decode}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: role[code="C753"].decode ? role[code="C753"].decode : role[code="C68609"].decode}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.administrableProduct.administrableDoseForm.standardCode.decode}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.dose.value}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.dose.unit.standardCode.decode}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.frequency.standardCode.decode}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions[role.code="C68609"].{id: label}</t>
+  </si>
+  <si>
+    <t>study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0]; studyIdentifiers[scopeId=$sponsorIdVal].text;)</t>
+  </si>
+  <si>
+    <t>TS</t>
+  </si>
+  <si>
+    <t>TSVAL JSONATA map</t>
+  </si>
+  <si>
+    <t>TSVALNF if empty</t>
+  </si>
+  <si>
+    <t>TSVALCD JSONATA map</t>
+  </si>
+  <si>
+    <t>TSVALCDREF JSONATA map</t>
+  </si>
+  <si>
+    <t>TSVALCDVER JSONATA map</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.frequency.standardCode.code}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.frequency.standardCode.codeSystem}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.frequency.standardCode.codeSystemVersion}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.dose.unit.standardCode.code}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.dose.unit.standardCode.codeSystem}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.dose.unit.standardCode.codeSystemVersion}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C98388"].model.code</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C98388"].model.codeSystem</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C98388"].model.codeSystemVersion</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: type.code}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: type.codeSystem}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: type.codeSystemVersion}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.scheduleTimelines[mainTimeline=true].plannedDuration.quantity.value &amp; " " &amp; study.versions.studyDesigns.scheduleTimelines[mainTimeline=true].plannedDuration.quantity.unit.standardCode.decode</t>
+  </si>
+  <si>
+    <t>$exists(study.versions.studyDesigns.population.cohorts) ? $count(study.versions.studyDesigns.population.cohorts) : ""</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C16084"].model.code</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C16084"].model.codeSystem</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C16084"].model.codeSystemVersion</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C16084"].timePerspective.code</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C16084"].timePerspective.codeSystem</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C16084"].timePerspective.codeSystemVersion</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C16084"].samplingMethod.code</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C16084"].samplingMethod.codeSystem</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C16084"].samplingMethod.codeSystemVersion</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.blindingSchema.standardCode.code</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.blindingSchema.standardCode.codeSystem</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.blindingSchema.standardCode.codeSystemVersion</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: role[code="C753"].decode ? role[code="C753"].code : role[code="C68609"].code}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: role[code="C753"].decode ? role[code="C753"].codeSystem : role[code="C68609"].codeSystem}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: role[code="C753"].decode ? role[code="C753"].codeSystemVersion : role[code="C68609"].codeSystemVersion}</t>
+  </si>
+  <si>
+    <t>study.study.versions.studyDesigns.studyPhase.standardCode.code</t>
+  </si>
+  <si>
+    <t>study.study.versions.studyDesigns.studyPhase.standardCode.codeSystem</t>
+  </si>
+  <si>
+    <t>study.study.versions.studyDesigns.studyPhase.standardCode.codeSystemVersion</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.route.standardCode.decode}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.route.standardCode.code}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.route.standardCode.codeSystem}</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions{id: administrations.route.standardCode.codeSystemVersion}</t>
+  </si>
+  <si>
+    <t>$exists(study.versions.roles.code[code="C142578"]) ? "Y" : ""</t>
+  </si>
+  <si>
+    <t>study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0];organizations[id=$sponsorIdVal].label;)</t>
+  </si>
+  <si>
+    <t>$exists(study.versions.studyDesigns.characteristics[code="C207613"]) ? "Y" : ""</t>
+  </si>
+  <si>
+    <t>PINF</t>
+  </si>
+  <si>
+    <t>$exists(study.versions.studyDesigns.population[includesHealthySubjects=true]) ? "Y" : ($exists(study.versions.studyDesigns.population.cohorts[includesHealthySubjects=true]) ? "Y" : "")</t>
+  </si>
+  <si>
+    <t>Healthy Subject Indicator Study Population / Cohort</t>
+  </si>
+  <si>
+    <t>study.versions.studyInterventions.administrations.administrableProduct[producDesignation.code="C202579"].pharmacologicClass.decode</t>
+  </si>
+  <si>
+    <t>$exists(study.versions.referenceIdentifiers.type[code="C215674"]) ? "Y" : ""</t>
+  </si>
+  <si>
+    <t>$exists(study.versions.studyDesigns.characteristics[code="C46079"]) ? "Y" : $exists(study.versions.studyDesigns.characteristics[code="C147145"]) ? "Y" : ""</t>
+  </si>
+  <si>
+    <t>$exists(study.versions.studyDesigns.indications[isRareDisease=true]) ? "Y" : ""</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.studyType.decode</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.studyType.code</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.studyType.codeSystem</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.studyType.codeSystemVersion</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C98388"].intentTypes.decode</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C98388"].intentTypes.code</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C98388"].intentTypes.codeSystem</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C98388"].intentTypes.codeSystemVersion</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C98388"].subTypes.decode</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C98388"].subTypes.code</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C98388"].subTypes.codeSystem</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C98388"].subTypes.codeSystemVersion</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.therapeuticAreas.decode</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.therapeuticAreas.code</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.therapeuticAreas.codeSystem</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.therapeuticAreas.codeSystemVersion</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.eligibilityCriteria.{id: identifier}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.eligibilityCriteria{id: category.decode}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.eligibilityCriteria{id: notes.codes.decode}</t>
+  </si>
+  <si>
     <t>$min([study.versions.studyDesigns.population.plannedAge.minValue.value,study.versions.studyDesigns.population.cohorts.plannedAge.minValue.value]) &amp; " " &amp; 
-study.versions.studyDesigns.population.plannedAge.minValue.unit.standardCode.decode &amp; " " &amp; study.versions.studyDesigns.population.cohorts.plannedAge.minValue.unit.standardCode.decode</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C16084"].model.decode</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C16084"].timePerspective.decode</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C16084"].populations.description</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C16084"].samplingMethod.decode</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.objectives[level.code="C85826"].{id: text}</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.objectives[level.code="C85827"].{id: text}</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.objectives[level.code="C163559"].{id: text}</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.objectives[level.code="C85826"].{id: objectives.endpoint.text}</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.objectives[level.code="C85827"].{id: objectives.endpoint.text}</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.objectives[level.code="C163559"].{id: objectives.endpoint.text}</t>
-  </si>
-  <si>
-    <t>Fixed content</t>
-  </si>
-  <si>
-    <t>..code.codeSystem</t>
-  </si>
-  <si>
-    <t>..code.codeSystemVersion</t>
-  </si>
-  <si>
-    <t>Minimum Response Duration</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions.{id: minimumResponseDuration.value &amp; " " &amp; minimumResponseDuration.unit.standardCode.decode}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions[role.code="C165822"].{id: label}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions[role.code="C41161"].{id: label}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: type.decode}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: administrations.duration.quantity.value &amp; " " &amp; administrations.duration.quantity.unit.standardCode.decode}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: role[code="C753"].decode ? role[code="C753"].decode : role[code="C68609"].decode}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: administrations.administrableProduct.administrableDoseForm.standardCode.decode}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: administrations.dose.value}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: administrations.dose.unit.standardCode.decode}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: administrations.frequency.standardCode.decode}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions[role.code="C68609"].{id: label}</t>
-  </si>
-  <si>
-    <t>study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0]; studyIdentifiers[scopeId=$sponsorIdVal].text;)</t>
-  </si>
-  <si>
-    <t>TS</t>
-  </si>
-  <si>
-    <t>TSVAL JSONATA map</t>
-  </si>
-  <si>
-    <t>TSVALNF if empty</t>
-  </si>
-  <si>
-    <t>TSVALCD JSONATA map</t>
-  </si>
-  <si>
-    <t>TSVALCDREF JSONATA map</t>
-  </si>
-  <si>
-    <t>TSVALCDVER JSONATA map</t>
-  </si>
-  <si>
-    <t>NI</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: administrations.frequency.standardCode.code}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: administrations.frequency.standardCode.codeSystem}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: administrations.frequency.standardCode.codeSystemVersion}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: administrations.dose.unit.standardCode.code}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: administrations.dose.unit.standardCode.codeSystem}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: administrations.dose.unit.standardCode.codeSystemVersion}</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C98388"].model.code</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C98388"].model.codeSystem</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C98388"].model.codeSystemVersion</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: type.code}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: type.codeSystem}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: type.codeSystemVersion}</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.scheduleTimelines[mainTimeline=true].plannedDuration.quantity.value &amp; " " &amp; study.versions.studyDesigns.scheduleTimelines[mainTimeline=true].plannedDuration.quantity.unit.standardCode.decode</t>
-  </si>
-  <si>
-    <t>$exists(study.versions.studyDesigns.population.cohorts) ? $count(study.versions.studyDesigns.population.cohorts) : ""</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C16084"].model.code</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C16084"].model.codeSystem</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C16084"].model.codeSystemVersion</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C16084"].timePerspective.code</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C16084"].timePerspective.codeSystem</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C16084"].timePerspective.codeSystemVersion</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C16084"].samplingMethod.code</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C16084"].samplingMethod.codeSystem</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C16084"].samplingMethod.codeSystemVersion</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.blindingSchema.standardCode.code</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.blindingSchema.standardCode.codeSystem</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.blindingSchema.standardCode.codeSystemVersion</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: role[code="C753"].decode ? role[code="C753"].code : role[code="C68609"].code}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: role[code="C753"].decode ? role[code="C753"].codeSystem : role[code="C68609"].codeSystem}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: role[code="C753"].decode ? role[code="C753"].codeSystemVersion : role[code="C68609"].codeSystemVersion}</t>
-  </si>
-  <si>
-    <t>study.study.versions.studyDesigns.studyPhase.standardCode.code</t>
-  </si>
-  <si>
-    <t>study.study.versions.studyDesigns.studyPhase.standardCode.codeSystem</t>
-  </si>
-  <si>
-    <t>study.study.versions.studyDesigns.studyPhase.standardCode.codeSystemVersion</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: administrations.route.standardCode.decode}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: administrations.route.standardCode.code}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: administrations.route.standardCode.codeSystem}</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions{id: administrations.route.standardCode.codeSystemVersion}</t>
-  </si>
-  <si>
-    <t>$exists(study.versions.roles.code[code="C142578"]) ? "Y" : ""</t>
-  </si>
-  <si>
-    <t>study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0];organizations[id=$sponsorIdVal].label;)</t>
-  </si>
-  <si>
-    <t>$exists(study.versions.studyDesigns.characteristics[code="C207613"]) ? "Y" : ""</t>
-  </si>
-  <si>
-    <t>PINF</t>
-  </si>
-  <si>
-    <t>$exists(study.versions.studyDesigns.population[includesHealthySubjects=true]) ? "Y" : ($exists(study.versions.studyDesigns.population.cohorts[includesHealthySubjects=true]) ? "Y" : "")</t>
-  </si>
-  <si>
-    <t>Healthy Subject Indicator Study Population / Cohort</t>
-  </si>
-  <si>
-    <t>study.versions.studyInterventions.administrations.administrableProduct[producDesignation.code="C202579"].pharmacologicClass.decode</t>
-  </si>
-  <si>
-    <t>$exists(study.versions.referenceIdentifiers.type[code="C215674"]) ? "Y" : ""</t>
-  </si>
-  <si>
-    <t>$exists(study.versions.studyDesigns.characteristics[code="C46079"]) ? "Y" : $exists(study.versions.studyDesigns.characteristics[code="C147145"]) ? "Y" : ""</t>
-  </si>
-  <si>
-    <t>$exists(study.versions.studyDesigns.indications[isRareDisease=true]) ? "Y" : ""</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.studyType.decode</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.studyType.code</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.studyType.codeSystem</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.studyType.codeSystemVersion</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C98388"].intentTypes.decode</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C98388"].intentTypes.code</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C98388"].intentTypes.codeSystem</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C98388"].intentTypes.codeSystemVersion</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C98388"].subTypes.decode</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C98388"].subTypes.code</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C98388"].subTypes.codeSystem</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C98388"].subTypes.codeSystemVersion</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.therapeuticAreas.decode</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.therapeuticAreas.code</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.therapeuticAreas.codeSystem</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.therapeuticAreas.codeSystemVersion</t>
+$distinct(study.versions.studyDesigns.population.plannedAge.minValue.unit.standardCode.decode)
+ &amp; " " &amp; $distinct(study.versions.studyDesigns.population.cohorts.plannedAge.minValue.unit.standardCode.decode)</t>
+  </si>
+  <si>
+    <t>$max([study.versions.studyDesigns.population.plannedAge.maxValue.value,study.versions.studyDesigns.population.cohorts.plannedAge.maxValue.value]) &amp; " " &amp; 
+$distinct(study.versions.studyDesigns.population.plannedAge.maxValue.unit.standardCode.decode) &amp; " " &amp; $distinct(study.versions.studyDesigns.population.cohorts.plannedAge.maxValue.unit.standardCode.decode)</t>
+  </si>
+  <si>
+    <t>study.versions.($EligTxt := function($id) {(eligibilityCriterionItems[id=$id].text)}; studyDesigns.eligibilityCriteria{id: $EligTxt(criterionItemId)})</t>
+  </si>
+  <si>
+    <t>study.versions.versionIdentifier</t>
   </si>
 </sst>
 </file>
@@ -2169,7 +2143,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2247,9 +2221,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2276,6 +2247,18 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2287,6 +2270,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2607,34 +2593,34 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
       <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="B7" s="17"/>
     </row>
@@ -2643,7 +2629,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="31" x14ac:dyDescent="0.35">
@@ -2651,7 +2637,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -2659,7 +2645,7 @@
         <v>79</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="31" x14ac:dyDescent="0.35">
@@ -2667,7 +2653,7 @@
         <v>56</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -2675,7 +2661,7 @@
         <v>58</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -2683,7 +2669,7 @@
         <v>57</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -2691,7 +2677,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -2699,29 +2685,29 @@
         <v>60</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="B18" s="17"/>
     </row>
     <row r="20" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -2751,26 +2737,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="41" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -2926,19 +2912,19 @@
         <v>68</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="O5" s="8" t="s">
         <v>66</v>
@@ -2972,19 +2958,19 @@
         <v>69</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="O6" s="8" t="s">
         <v>66</v>
@@ -3021,16 +3007,16 @@
         <v>77</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="O7" s="8" t="s">
         <v>66</v>
@@ -3066,19 +3052,19 @@
         <v>72</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="O8" s="8" t="s">
         <v>66</v>
@@ -3114,19 +3100,19 @@
         <v>73</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="O9" s="8" t="s">
         <v>66</v>
@@ -3192,16 +3178,16 @@
         <v>74</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="L11" s="7" t="s">
         <v>78</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="O11" s="8" t="s">
         <v>66</v>
@@ -3237,19 +3223,19 @@
         <v>75</v>
       </c>
       <c r="J12" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="M12" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="K12" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>389</v>
-      </c>
       <c r="N12" s="7" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="O12" s="8" t="s">
         <v>66</v>
@@ -3297,26 +3283,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="41" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -3470,19 +3456,19 @@
         <v>72</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>66</v>
@@ -3516,19 +3502,19 @@
         <v>73</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="O6" s="4" t="s">
         <v>66</v>
@@ -3562,19 +3548,19 @@
         <v>100</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="O7" s="4" t="s">
         <v>66</v>
@@ -3608,19 +3594,19 @@
         <v>101</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="O8" s="4" t="s">
         <v>66</v>
@@ -3657,16 +3643,16 @@
         <v>103</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="O9" s="4" t="s">
         <v>66</v>
@@ -3711,26 +3697,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="41" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -3888,16 +3874,16 @@
         <v>128</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>105</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>66</v>
@@ -3933,19 +3919,19 @@
         <v>123</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>108</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>66</v>
@@ -3981,19 +3967,19 @@
         <v>124</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>110</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="O7" s="6" t="s">
         <v>66</v>
@@ -4029,19 +4015,19 @@
         <v>68</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="O8" s="6" t="s">
         <v>66</v>
@@ -4077,19 +4063,19 @@
         <v>69</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="O9" s="6" t="s">
         <v>66</v>
@@ -4125,19 +4111,19 @@
         <v>125</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="M10" s="6" t="s">
         <v>116</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="O10" s="6" t="s">
         <v>66</v>
@@ -4173,19 +4159,19 @@
         <v>126</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>118</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="O11" s="6" t="s">
         <v>66</v>
@@ -4212,97 +4198,80 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A2D413-6E3B-5A40-9DE8-0245851A536D}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="5" width="18.6328125" customWidth="1"/>
-    <col min="6" max="13" width="25.81640625" customWidth="1"/>
-    <col min="16" max="16" width="15" style="23" customWidth="1"/>
+    <col min="6" max="6" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6328125" style="40" customWidth="1"/>
+    <col min="8" max="8" width="29.81640625" style="16" customWidth="1"/>
+    <col min="9" max="11" width="8.6328125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-    </row>
-    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="N2" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="P2" s="24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="87" x14ac:dyDescent="0.35">
+      <c r="G1" s="37" t="s">
+        <v>425</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>446</v>
+      </c>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+    </row>
+    <row r="2" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="H2" s="33"/>
+    </row>
+    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>82</v>
@@ -4313,168 +4282,90 @@
       <c r="E3" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="P3" s="26" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="F3" s="4"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="9" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>84</v>
+        <v>130</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>85</v>
+        <v>131</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>82</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>8</v>
+        <v>88</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="27"/>
-    </row>
-    <row r="5" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="F4" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>533</v>
+      </c>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>82</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="12" t="s">
-        <v>395</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="P5" s="27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F5" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" s="45" t="s">
+        <v>538</v>
+      </c>
+      <c r="H5" s="33"/>
+    </row>
+    <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>82</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="12" t="s">
-        <v>397</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>379</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="P6" s="27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="F6" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>534</v>
+      </c>
+      <c r="H6" s="33"/>
+    </row>
+    <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>82</v>
@@ -4483,175 +4374,61 @@
         <v>142</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="12" t="s">
-        <v>398</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="P7" s="27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="101.5" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>535</v>
+      </c>
+      <c r="H7" s="33"/>
+    </row>
+    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>82</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>142</v>
+        <v>94</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="12" t="s">
-        <v>399</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="P8" s="27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="F8" s="4"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="33"/>
+    </row>
+    <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>82</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="P9" s="27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="F9" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="P10" s="27" t="s">
-        <v>129</v>
-      </c>
+      <c r="G9" s="38" t="s">
+        <v>539</v>
+      </c>
+      <c r="H9" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:P1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="I8" r:id="rId1" display="StudyVersion/@studyDesigns/StudyDesign/@population/StudyDesignPopulation/@criteria/EligibilityCriterion/@notes/CommentAnnotation/@codes/Code/@decode" xr:uid="{29EC803E-5671-C341-849B-0FED76596B9A}"/>
-    <hyperlink ref="I10" r:id="rId2" xr:uid="{DC6E40E2-1E2E-F746-9D13-D07C35795C8E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4661,7 +4438,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G1" sqref="G1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4696,14 +4473,14 @@
         <v>80</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>440</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>463</v>
-      </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
+        <v>425</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>446</v>
+      </c>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
     </row>
     <row r="2" spans="1:11" ht="93" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
@@ -4724,10 +4501,10 @@
       <c r="F2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="35" t="s">
-        <v>478</v>
-      </c>
-      <c r="H2" s="34"/>
+      <c r="G2" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
@@ -4746,17 +4523,17 @@
         <v>83</v>
       </c>
       <c r="F3" s="5"/>
-      <c r="G3" s="33"/>
+      <c r="G3" s="32"/>
       <c r="H3" s="9" t="s">
-        <v>479</v>
+        <v>462</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>106</v>
@@ -4768,15 +4545,15 @@
         <v>83</v>
       </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>82</v>
@@ -4788,15 +4565,15 @@
         <v>97</v>
       </c>
       <c r="F5" s="12"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
     </row>
     <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>82</v>
@@ -4808,15 +4585,15 @@
         <v>83</v>
       </c>
       <c r="F6" s="12"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="34"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="33"/>
     </row>
     <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>82</v>
@@ -4828,116 +4605,116 @@
         <v>83</v>
       </c>
       <c r="F7" s="12"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="34"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="33"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>82</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F8" s="12"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="33"/>
     </row>
     <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>82</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>97</v>
       </c>
       <c r="F9" s="12"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="34"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="33"/>
     </row>
     <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>82</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F10" s="12"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="34"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33"/>
     </row>
     <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>82</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>464</v>
-      </c>
-      <c r="H11" s="34"/>
+        <v>159</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>447</v>
+      </c>
+      <c r="H11" s="33"/>
     </row>
     <row r="12" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>82</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>418</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>465</v>
-      </c>
-      <c r="H12" s="34"/>
+        <v>403</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>448</v>
+      </c>
+      <c r="H12" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4948,8 +4725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DEA66B-9A3B-A542-95A2-9E48A8B13E1D}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="C4" zoomScale="109" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4969,1358 +4746,1358 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="F1" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="28" t="s">
-        <v>480</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>481</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>482</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>483</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>484</v>
+      <c r="G1" s="27" t="s">
+        <v>463</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>464</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>465</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>466</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="14" t="s">
-        <v>400</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+        <v>385</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="14" t="s">
-        <v>401</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+        <v>386</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="14" t="s">
-        <v>402</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>442</v>
-      </c>
-      <c r="H4" s="36" t="s">
-        <v>526</v>
+        <v>387</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>537</v>
+      </c>
+      <c r="H4" s="35" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>403</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>443</v>
+        <v>388</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>404</v>
-      </c>
-      <c r="G6" s="29" t="s">
-        <v>444</v>
+        <v>389</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="F7" s="14"/>
-      <c r="G7" s="29" t="s">
-        <v>477</v>
+      <c r="G7" s="28" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="D8" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>184</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>467</v>
+        <v>449</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>405</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>468</v>
+        <v>390</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>523</v>
+        <v>200</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>406</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>474</v>
+        <v>391</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>473</v>
+        <v>206</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>407</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>476</v>
-      </c>
-      <c r="I15" s="29" t="s">
-        <v>487</v>
-      </c>
-      <c r="J15" s="29" t="s">
-        <v>488</v>
-      </c>
-      <c r="K15" s="29" t="s">
-        <v>489</v>
+        <v>392</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>459</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>470</v>
+      </c>
+      <c r="J15" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="K15" s="28" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>408</v>
-      </c>
-      <c r="G16" s="29" t="s">
+        <v>393</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>458</v>
+      </c>
+      <c r="I16" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="J16" s="28" t="s">
+        <v>474</v>
+      </c>
+      <c r="K16" s="28" t="s">
         <v>475</v>
-      </c>
-      <c r="I16" s="29" t="s">
-        <v>490</v>
-      </c>
-      <c r="J16" s="29" t="s">
-        <v>491</v>
-      </c>
-      <c r="K16" s="29" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="G17" s="37" t="s">
-        <v>525</v>
+        <v>215</v>
+      </c>
+      <c r="G17" s="36" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="14" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="14" t="s">
-        <v>528</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>527</v>
+        <v>511</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="14" t="s">
-        <v>409</v>
-      </c>
-      <c r="G20" s="29" t="s">
-        <v>448</v>
+        <v>394</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="14" t="s">
-        <v>237</v>
-      </c>
-      <c r="G21" s="30" t="s">
-        <v>447</v>
-      </c>
-      <c r="I21" s="30" t="s">
-        <v>493</v>
-      </c>
-      <c r="J21" s="30" t="s">
-        <v>494</v>
-      </c>
-      <c r="K21" s="30" t="s">
-        <v>495</v>
+        <v>227</v>
+      </c>
+      <c r="G21" s="29" t="s">
+        <v>431</v>
+      </c>
+      <c r="I21" s="29" t="s">
+        <v>476</v>
+      </c>
+      <c r="J21" s="29" t="s">
+        <v>477</v>
+      </c>
+      <c r="K21" s="29" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="G22" s="29" t="s">
-        <v>470</v>
-      </c>
-      <c r="I22" s="29" t="s">
-        <v>496</v>
-      </c>
-      <c r="J22" s="29" t="s">
-        <v>497</v>
-      </c>
-      <c r="K22" s="29" t="s">
-        <v>498</v>
+        <v>230</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>453</v>
+      </c>
+      <c r="I22" s="28" t="s">
+        <v>479</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>480</v>
+      </c>
+      <c r="K22" s="28" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="13" t="s">
-        <v>437</v>
-      </c>
-      <c r="G23" s="29" t="s">
-        <v>499</v>
+        <v>422</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>482</v>
       </c>
       <c r="H23" t="s">
-        <v>485</v>
+        <v>468</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="14" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
       <c r="F25" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="G25" s="29" t="s">
-        <v>449</v>
+        <v>242</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
       <c r="F26" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="G26" s="30" t="s">
-        <v>500</v>
+        <v>243</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
       <c r="F27" s="14" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="G28" s="29" t="s">
-        <v>459</v>
+        <v>252</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="G29" s="29" t="s">
-        <v>457</v>
+        <v>258</v>
+      </c>
+      <c r="G29" s="28" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="G30" s="29" t="s">
-        <v>458</v>
+        <v>262</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
       <c r="F31" s="14" t="s">
-        <v>273</v>
-      </c>
-      <c r="G31" s="32" t="s">
-        <v>453</v>
-      </c>
-      <c r="I31" s="32" t="s">
-        <v>501</v>
-      </c>
-      <c r="J31" s="32" t="s">
-        <v>502</v>
-      </c>
-      <c r="K31" s="32" t="s">
-        <v>503</v>
+        <v>263</v>
+      </c>
+      <c r="G31" s="31" t="s">
+        <v>436</v>
+      </c>
+      <c r="I31" s="31" t="s">
+        <v>484</v>
+      </c>
+      <c r="J31" s="31" t="s">
+        <v>485</v>
+      </c>
+      <c r="K31" s="31" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
       <c r="F32" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="G32" s="30" t="s">
-        <v>454</v>
-      </c>
-      <c r="I32" s="30" t="s">
-        <v>504</v>
-      </c>
-      <c r="J32" s="30" t="s">
-        <v>505</v>
-      </c>
-      <c r="K32" s="30" t="s">
-        <v>506</v>
+        <v>266</v>
+      </c>
+      <c r="G32" s="29" t="s">
+        <v>437</v>
+      </c>
+      <c r="I32" s="29" t="s">
+        <v>487</v>
+      </c>
+      <c r="J32" s="29" t="s">
+        <v>488</v>
+      </c>
+      <c r="K32" s="29" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
       <c r="F33" s="14" t="s">
-        <v>411</v>
-      </c>
-      <c r="G33" s="30" t="s">
-        <v>455</v>
+        <v>396</v>
+      </c>
+      <c r="G33" s="29" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
       <c r="F34" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="G34" s="30" t="s">
-        <v>456</v>
-      </c>
-      <c r="I34" s="30" t="s">
-        <v>507</v>
-      </c>
-      <c r="J34" s="30" t="s">
-        <v>508</v>
-      </c>
-      <c r="K34" s="30" t="s">
-        <v>509</v>
+        <v>272</v>
+      </c>
+      <c r="G34" s="29" t="s">
+        <v>439</v>
+      </c>
+      <c r="I34" s="29" t="s">
+        <v>490</v>
+      </c>
+      <c r="J34" s="29" t="s">
+        <v>491</v>
+      </c>
+      <c r="K34" s="29" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="15" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="G35" s="29" t="s">
-        <v>462</v>
+        <v>275</v>
+      </c>
+      <c r="G35" s="28" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="15" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>290</v>
-      </c>
-      <c r="G36" s="29" t="s">
-        <v>460</v>
+        <v>280</v>
+      </c>
+      <c r="G36" s="28" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>293</v>
-      </c>
-      <c r="G37" s="29" t="s">
-        <v>461</v>
+        <v>283</v>
+      </c>
+      <c r="G37" s="28" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="15" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="15" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="G38" s="29" t="s">
-        <v>529</v>
+        <v>286</v>
+      </c>
+      <c r="G38" s="28" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="15" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="20"/>
       <c r="F39" s="14" t="s">
-        <v>299</v>
-      </c>
-      <c r="G39" s="29" t="s">
-        <v>530</v>
+        <v>289</v>
+      </c>
+      <c r="G39" s="28" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A40" s="15" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="20"/>
       <c r="F40" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="G40" s="29" t="s">
-        <v>451</v>
+        <v>397</v>
+      </c>
+      <c r="G40" s="28" t="s">
+        <v>435</v>
       </c>
       <c r="H40" t="s">
-        <v>485</v>
+        <v>468</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="15" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="20" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>413</v>
-      </c>
-      <c r="G41" s="30" t="s">
-        <v>471</v>
+        <v>398</v>
+      </c>
+      <c r="G41" s="29" t="s">
+        <v>454</v>
       </c>
       <c r="H41" t="s">
-        <v>485</v>
+        <v>468</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="15" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="20"/>
       <c r="F42" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="G42" s="29" t="s">
-        <v>531</v>
+        <v>301</v>
+      </c>
+      <c r="G42" s="28" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="20"/>
       <c r="F43" s="14" t="s">
-        <v>315</v>
-      </c>
-      <c r="G43" s="30" t="s">
-        <v>532</v>
+        <v>305</v>
+      </c>
+      <c r="G43" s="29" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="15" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A45" s="15" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>321</v>
-      </c>
-      <c r="G45" s="29" t="s">
-        <v>519</v>
-      </c>
-      <c r="I45" s="29" t="s">
-        <v>520</v>
-      </c>
-      <c r="J45" s="29" t="s">
-        <v>521</v>
-      </c>
-      <c r="K45" s="29" t="s">
-        <v>522</v>
+        <v>311</v>
+      </c>
+      <c r="G45" s="28" t="s">
+        <v>502</v>
+      </c>
+      <c r="I45" s="28" t="s">
+        <v>503</v>
+      </c>
+      <c r="J45" s="28" t="s">
+        <v>504</v>
+      </c>
+      <c r="K45" s="28" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A46" s="15" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="15" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
       <c r="F47" s="14" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="15" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="20"/>
       <c r="F48" s="19" t="s">
-        <v>414</v>
-      </c>
-      <c r="G48" s="29" t="s">
-        <v>524</v>
+        <v>399</v>
+      </c>
+      <c r="G48" s="28" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="15" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E49" s="20"/>
       <c r="F49" s="14" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="15" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="20"/>
       <c r="F50" s="14" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="15" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="20"/>
       <c r="F51" s="14" t="s">
-        <v>343</v>
-      </c>
-      <c r="G51" s="32" t="s">
-        <v>533</v>
-      </c>
-      <c r="I51" s="32" t="s">
-        <v>534</v>
-      </c>
-      <c r="J51" s="32" t="s">
-        <v>535</v>
-      </c>
-      <c r="K51" s="32" t="s">
-        <v>536</v>
+        <v>333</v>
+      </c>
+      <c r="G51" s="31" t="s">
+        <v>516</v>
+      </c>
+      <c r="I51" s="31" t="s">
+        <v>517</v>
+      </c>
+      <c r="J51" s="31" t="s">
+        <v>518</v>
+      </c>
+      <c r="K51" s="31" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A52" s="15" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="20"/>
       <c r="F52" s="14" t="s">
-        <v>347</v>
-      </c>
-      <c r="G52" s="29" t="s">
-        <v>450</v>
-      </c>
-      <c r="I52" s="29" t="s">
-        <v>510</v>
-      </c>
-      <c r="J52" s="29" t="s">
-        <v>511</v>
-      </c>
-      <c r="K52" s="29" t="s">
-        <v>512</v>
+        <v>337</v>
+      </c>
+      <c r="G52" s="28" t="s">
+        <v>434</v>
+      </c>
+      <c r="I52" s="28" t="s">
+        <v>493</v>
+      </c>
+      <c r="J52" s="28" t="s">
+        <v>494</v>
+      </c>
+      <c r="K52" s="28" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A53" s="15" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="D53" s="15"/>
       <c r="E53" s="15"/>
       <c r="F53" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="G53" s="30" t="s">
-        <v>472</v>
-      </c>
-      <c r="I53" s="30" t="s">
-        <v>513</v>
-      </c>
-      <c r="J53" s="30" t="s">
-        <v>514</v>
-      </c>
-      <c r="K53" s="30" t="s">
-        <v>515</v>
+        <v>341</v>
+      </c>
+      <c r="G53" s="29" t="s">
+        <v>455</v>
+      </c>
+      <c r="I53" s="29" t="s">
+        <v>496</v>
+      </c>
+      <c r="J53" s="29" t="s">
+        <v>497</v>
+      </c>
+      <c r="K53" s="29" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="15" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="15"/>
       <c r="F54" s="14" t="s">
-        <v>352</v>
-      </c>
-      <c r="G54" s="29" t="s">
-        <v>545</v>
-      </c>
-      <c r="I54" s="29" t="s">
-        <v>546</v>
-      </c>
-      <c r="J54" s="29" t="s">
-        <v>547</v>
-      </c>
-      <c r="K54" s="29" t="s">
-        <v>548</v>
+        <v>342</v>
+      </c>
+      <c r="G54" s="28" t="s">
+        <v>528</v>
+      </c>
+      <c r="I54" s="28" t="s">
+        <v>529</v>
+      </c>
+      <c r="J54" s="28" t="s">
+        <v>530</v>
+      </c>
+      <c r="K54" s="28" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="15" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="E55" s="15"/>
       <c r="F55" s="14" t="s">
-        <v>358</v>
-      </c>
-      <c r="G55" s="29" t="s">
-        <v>537</v>
-      </c>
-      <c r="I55" s="29" t="s">
-        <v>538</v>
-      </c>
-      <c r="J55" s="29" t="s">
-        <v>539</v>
-      </c>
-      <c r="K55" s="29" t="s">
-        <v>540</v>
+        <v>348</v>
+      </c>
+      <c r="G55" s="28" t="s">
+        <v>520</v>
+      </c>
+      <c r="I55" s="28" t="s">
+        <v>521</v>
+      </c>
+      <c r="J55" s="28" t="s">
+        <v>522</v>
+      </c>
+      <c r="K55" s="28" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="15" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="15"/>
       <c r="F56" s="14" t="s">
-        <v>363</v>
-      </c>
-      <c r="G56" s="29" t="s">
-        <v>445</v>
+        <v>353</v>
+      </c>
+      <c r="G56" s="28" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="15" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57" s="15"/>
       <c r="F57" s="14" t="s">
-        <v>367</v>
-      </c>
-      <c r="G57" s="32" t="s">
-        <v>446</v>
-      </c>
-      <c r="H57" s="36" t="s">
-        <v>485</v>
-      </c>
-      <c r="I57" s="32" t="s">
-        <v>516</v>
-      </c>
-      <c r="J57" s="32" t="s">
-        <v>517</v>
-      </c>
-      <c r="K57" s="32" t="s">
-        <v>518</v>
+        <v>357</v>
+      </c>
+      <c r="G57" s="31" t="s">
+        <v>430</v>
+      </c>
+      <c r="H57" s="35" t="s">
+        <v>468</v>
+      </c>
+      <c r="I57" s="31" t="s">
+        <v>499</v>
+      </c>
+      <c r="J57" s="31" t="s">
+        <v>500</v>
+      </c>
+      <c r="K57" s="31" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="15" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="G58" s="29" t="s">
+        <v>361</v>
+      </c>
+      <c r="G58" s="28" t="s">
+        <v>452</v>
+      </c>
+      <c r="H58" s="35" t="s">
         <v>469</v>
-      </c>
-      <c r="H58" s="36" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="15" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="D59" s="15"/>
       <c r="E59" s="15"/>
       <c r="F59" s="14" t="s">
-        <v>375</v>
-      </c>
-      <c r="G59" s="29" t="s">
-        <v>541</v>
-      </c>
-      <c r="I59" s="29" t="s">
-        <v>542</v>
-      </c>
-      <c r="J59" s="29" t="s">
-        <v>543</v>
-      </c>
-      <c r="K59" s="29" t="s">
-        <v>544</v>
+        <v>365</v>
+      </c>
+      <c r="G59" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="I59" s="28" t="s">
+        <v>525</v>
+      </c>
+      <c r="J59" s="28" t="s">
+        <v>526</v>
+      </c>
+      <c r="K59" s="28" t="s">
+        <v>527</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add mapping and start TI code
</commit_message>
<xml_diff>
--- a/Maps/sdtm_mapping_paths.xlsx
+++ b/Maps/sdtm_mapping_paths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\SDTM_mapper\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E189ADAB-3C48-4B40-99BF-48E6B02934AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877B4A93-A46B-4D5D-87DD-B230E77EE1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11385" yWindow="-18030" windowWidth="23910" windowHeight="16860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="535">
   <si>
     <t>Class</t>
   </si>
@@ -62,12 +62,6 @@
     <t>Condition Notes</t>
   </si>
   <si>
-    <t>ConditionAssignment</t>
-  </si>
-  <si>
-    <t>condition</t>
-  </si>
-  <si>
     <t>Identifier</t>
   </si>
   <si>
@@ -81,9 +75,6 @@
   </si>
   <si>
     <t>StudyElement</t>
-  </si>
-  <si>
-    <t>StudyEpoch</t>
   </si>
   <si>
     <t>StudyIdentifier</t>
@@ -249,9 +240,6 @@
     <t>Mapped</t>
   </si>
   <si>
-    <t>Not Required</t>
-  </si>
-  <si>
     <t>StudyVersion/@studyDesigns/StudyDesign/@arms/StudyArm/@label</t>
   </si>
   <si>
@@ -261,30 +249,15 @@
     <t>next</t>
   </si>
   <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@epochs/StudyEpoch/@next</t>
-  </si>
-  <si>
     <t>StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@label</t>
   </si>
   <si>
     <t>StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@description</t>
   </si>
   <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@scheduleTimelines/ScheduleTimeline/@instances/ScheduledDecisionInstance/@conditionAssignments/ConditionAssignment/@condition</t>
-  </si>
-  <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@epochs/StudyEpoch/@label</t>
-  </si>
-  <si>
     <t>Set to "TA"</t>
   </si>
   <si>
-    <t>Create an order number after ordering the arm related epochs based on the StudyEpoch next relationship.</t>
-  </si>
-  <si>
-    <t>If the condition points to an scheduledActivityInstance which refers to the same epoch then the transition rule can be disregarded for SDTM TATRANS variable creation.</t>
-  </si>
-  <si>
     <t>Overall Notes</t>
   </si>
   <si>
@@ -1170,16 +1143,10 @@
     <t>Arm Specific Planned Order of Element Within Arm</t>
   </si>
   <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@arms/StudyArm/@id=StudyVersion/@studyDesigns/StudyDesign/@studyCells/StudyCell/@arm | StudyVersion/@studyDesigns/StudyDesign/@epochs/StudyEpoch/@id=StudyVersion/@studyDesigns/StudyDesign/@studyCells/StudyCell/@epoch</t>
-  </si>
-  <si>
     <t>Arm Specific Element Name</t>
   </si>
   <si>
     <t>Arm Specific Element Description</t>
-  </si>
-  <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@arms/StudyArm/@id=StudyVersion/@studyDesigns/StudyDesign/@studyCells/StudyCell/@arm | StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@id=StudyVersion/@studyDesigns/StudyDesign/@studyCells/StudyCell/@elements | StudyVersion/@studyDesigns/StudyDesign/@scheduleTimelines/ScheduleTimeline/@instances/ScheduledDecisionInstance/@epoch=StudyVersion/@studyDesigns/StudyDesign/@studyCells/StudyCell/@epoch</t>
   </si>
   <si>
     <t>Arm Specific Transition Rule</t>
@@ -1903,6 +1870,24 @@
   </si>
   <si>
     <t>study.versions.versionIdentifier</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.arms.{id: label}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.arms.{id: description}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.($ElementName := function($id) {(elements[id=$id].label)}; studyCells.{armId: $ElementName(elementIds[0])})</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.($ElementName := function($id) {(elements[id=$id].description)}; studyCells.{armId: $ElementName(elementIds[0])})</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.($EpochName := function($id) {(epochs[id=$id].label)}; studyCells.{armId: $EpochName(epochId[0])})</t>
   </si>
 </sst>
 </file>
@@ -2143,7 +2128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2259,6 +2244,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2271,8 +2259,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2593,34 +2587,34 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="B7" s="17"/>
     </row>
@@ -2629,7 +2623,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="31" x14ac:dyDescent="0.35">
@@ -2637,39 +2631,39 @@
         <v>1</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>410</v>
+        <v>399</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>411</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -2677,37 +2671,37 @@
         <v>5</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
       <c r="B18" s="17"/>
     </row>
     <row r="20" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -2717,175 +2711,125 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CEFEB0-0887-1349-82EC-A63800D98F30}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="215" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="17.81640625" customWidth="1"/>
-    <col min="6" max="7" width="18.1796875" customWidth="1"/>
-    <col min="8" max="8" width="19.81640625" customWidth="1"/>
-    <col min="9" max="9" width="67.36328125" customWidth="1"/>
-    <col min="10" max="10" width="32.36328125" customWidth="1"/>
-    <col min="11" max="11" width="71" customWidth="1"/>
-    <col min="12" max="12" width="36.453125" customWidth="1"/>
-    <col min="13" max="15" width="25.81640625" customWidth="1"/>
-    <col min="16" max="16" width="19.1796875" style="23" customWidth="1"/>
+    <col min="6" max="6" width="25.81640625" customWidth="1"/>
+    <col min="7" max="7" width="30.08984375" style="41" customWidth="1"/>
+    <col min="8" max="8" width="18.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="44" t="s">
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-    </row>
-    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>414</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>435</v>
+      </c>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+    </row>
+    <row r="2" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P2" s="21" t="s">
+      <c r="C2" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="D2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="H2" s="33"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+    </row>
+    <row r="3" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="P3" s="22" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="9" t="s">
+        <v>529</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="1:11" ht="31" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="31" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+      <c r="B4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="5"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="P4" s="22"/>
-    </row>
-    <row r="5" spans="1:16" ht="31" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>31</v>
       </c>
@@ -2893,45 +2837,22 @@
         <v>32</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>11</v>
+        <v>363</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>369</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="P5" s="22"/>
-    </row>
-    <row r="6" spans="1:16" ht="31" x14ac:dyDescent="0.35">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>34</v>
       </c>
@@ -2939,93 +2860,43 @@
         <v>35</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>369</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="P6" s="22"/>
-    </row>
-    <row r="7" spans="1:16" ht="62" x14ac:dyDescent="0.35">
+        <v>364</v>
+      </c>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>40</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>13</v>
+        <v>365</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="P7" s="22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>41</v>
       </c>
@@ -3033,47 +2904,22 @@
         <v>42</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="F8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>369</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="O8" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="P8" s="22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+        <v>366</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3081,180 +2927,62 @@
         <v>45</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>369</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>376</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="P9" s="22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="P10" s="22"/>
-    </row>
-    <row r="11" spans="1:16" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+      <c r="B11" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>6</v>
+        <v>368</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="P11" s="22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="58" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="O12" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="P12" s="22" t="s">
-        <v>28</v>
+        <v>534</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:P1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="I8" r:id="rId1" xr:uid="{1D5F4684-2747-B042-942D-56EF8BE3ECAD}"/>
-    <hyperlink ref="I9" r:id="rId2" display="StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@label" xr:uid="{C06B2C68-446F-0444-B70D-BA9010E9E824}"/>
-    <hyperlink ref="I12" r:id="rId3" display="StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@label" xr:uid="{7FA8F4E3-E05A-394F-87CB-D7A8712D361C}"/>
-    <hyperlink ref="K11" r:id="rId4" display="StudyVersion/@studyDesigns/StudyDesign/@scheduleTimelines/ScheduleTimeline/@instances/ScheduledDecisionInstance/@epoch=StudyVersion/@studyDesigns/StudyDesign/@studyCells/StudyCell/@elements/StudyEpoch/@id" xr:uid="{F84732A8-99E3-6443-87EC-DA88BBE975B7}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3283,42 +3011,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
+      <c r="A1" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>21</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>0</v>
@@ -3327,99 +3055,99 @@
         <v>1</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>5</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="P2" s="24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="O3" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="M3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>66</v>
-      </c>
       <c r="P3" s="22" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="9" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
@@ -3431,231 +3159,231 @@
     </row>
     <row r="5" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P5" s="25"/>
     </row>
     <row r="6" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>91</v>
-      </c>
       <c r="E6" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="12" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P6" s="25"/>
     </row>
     <row r="7" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="12" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="J7" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="M7" s="12" t="s">
         <v>369</v>
       </c>
-      <c r="K7" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>380</v>
-      </c>
       <c r="N7" s="4" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P7" s="25"/>
     </row>
     <row r="8" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="12" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P8" s="25"/>
     </row>
     <row r="9" spans="1:16" ht="145" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="12" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P9" s="25"/>
     </row>
@@ -3681,7 +3409,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3697,42 +3425,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
+      <c r="A1" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="48"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>0</v>
@@ -3741,99 +3469,99 @@
         <v>1</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="P3" s="26" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -3846,338 +3574,338 @@
     </row>
     <row r="5" spans="1:16" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P5" s="26" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>91</v>
-      </c>
       <c r="E6" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P6" s="26" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P7" s="26" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>120</v>
-      </c>
       <c r="F8" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P8" s="26" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>91</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>2</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P9" s="26" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P10" s="26" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P11" s="26" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -4200,8 +3928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A2D413-6E3B-5A40-9DE8-0245851A536D}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4215,28 +3943,28 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>21</v>
-      </c>
       <c r="F1" s="11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="G1" s="37" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
@@ -4244,161 +3972,161 @@
     </row>
     <row r="2" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>461</v>
+        <v>450</v>
       </c>
       <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="38"/>
       <c r="H3" s="9" t="s">
-        <v>532</v>
+        <v>521</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="G4" s="39" t="s">
-        <v>533</v>
+        <v>522</v>
       </c>
       <c r="H4" s="33"/>
     </row>
     <row r="5" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>91</v>
-      </c>
       <c r="E5" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="G5" s="45" t="s">
-        <v>538</v>
+        <v>124</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>527</v>
       </c>
       <c r="H5" s="33"/>
     </row>
     <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G6" s="39" t="s">
-        <v>534</v>
+        <v>523</v>
       </c>
       <c r="H6" s="33"/>
     </row>
     <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="G7" s="39" t="s">
-        <v>535</v>
+        <v>524</v>
       </c>
       <c r="H7" s="33"/>
     </row>
     <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="38"/>
@@ -4406,25 +4134,25 @@
     </row>
     <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="G9" s="38" t="s">
-        <v>539</v>
+        <v>528</v>
       </c>
       <c r="H9" s="33"/>
     </row>
@@ -4438,7 +4166,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:K1048576"/>
+      <selection activeCell="G1" sqref="G1:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4455,28 +4183,28 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>21</v>
-      </c>
       <c r="F1" s="10" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
@@ -4484,65 +4212,65 @@
     </row>
     <row r="2" spans="1:11" ht="93" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>461</v>
+        <v>450</v>
       </c>
       <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="32"/>
       <c r="H3" s="9" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="32"/>
@@ -4550,19 +4278,19 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="32"/>
@@ -4570,19 +4298,19 @@
     </row>
     <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="32"/>
@@ -4590,19 +4318,19 @@
     </row>
     <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>91</v>
-      </c>
       <c r="E7" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="32"/>
@@ -4610,19 +4338,19 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="32"/>
@@ -4630,19 +4358,19 @@
     </row>
     <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="32"/>
@@ -4650,19 +4378,19 @@
     </row>
     <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="32"/>
@@ -4670,49 +4398,49 @@
     </row>
     <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>447</v>
+        <v>436</v>
       </c>
       <c r="H11" s="33"/>
     </row>
     <row r="12" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="G12" s="32" t="s">
-        <v>448</v>
+        <v>437</v>
       </c>
       <c r="H12" s="33"/>
     </row>
@@ -4746,1358 +4474,1358 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="I1" s="27" t="s">
-        <v>465</v>
+        <v>454</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>466</v>
+        <v>455</v>
       </c>
       <c r="K1" s="27" t="s">
-        <v>467</v>
+        <v>456</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="14" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="14" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="14" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>537</v>
+        <v>526</v>
       </c>
       <c r="H4" s="35" t="s">
-        <v>509</v>
+        <v>498</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D7" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>174</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>183</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="28" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>451</v>
+        <v>440</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="14" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>506</v>
+        <v>495</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>457</v>
+        <v>446</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>456</v>
+        <v>445</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="G15" s="28" t="s">
+        <v>448</v>
+      </c>
+      <c r="I15" s="28" t="s">
         <v>459</v>
       </c>
-      <c r="I15" s="28" t="s">
-        <v>470</v>
-      </c>
       <c r="J15" s="28" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
       <c r="K15" s="28" t="s">
-        <v>472</v>
+        <v>461</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>458</v>
+        <v>447</v>
       </c>
       <c r="I16" s="28" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="J16" s="28" t="s">
-        <v>474</v>
+        <v>463</v>
       </c>
       <c r="K16" s="28" t="s">
-        <v>475</v>
+        <v>464</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="14" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="14" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="14" t="s">
-        <v>511</v>
+        <v>500</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>510</v>
+        <v>499</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="14" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="14" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
       <c r="I21" s="29" t="s">
-        <v>476</v>
+        <v>465</v>
       </c>
       <c r="J21" s="29" t="s">
-        <v>477</v>
+        <v>466</v>
       </c>
       <c r="K21" s="29" t="s">
-        <v>478</v>
+        <v>467</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>453</v>
+        <v>442</v>
       </c>
       <c r="I22" s="28" t="s">
-        <v>479</v>
+        <v>468</v>
       </c>
       <c r="J22" s="28" t="s">
-        <v>480</v>
+        <v>469</v>
       </c>
       <c r="K22" s="28" t="s">
-        <v>481</v>
+        <v>470</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="13" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>482</v>
+        <v>471</v>
       </c>
       <c r="H23" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="14" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
       <c r="F25" s="14" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
       <c r="F26" s="14" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
       <c r="F27" s="14" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="G28" s="28" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="G29" s="28" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="D30" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="F30" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="E30" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>262</v>
-      </c>
       <c r="G30" s="28" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
       <c r="F31" s="14" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="G31" s="31" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="I31" s="31" t="s">
-        <v>484</v>
+        <v>473</v>
       </c>
       <c r="J31" s="31" t="s">
-        <v>485</v>
+        <v>474</v>
       </c>
       <c r="K31" s="31" t="s">
-        <v>486</v>
+        <v>475</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
       <c r="F32" s="14" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="G32" s="29" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="I32" s="29" t="s">
-        <v>487</v>
+        <v>476</v>
       </c>
       <c r="J32" s="29" t="s">
-        <v>488</v>
+        <v>477</v>
       </c>
       <c r="K32" s="29" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
       <c r="F33" s="14" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="G33" s="29" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
       <c r="F34" s="14" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="G34" s="29" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="I34" s="29" t="s">
-        <v>490</v>
+        <v>479</v>
       </c>
       <c r="J34" s="29" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="K34" s="29" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="15" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="G35" s="28" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="15" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="G36" s="28" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="G37" s="28" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="15" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="15" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="G38" s="28" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="15" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="20"/>
       <c r="F39" s="14" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="G39" s="28" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A40" s="15" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="20"/>
       <c r="F40" s="14" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="G40" s="28" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="H40" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="15" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="20" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
       <c r="G41" s="29" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
       <c r="H41" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="15" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="20"/>
       <c r="F42" s="14" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="G42" s="28" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="20"/>
       <c r="F43" s="14" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="G43" s="29" t="s">
-        <v>515</v>
+        <v>504</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="15" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A45" s="15" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="G45" s="28" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
       <c r="I45" s="28" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="J45" s="28" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
       <c r="K45" s="28" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A46" s="15" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="15" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
       <c r="F47" s="14" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="15" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="20"/>
       <c r="F48" s="19" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="G48" s="28" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="15" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="E49" s="20"/>
       <c r="F49" s="14" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="15" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="20"/>
       <c r="F50" s="14" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="15" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="20"/>
       <c r="F51" s="14" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="G51" s="31" t="s">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="I51" s="31" t="s">
-        <v>517</v>
+        <v>506</v>
       </c>
       <c r="J51" s="31" t="s">
-        <v>518</v>
+        <v>507</v>
       </c>
       <c r="K51" s="31" t="s">
-        <v>519</v>
+        <v>508</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A52" s="15" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="20"/>
       <c r="F52" s="14" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="G52" s="28" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
       <c r="I52" s="28" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
       <c r="J52" s="28" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
       <c r="K52" s="28" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A53" s="15" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="D53" s="15"/>
       <c r="E53" s="15"/>
       <c r="F53" s="14" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="G53" s="29" t="s">
-        <v>455</v>
+        <v>444</v>
       </c>
       <c r="I53" s="29" t="s">
-        <v>496</v>
+        <v>485</v>
       </c>
       <c r="J53" s="29" t="s">
-        <v>497</v>
+        <v>486</v>
       </c>
       <c r="K53" s="29" t="s">
-        <v>498</v>
+        <v>487</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="15" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="15"/>
       <c r="F54" s="14" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="G54" s="28" t="s">
-        <v>528</v>
+        <v>517</v>
       </c>
       <c r="I54" s="28" t="s">
-        <v>529</v>
+        <v>518</v>
       </c>
       <c r="J54" s="28" t="s">
-        <v>530</v>
+        <v>519</v>
       </c>
       <c r="K54" s="28" t="s">
-        <v>531</v>
+        <v>520</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="15" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="E55" s="15"/>
       <c r="F55" s="14" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="G55" s="28" t="s">
-        <v>520</v>
+        <v>509</v>
       </c>
       <c r="I55" s="28" t="s">
-        <v>521</v>
+        <v>510</v>
       </c>
       <c r="J55" s="28" t="s">
-        <v>522</v>
+        <v>511</v>
       </c>
       <c r="K55" s="28" t="s">
-        <v>523</v>
+        <v>512</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="15" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="15"/>
       <c r="F56" s="14" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="G56" s="28" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="15" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57" s="15"/>
       <c r="F57" s="14" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="G57" s="31" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
       <c r="H57" s="35" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
       <c r="I57" s="31" t="s">
-        <v>499</v>
+        <v>488</v>
       </c>
       <c r="J57" s="31" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="K57" s="31" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="15" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="G58" s="28" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
       <c r="H58" s="35" t="s">
-        <v>469</v>
+        <v>458</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="15" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="D59" s="15"/>
       <c r="E59" s="15"/>
       <c r="F59" s="14" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="G59" s="28" t="s">
-        <v>524</v>
+        <v>513</v>
       </c>
       <c r="I59" s="28" t="s">
-        <v>525</v>
+        <v>514</v>
       </c>
       <c r="J59" s="28" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="K59" s="28" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated mappings for correct array handling
</commit_message>
<xml_diff>
--- a/Maps/sdtm_mapping_paths.xlsx
+++ b/Maps/sdtm_mapping_paths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\SDTM_mapper\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877B4A93-A46B-4D5D-87DD-B230E77EE1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B27FA80-F521-420D-A6D1-DEB7FAF21865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10380" yWindow="-19830" windowWidth="31995" windowHeight="17895" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -1809,9 +1809,6 @@
     <t>study.versions.studyDesigns.studyType.codeSystemVersion</t>
   </si>
   <si>
-    <t>study.versions.studyDesigns[studyType.code="C98388"].intentTypes.decode</t>
-  </si>
-  <si>
     <t>study.versions.studyDesigns[studyType.code="C98388"].intentTypes.code</t>
   </si>
   <si>
@@ -1819,9 +1816,6 @@
   </si>
   <si>
     <t>study.versions.studyDesigns[studyType.code="C98388"].intentTypes.codeSystemVersion</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns[studyType.code="C98388"].subTypes.decode</t>
   </si>
   <si>
     <t>study.versions.studyDesigns[studyType.code="C98388"].subTypes.code</t>
@@ -1888,6 +1882,12 @@
   </si>
   <si>
     <t>study.versions.studyDesigns.($EpochName := function($id) {(epochs[id=$id].label)}; studyCells.{armId: $EpochName(epochId[0])})</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C98388"].intentTypes.{id: decode}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns[studyType.code="C98388"].subTypes.{id: decode}</t>
   </si>
 </sst>
 </file>
@@ -2247,6 +2247,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2254,9 +2257,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2713,7 +2713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CEFEB0-0887-1349-82EC-A63800D98F30}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+    <sheetView zoomScale="87" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -2800,7 +2800,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="6"/>
       <c r="H3" s="9" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
@@ -2826,7 +2826,7 @@
         <v>361</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="31" x14ac:dyDescent="0.35">
@@ -2849,7 +2849,7 @@
         <v>363</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
@@ -2893,7 +2893,7 @@
         <v>365</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
@@ -2916,7 +2916,7 @@
         <v>366</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
@@ -2979,7 +2979,7 @@
         <v>368</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
   </sheetData>
@@ -3011,26 +3011,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="45" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -3425,13 +3425,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="46" t="s">
         <v>13</v>
       </c>
@@ -4013,7 +4013,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="38"/>
       <c r="H3" s="9" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -4036,7 +4036,7 @@
         <v>122</v>
       </c>
       <c r="G4" s="39" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H4" s="33"/>
     </row>
@@ -4060,7 +4060,7 @@
         <v>124</v>
       </c>
       <c r="G5" s="41" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="H5" s="33"/>
     </row>
@@ -4084,7 +4084,7 @@
         <v>126</v>
       </c>
       <c r="G6" s="39" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="H6" s="33"/>
     </row>
@@ -4108,7 +4108,7 @@
         <v>128</v>
       </c>
       <c r="G7" s="39" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="H7" s="33"/>
     </row>
@@ -4152,7 +4152,7 @@
         <v>132</v>
       </c>
       <c r="G9" s="38" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="H9" s="33"/>
     </row>
@@ -4453,8 +4453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DEA66B-9A3B-A542-95A2-9E48A8B13E1D}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScale="109" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="E46" zoomScale="109" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4542,7 +4542,7 @@
         <v>375</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="87" x14ac:dyDescent="0.35">
@@ -4561,7 +4561,7 @@
         <v>376</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="H4" s="35" t="s">
         <v>498</v>
@@ -5682,16 +5682,16 @@
         <v>333</v>
       </c>
       <c r="G54" s="28" t="s">
+        <v>515</v>
+      </c>
+      <c r="I54" s="28" t="s">
+        <v>516</v>
+      </c>
+      <c r="J54" s="28" t="s">
         <v>517</v>
       </c>
-      <c r="I54" s="28" t="s">
+      <c r="K54" s="28" t="s">
         <v>518</v>
-      </c>
-      <c r="J54" s="28" t="s">
-        <v>519</v>
-      </c>
-      <c r="K54" s="28" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
@@ -5712,16 +5712,16 @@
         <v>339</v>
       </c>
       <c r="G55" s="28" t="s">
+        <v>533</v>
+      </c>
+      <c r="I55" s="28" t="s">
         <v>509</v>
       </c>
-      <c r="I55" s="28" t="s">
+      <c r="J55" s="28" t="s">
         <v>510</v>
       </c>
-      <c r="J55" s="28" t="s">
+      <c r="K55" s="28" t="s">
         <v>511</v>
-      </c>
-      <c r="K55" s="28" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -5816,16 +5816,16 @@
         <v>356</v>
       </c>
       <c r="G59" s="28" t="s">
+        <v>534</v>
+      </c>
+      <c r="I59" s="28" t="s">
+        <v>512</v>
+      </c>
+      <c r="J59" s="28" t="s">
         <v>513</v>
       </c>
-      <c r="I59" s="28" t="s">
+      <c r="K59" s="28" t="s">
         <v>514</v>
-      </c>
-      <c r="J59" s="28" t="s">
-        <v>515</v>
-      </c>
-      <c r="K59" s="28" t="s">
-        <v>516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added TE + update readme
</commit_message>
<xml_diff>
--- a/Maps/sdtm_mapping_paths.xlsx
+++ b/Maps/sdtm_mapping_paths.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\SDTM_mapper\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF02826-FA8F-4BC6-A844-8300B1ACFCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9703863-7176-48E8-B68E-FC6F45150D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10890" yWindow="-20340" windowWidth="31995" windowHeight="17895" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4515" yWindow="-19065" windowWidth="27645" windowHeight="13335" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="527">
   <si>
     <t>Class</t>
   </si>
@@ -68,15 +68,9 @@
     <t>Timing</t>
   </si>
   <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>StudyArm</t>
   </si>
   <si>
-    <t>StudyElement</t>
-  </si>
-  <si>
     <t>StudyIdentifier</t>
   </si>
   <si>
@@ -117,9 +111,6 @@
   </si>
   <si>
     <t>Req </t>
-  </si>
-  <si>
-    <t>Y </t>
   </si>
   <si>
     <t>DOMAIN </t>
@@ -249,15 +240,6 @@
     <t>next</t>
   </si>
   <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@label</t>
-  </si>
-  <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@description</t>
-  </si>
-  <si>
-    <t>Set to "TA"</t>
-  </si>
-  <si>
     <t>Overall Notes</t>
   </si>
   <si>
@@ -321,18 +303,6 @@
     <t>Planned Duration of Element</t>
   </si>
   <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@transitionStartRule/TransitionRule/@text</t>
-  </si>
-  <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@transitionEndRule/TransitionRule/@text</t>
-  </si>
-  <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@scheduleTimelines/ScheduleTimeline/@timings/Timing/@value</t>
-  </si>
-  <si>
-    <t>The element length can be calculated based on timing values based on the used logic for a trial. For example select the last timing value of epoch related to the element and subtract the timing value of the last scheduledInstance referencing to the previous epoch.</t>
-  </si>
-  <si>
     <t>VISITNUM</t>
   </si>
   <si>
@@ -1161,9 +1131,6 @@
     <t>Element End Rule</t>
   </si>
   <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@id=StudyVersion/@studyDesigns/StudyDesign/@studyCells/StudyCell/@elements | StudyVersion/@studyDesigns/StudyDesign/@studyCells/StudyCell/@epoch = StudyVersion/@studyDesigns/StudyDesign/@scheduleTimelines/ScheduleTimeline/@instances/ScheduledActivityInstance/@epoch</t>
-  </si>
-  <si>
     <t>Element Duration</t>
   </si>
   <si>
@@ -1233,43 +1200,10 @@
     <t>USDM Columns</t>
   </si>
   <si>
-    <t>The target class in USDM where the M11 element is mapped</t>
-  </si>
-  <si>
-    <t>The target attribute in USDM where the M11 element is mapped</t>
-  </si>
-  <si>
-    <t>Notes on the overall mapping</t>
-  </si>
-  <si>
-    <t>The full path to the place in USDM holding the dtaa for the M11 element</t>
-  </si>
-  <si>
-    <t>Any notes relating to the target path</t>
-  </si>
-  <si>
-    <t>The conditions applicable to the target path mapping</t>
-  </si>
-  <si>
-    <t>Any associated notes relevant to the conditions</t>
-  </si>
-  <si>
-    <t>Mapping status, either "Mapped" or "To Be Mapped"</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Class and Attribute</t>
-  </si>
-  <si>
-    <t>The specified class and attribute to be used in a mapping are specified up to the level of reference, the complex datatype or lower if needed for specificity. The corresponding path further specifies specific the exact attributes used from complex datatypes or subclasses.</t>
-  </si>
-  <si>
     <t>Multiple Mappings</t>
-  </si>
-  <si>
-    <t>In some cases there is more than one mapping for the same M11 item. These mappings are usually distinct where either one of them may be used (and the other is expected to be not available) or they need to be all combined for the M11 item.</t>
   </si>
   <si>
     <t>SDTM Version</t>
@@ -1889,6 +1823,48 @@
   <si>
     <t>study.versions.studyDesigns.indications.{id: label}</t>
   </si>
+  <si>
+    <t>The name of the original mapping in DDF USDM v4.0</t>
+  </si>
+  <si>
+    <t>Fixed Content</t>
+  </si>
+  <si>
+    <t>The USDM v4.0 mappings combined to a JSONATA query</t>
+  </si>
+  <si>
+    <t>In case content is fixed and no mapping is needed the corresponding value is presented in this column</t>
+  </si>
+  <si>
+    <t>TSVALNF (in case of TS)</t>
+  </si>
+  <si>
+    <t>value to be presented in case no value is returned based on a JSONATA query</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In case there is more than one mapping for the same SDTM item these mappings are provided in separate rows in the USDM v4.0 mapping file. In this mapping file, they are combined again to 1 JSONata query. </t>
+  </si>
+  <si>
+    <t>Resulting domains</t>
+  </si>
+  <si>
+    <t>For the resulting domains, the specified variables are transposed to columns and the result values are presented in rows.</t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.elements.{id: label}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.elements.{id: description}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.elements.{id: transitionStartRule.text}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.elements.{id: transitionEndRule.text}</t>
+  </si>
 </sst>
 </file>
 
@@ -1978,7 +1954,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2011,6 +1987,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2191,17 +2173,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2247,9 +2220,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2267,6 +2237,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2575,8 +2557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2587,121 +2569,105 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>413</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>408</v>
+        <v>386</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>412</v>
+        <v>390</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>410</v>
+        <v>388</v>
       </c>
       <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>409</v>
+        <v>387</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="B7" s="17"/>
     </row>
-    <row r="9" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>395</v>
+        <v>513</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
-        <v>1</v>
+        <v>392</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
-        <v>70</v>
+        <v>514</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>397</v>
+        <v>516</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
-        <v>53</v>
+        <v>517</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>398</v>
+        <v>518</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>399</v>
-      </c>
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
     </row>
     <row r="14" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>400</v>
-      </c>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
     </row>
     <row r="15" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>401</v>
-      </c>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
     </row>
     <row r="16" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>402</v>
-      </c>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
     </row>
     <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
-        <v>403</v>
+        <v>384</v>
       </c>
       <c r="B18" s="17"/>
     </row>
-    <row r="20" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="62" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
-        <v>404</v>
+        <v>385</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="18" t="s">
-        <v>406</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>407</v>
+        <v>519</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>520</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>521</v>
       </c>
     </row>
   </sheetData>
@@ -2713,94 +2679,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CEFEB0-0887-1349-82EC-A63800D98F30}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A2" zoomScale="87" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="17.81640625" customWidth="1"/>
     <col min="6" max="6" width="25.81640625" customWidth="1"/>
-    <col min="7" max="7" width="30.08984375" style="41" customWidth="1"/>
+    <col min="7" max="7" width="30.08984375" style="38" customWidth="1"/>
     <col min="8" max="8" width="18.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="37" t="s">
-        <v>414</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>434</v>
-      </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
+        <v>65</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>412</v>
+      </c>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>449</v>
-      </c>
-      <c r="H2" s="33"/>
+        <v>427</v>
+      </c>
+      <c r="H2" s="30"/>
       <c r="I2" s="16"/>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
     </row>
     <row r="3" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="6"/>
       <c r="H3" s="9" t="s">
-        <v>520</v>
+        <v>498</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
@@ -2808,178 +2774,178 @@
     </row>
     <row r="4" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F4" s="6" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>521</v>
+        <v>499</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F5" s="6" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>522</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>37</v>
-      </c>
       <c r="E6" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F7" s="6" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>523</v>
+        <v>501</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>524</v>
+        <v>502</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="F11" s="6" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>525</v>
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -2989,10 +2955,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF74871-8230-F544-A683-17CFA4CB76B6}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3000,406 +2966,205 @@
     <col min="1" max="1" width="18.36328125" customWidth="1"/>
     <col min="2" max="2" width="20.36328125" customWidth="1"/>
     <col min="3" max="5" width="9.36328125" customWidth="1"/>
-    <col min="6" max="6" width="18.1796875" customWidth="1"/>
-    <col min="7" max="7" width="18.81640625" customWidth="1"/>
-    <col min="8" max="9" width="39.453125" customWidth="1"/>
-    <col min="10" max="10" width="25.81640625" customWidth="1"/>
-    <col min="11" max="11" width="49.36328125" customWidth="1"/>
-    <col min="12" max="12" width="45.6328125" customWidth="1"/>
-    <col min="13" max="13" width="25.81640625" customWidth="1"/>
-    <col min="16" max="16" width="15.36328125" style="23" customWidth="1"/>
+    <col min="6" max="6" width="25.81640625" customWidth="1"/>
+    <col min="7" max="7" width="39.90625" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" style="46"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="42" t="s">
+    <row r="1" spans="1:11" ht="42" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-    </row>
-    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="11" t="s">
+      <c r="F1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>412</v>
+      </c>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+    </row>
+    <row r="2" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>427</v>
+      </c>
+      <c r="H2" s="48"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="P2" s="24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>62</v>
-      </c>
       <c r="C3" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>379</v>
+      </c>
+      <c r="G4" s="47" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="P3" s="22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+      <c r="B5" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="25"/>
-    </row>
-    <row r="5" spans="1:16" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
+      <c r="E5" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="G5" s="47" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B6" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="C6" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="12" t="s">
+      <c r="E6" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="G6" s="47" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="D7" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>360</v>
       </c>
-      <c r="K5" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>390</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="P5" s="25"/>
-    </row>
-    <row r="6" spans="1:16" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="G7" s="47" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>391</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="P6" s="25"/>
-    </row>
-    <row r="7" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>369</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="P7" s="25"/>
-    </row>
-    <row r="8" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>88</v>
-      </c>
       <c r="F8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="M8" s="12" t="s">
-        <v>370</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="P8" s="25"/>
-    </row>
-    <row r="9" spans="1:16" ht="145" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>371</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>360</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>372</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>373</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="P9" s="25"/>
+        <v>361</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F1:P1"/>
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="I5" r:id="rId1" xr:uid="{E053A7EE-A6B6-0C49-A873-A5D47AAC1488}"/>
-    <hyperlink ref="I6" r:id="rId2" display="StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@label" xr:uid="{31AD9372-B2CC-694E-9277-8272D6713D7A}"/>
-    <hyperlink ref="I7" r:id="rId3" display="StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@label" xr:uid="{01BA93B0-461F-464E-B492-C18F62119A7F}"/>
-    <hyperlink ref="I8" r:id="rId4" display="StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@label" xr:uid="{77173A6E-AC0D-0E4B-A5F9-0736669220F5}"/>
-    <hyperlink ref="K9" r:id="rId5" display="StudyVersion/@studyDesigns/StudyDesign/@elements/StudyElement/@id=StudyVersion/@studyDesigns/StudyDesign/@studyCells/StudyCell/@elements" xr:uid="{C8126432-A48E-4046-9B2B-EA181A78C848}"/>
-    <hyperlink ref="I9" r:id="rId6" xr:uid="{DD078117-90CA-FA4E-8C1D-A39EBDABA681}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3421,46 +3186,46 @@
     <col min="8" max="8" width="60.453125" customWidth="1"/>
     <col min="9" max="13" width="26" customWidth="1"/>
     <col min="14" max="15" width="19.453125" customWidth="1"/>
-    <col min="16" max="16" width="16.36328125" style="23" customWidth="1"/>
+    <col min="16" max="16" width="16.36328125" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="48"/>
+      <c r="A1" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="44"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>0</v>
@@ -3469,99 +3234,99 @@
         <v>1</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="P3" s="26" t="s">
-        <v>120</v>
+      <c r="P3" s="23" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -3570,119 +3335,119 @@
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
-      <c r="P4" s="26"/>
+      <c r="P4" s="23"/>
     </row>
     <row r="5" spans="1:16" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="P5" s="26" t="s">
-        <v>120</v>
+        <v>60</v>
+      </c>
+      <c r="P5" s="23" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="P6" s="26" t="s">
-        <v>120</v>
+        <v>60</v>
+      </c>
+      <c r="P6" s="23" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>7</v>
@@ -3692,220 +3457,220 @@
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="P7" s="26" t="s">
-        <v>120</v>
+        <v>60</v>
+      </c>
+      <c r="P7" s="23" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="P8" s="26" t="s">
-        <v>120</v>
+        <v>60</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>88</v>
-      </c>
       <c r="F9" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>2</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="P9" s="26" t="s">
-        <v>120</v>
+        <v>60</v>
+      </c>
+      <c r="P9" s="23" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="P10" s="26" t="s">
-        <v>120</v>
+        <v>60</v>
+      </c>
+      <c r="P10" s="23" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="P11" s="26" t="s">
-        <v>120</v>
+        <v>60</v>
+      </c>
+      <c r="P11" s="23" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -3928,233 +3693,233 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A2D413-6E3B-5A40-9DE8-0245851A536D}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K3" sqref="G1:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="5" width="18.6328125" customWidth="1"/>
     <col min="6" max="6" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.6328125" style="40" customWidth="1"/>
+    <col min="7" max="7" width="26.6328125" style="37" customWidth="1"/>
     <col min="8" max="8" width="29.81640625" style="16" customWidth="1"/>
     <col min="9" max="11" width="8.6328125" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>18</v>
-      </c>
       <c r="F1" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="37" t="s">
-        <v>414</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>434</v>
-      </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
+        <v>65</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>412</v>
+      </c>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="34" t="s">
-        <v>449</v>
-      </c>
-      <c r="H2" s="33"/>
+        <v>58</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>427</v>
+      </c>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="38"/>
+      <c r="G3" s="35"/>
       <c r="H3" s="9" t="s">
-        <v>512</v>
+        <v>490</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>79</v>
-      </c>
       <c r="E4" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>513</v>
-      </c>
-      <c r="H4" s="33"/>
+        <v>112</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>491</v>
+      </c>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="G5" s="41" t="s">
-        <v>518</v>
-      </c>
-      <c r="H5" s="33"/>
+        <v>114</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>496</v>
+      </c>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="G6" s="39" t="s">
-        <v>514</v>
-      </c>
-      <c r="H6" s="33"/>
+        <v>116</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>492</v>
+      </c>
+      <c r="H6" s="30"/>
     </row>
     <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="G7" s="39" t="s">
-        <v>515</v>
-      </c>
-      <c r="H7" s="33"/>
+        <v>118</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>493</v>
+      </c>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="33"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="G9" s="38" t="s">
-        <v>519</v>
-      </c>
-      <c r="H9" s="33"/>
+        <v>122</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>497</v>
+      </c>
+      <c r="H9" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4165,8 +3930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF8120D-B51B-094C-AABA-CA55EB26DD5D}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:K3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4183,266 +3948,266 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>18</v>
-      </c>
       <c r="F1" s="10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>434</v>
-      </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
+        <v>392</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>412</v>
+      </c>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="93" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="34" t="s">
-        <v>449</v>
-      </c>
-      <c r="H2" s="33"/>
+        <v>58</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>427</v>
+      </c>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F3" s="5"/>
-      <c r="G3" s="32"/>
+      <c r="G3" s="29"/>
       <c r="H3" s="9" t="s">
-        <v>450</v>
+        <v>428</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="33"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F5" s="12"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="33"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>79</v>
-      </c>
       <c r="E6" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F6" s="12"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="33"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="30"/>
     </row>
     <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F7" s="12"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="33"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F8" s="12"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="33"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F9" s="12"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="33"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="30"/>
     </row>
     <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F10" s="12"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="33"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30"/>
     </row>
     <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="G11" s="32" t="s">
-        <v>435</v>
-      </c>
-      <c r="H11" s="33"/>
+        <v>140</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>413</v>
+      </c>
+      <c r="H11" s="30"/>
     </row>
     <row r="12" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>392</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>436</v>
-      </c>
-      <c r="H12" s="33"/>
+        <v>381</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>414</v>
+      </c>
+      <c r="H12" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4453,8 +4218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DEA66B-9A3B-A542-95A2-9E48A8B13E1D}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="109" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="I1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4474,1358 +4239,1358 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>451</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>452</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>453</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>454</v>
-      </c>
-      <c r="K1" s="27" t="s">
-        <v>455</v>
+        <v>126</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>429</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>430</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>431</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>432</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>415</v>
+        <v>363</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="14" t="s">
-        <v>375</v>
-      </c>
-      <c r="G3" s="28" t="s">
-        <v>516</v>
+        <v>364</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="14" t="s">
-        <v>376</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>517</v>
-      </c>
-      <c r="H4" s="35" t="s">
-        <v>497</v>
+        <v>365</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>495</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>416</v>
+        <v>366</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>417</v>
+        <v>367</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="F7" s="14"/>
-      <c r="G7" s="28" t="s">
-        <v>448</v>
+      <c r="G7" s="25" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D8" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>165</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>437</v>
-      </c>
-      <c r="G10" s="28" t="s">
-        <v>438</v>
+        <v>415</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>379</v>
-      </c>
-      <c r="G11" s="28" t="s">
-        <v>439</v>
+        <v>368</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="G12" s="28" t="s">
-        <v>494</v>
+        <v>181</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>380</v>
-      </c>
-      <c r="G13" s="28" t="s">
-        <v>445</v>
+        <v>369</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="G14" s="28" t="s">
-        <v>444</v>
+        <v>187</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>381</v>
-      </c>
-      <c r="G15" s="28" t="s">
-        <v>447</v>
-      </c>
-      <c r="I15" s="28" t="s">
-        <v>458</v>
-      </c>
-      <c r="J15" s="28" t="s">
-        <v>459</v>
-      </c>
-      <c r="K15" s="28" t="s">
-        <v>460</v>
+        <v>370</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>425</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>436</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>437</v>
+      </c>
+      <c r="K15" s="25" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>382</v>
-      </c>
-      <c r="G16" s="28" t="s">
-        <v>446</v>
-      </c>
-      <c r="I16" s="28" t="s">
-        <v>461</v>
-      </c>
-      <c r="J16" s="28" t="s">
-        <v>462</v>
-      </c>
-      <c r="K16" s="28" t="s">
-        <v>463</v>
+        <v>371</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>424</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>439</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>440</v>
+      </c>
+      <c r="K16" s="25" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="G17" s="36" t="s">
-        <v>496</v>
+        <v>196</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="14" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="14" t="s">
-        <v>499</v>
-      </c>
-      <c r="G19" s="28" t="s">
-        <v>498</v>
+        <v>477</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="G20" s="28" t="s">
-        <v>534</v>
+        <v>372</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="G21" s="29" t="s">
-        <v>420</v>
-      </c>
-      <c r="I21" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="J21" s="29" t="s">
-        <v>465</v>
-      </c>
-      <c r="K21" s="29" t="s">
-        <v>466</v>
+        <v>208</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>398</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>442</v>
+      </c>
+      <c r="J21" s="26" t="s">
+        <v>443</v>
+      </c>
+      <c r="K21" s="26" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="G22" s="28" t="s">
-        <v>441</v>
-      </c>
-      <c r="I22" s="28" t="s">
-        <v>467</v>
-      </c>
-      <c r="J22" s="28" t="s">
-        <v>468</v>
-      </c>
-      <c r="K22" s="28" t="s">
-        <v>469</v>
+        <v>211</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>419</v>
+      </c>
+      <c r="I22" s="25" t="s">
+        <v>445</v>
+      </c>
+      <c r="J22" s="25" t="s">
+        <v>446</v>
+      </c>
+      <c r="K22" s="25" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="13" t="s">
-        <v>411</v>
-      </c>
-      <c r="G23" s="28" t="s">
-        <v>470</v>
+        <v>389</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>448</v>
       </c>
       <c r="H23" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="14" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
       <c r="F25" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="G25" s="28" t="s">
-        <v>421</v>
+        <v>223</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
       <c r="F26" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="G26" s="29" t="s">
-        <v>471</v>
+        <v>224</v>
+      </c>
+      <c r="G26" s="26" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
       <c r="F27" s="14" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="G28" s="28" t="s">
-        <v>430</v>
+        <v>233</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="G29" s="28" t="s">
-        <v>428</v>
+        <v>239</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="G30" s="28" t="s">
-        <v>429</v>
+        <v>243</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
       <c r="F31" s="14" t="s">
-        <v>254</v>
-      </c>
-      <c r="G31" s="31" t="s">
-        <v>424</v>
-      </c>
-      <c r="I31" s="31" t="s">
-        <v>472</v>
-      </c>
-      <c r="J31" s="31" t="s">
-        <v>473</v>
-      </c>
-      <c r="K31" s="31" t="s">
-        <v>474</v>
+        <v>244</v>
+      </c>
+      <c r="G31" s="28" t="s">
+        <v>402</v>
+      </c>
+      <c r="I31" s="28" t="s">
+        <v>450</v>
+      </c>
+      <c r="J31" s="28" t="s">
+        <v>451</v>
+      </c>
+      <c r="K31" s="28" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
       <c r="F32" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="G32" s="29" t="s">
-        <v>425</v>
-      </c>
-      <c r="I32" s="29" t="s">
-        <v>475</v>
-      </c>
-      <c r="J32" s="29" t="s">
-        <v>476</v>
-      </c>
-      <c r="K32" s="29" t="s">
-        <v>477</v>
+        <v>247</v>
+      </c>
+      <c r="G32" s="26" t="s">
+        <v>403</v>
+      </c>
+      <c r="I32" s="26" t="s">
+        <v>453</v>
+      </c>
+      <c r="J32" s="26" t="s">
+        <v>454</v>
+      </c>
+      <c r="K32" s="26" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
       <c r="F33" s="14" t="s">
-        <v>385</v>
-      </c>
-      <c r="G33" s="29" t="s">
-        <v>426</v>
+        <v>374</v>
+      </c>
+      <c r="G33" s="26" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
       <c r="F34" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="G34" s="29" t="s">
-        <v>427</v>
-      </c>
-      <c r="I34" s="29" t="s">
-        <v>478</v>
-      </c>
-      <c r="J34" s="29" t="s">
-        <v>479</v>
-      </c>
-      <c r="K34" s="29" t="s">
-        <v>480</v>
+        <v>253</v>
+      </c>
+      <c r="G34" s="26" t="s">
+        <v>405</v>
+      </c>
+      <c r="I34" s="26" t="s">
+        <v>456</v>
+      </c>
+      <c r="J34" s="26" t="s">
+        <v>457</v>
+      </c>
+      <c r="K34" s="26" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="15" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="G35" s="28" t="s">
-        <v>433</v>
+        <v>256</v>
+      </c>
+      <c r="G35" s="25" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="15" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="G36" s="28" t="s">
-        <v>431</v>
+        <v>261</v>
+      </c>
+      <c r="G36" s="25" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="G37" s="28" t="s">
-        <v>432</v>
+        <v>264</v>
+      </c>
+      <c r="G37" s="25" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="15" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="15" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="G38" s="28" t="s">
-        <v>500</v>
+        <v>267</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="15" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="20"/>
       <c r="F39" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="G39" s="28" t="s">
-        <v>501</v>
+        <v>270</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A40" s="15" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="20"/>
       <c r="F40" s="14" t="s">
-        <v>386</v>
-      </c>
-      <c r="G40" s="28" t="s">
-        <v>423</v>
+        <v>375</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>401</v>
       </c>
       <c r="H40" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="15" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="20" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>387</v>
-      </c>
-      <c r="G41" s="29" t="s">
-        <v>442</v>
+        <v>376</v>
+      </c>
+      <c r="G41" s="26" t="s">
+        <v>420</v>
       </c>
       <c r="H41" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="15" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="20"/>
       <c r="F42" s="14" t="s">
-        <v>292</v>
-      </c>
-      <c r="G42" s="28" t="s">
-        <v>502</v>
+        <v>282</v>
+      </c>
+      <c r="G42" s="25" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="20"/>
       <c r="F43" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="G43" s="29" t="s">
-        <v>503</v>
+        <v>286</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="15" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A45" s="15" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="G45" s="28" t="s">
-        <v>490</v>
-      </c>
-      <c r="I45" s="28" t="s">
-        <v>491</v>
-      </c>
-      <c r="J45" s="28" t="s">
-        <v>492</v>
-      </c>
-      <c r="K45" s="28" t="s">
-        <v>493</v>
+        <v>292</v>
+      </c>
+      <c r="G45" s="25" t="s">
+        <v>468</v>
+      </c>
+      <c r="I45" s="25" t="s">
+        <v>469</v>
+      </c>
+      <c r="J45" s="25" t="s">
+        <v>470</v>
+      </c>
+      <c r="K45" s="25" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A46" s="15" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="15" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
       <c r="F47" s="14" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="15" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="20"/>
       <c r="F48" s="19" t="s">
-        <v>388</v>
-      </c>
-      <c r="G48" s="28" t="s">
-        <v>495</v>
+        <v>377</v>
+      </c>
+      <c r="G48" s="25" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="15" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="E49" s="20"/>
       <c r="F49" s="14" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="15" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="20"/>
       <c r="F50" s="14" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="15" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="20"/>
       <c r="F51" s="14" t="s">
-        <v>324</v>
-      </c>
-      <c r="G51" s="31" t="s">
-        <v>504</v>
-      </c>
-      <c r="I51" s="31" t="s">
-        <v>505</v>
-      </c>
-      <c r="J51" s="31" t="s">
-        <v>506</v>
-      </c>
-      <c r="K51" s="31" t="s">
-        <v>507</v>
+        <v>314</v>
+      </c>
+      <c r="G51" s="28" t="s">
+        <v>482</v>
+      </c>
+      <c r="I51" s="28" t="s">
+        <v>483</v>
+      </c>
+      <c r="J51" s="28" t="s">
+        <v>484</v>
+      </c>
+      <c r="K51" s="28" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A52" s="15" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="20"/>
       <c r="F52" s="14" t="s">
-        <v>328</v>
-      </c>
-      <c r="G52" s="28" t="s">
-        <v>422</v>
-      </c>
-      <c r="I52" s="28" t="s">
-        <v>481</v>
-      </c>
-      <c r="J52" s="28" t="s">
-        <v>482</v>
-      </c>
-      <c r="K52" s="28" t="s">
-        <v>483</v>
+        <v>318</v>
+      </c>
+      <c r="G52" s="25" t="s">
+        <v>400</v>
+      </c>
+      <c r="I52" s="25" t="s">
+        <v>459</v>
+      </c>
+      <c r="J52" s="25" t="s">
+        <v>460</v>
+      </c>
+      <c r="K52" s="25" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A53" s="15" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="D53" s="15"/>
       <c r="E53" s="15"/>
       <c r="F53" s="14" t="s">
-        <v>332</v>
-      </c>
-      <c r="G53" s="29" t="s">
-        <v>443</v>
-      </c>
-      <c r="I53" s="29" t="s">
-        <v>484</v>
-      </c>
-      <c r="J53" s="29" t="s">
-        <v>485</v>
-      </c>
-      <c r="K53" s="29" t="s">
-        <v>486</v>
+        <v>322</v>
+      </c>
+      <c r="G53" s="26" t="s">
+        <v>421</v>
+      </c>
+      <c r="I53" s="26" t="s">
+        <v>462</v>
+      </c>
+      <c r="J53" s="26" t="s">
+        <v>463</v>
+      </c>
+      <c r="K53" s="26" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="15" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="15"/>
       <c r="F54" s="14" t="s">
-        <v>333</v>
-      </c>
-      <c r="G54" s="28" t="s">
-        <v>508</v>
-      </c>
-      <c r="I54" s="28" t="s">
-        <v>509</v>
-      </c>
-      <c r="J54" s="28" t="s">
-        <v>510</v>
-      </c>
-      <c r="K54" s="28" t="s">
-        <v>511</v>
+        <v>323</v>
+      </c>
+      <c r="G54" s="25" t="s">
+        <v>486</v>
+      </c>
+      <c r="I54" s="25" t="s">
+        <v>487</v>
+      </c>
+      <c r="J54" s="25" t="s">
+        <v>488</v>
+      </c>
+      <c r="K54" s="25" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="15" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="E55" s="15"/>
       <c r="F55" s="14" t="s">
-        <v>339</v>
-      </c>
-      <c r="G55" s="28" t="s">
-        <v>526</v>
-      </c>
-      <c r="I55" s="28" t="s">
-        <v>528</v>
-      </c>
-      <c r="J55" s="28" t="s">
-        <v>529</v>
-      </c>
-      <c r="K55" s="28" t="s">
-        <v>530</v>
+        <v>329</v>
+      </c>
+      <c r="G55" s="25" t="s">
+        <v>504</v>
+      </c>
+      <c r="I55" s="25" t="s">
+        <v>506</v>
+      </c>
+      <c r="J55" s="25" t="s">
+        <v>507</v>
+      </c>
+      <c r="K55" s="25" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="15" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="15"/>
       <c r="F56" s="14" t="s">
-        <v>344</v>
-      </c>
-      <c r="G56" s="28" t="s">
-        <v>418</v>
+        <v>334</v>
+      </c>
+      <c r="G56" s="25" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="15" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57" s="15"/>
       <c r="F57" s="14" t="s">
-        <v>348</v>
-      </c>
-      <c r="G57" s="31" t="s">
-        <v>419</v>
-      </c>
-      <c r="H57" s="35" t="s">
-        <v>456</v>
-      </c>
-      <c r="I57" s="31" t="s">
-        <v>487</v>
-      </c>
-      <c r="J57" s="31" t="s">
-        <v>488</v>
-      </c>
-      <c r="K57" s="31" t="s">
-        <v>489</v>
+        <v>338</v>
+      </c>
+      <c r="G57" s="28" t="s">
+        <v>397</v>
+      </c>
+      <c r="H57" s="32" t="s">
+        <v>434</v>
+      </c>
+      <c r="I57" s="28" t="s">
+        <v>465</v>
+      </c>
+      <c r="J57" s="28" t="s">
+        <v>466</v>
+      </c>
+      <c r="K57" s="28" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="15" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>352</v>
-      </c>
-      <c r="G58" s="28" t="s">
-        <v>440</v>
-      </c>
-      <c r="H58" s="35" t="s">
-        <v>457</v>
+        <v>342</v>
+      </c>
+      <c r="G58" s="25" t="s">
+        <v>418</v>
+      </c>
+      <c r="H58" s="32" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="15" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="D59" s="15"/>
       <c r="E59" s="15"/>
       <c r="F59" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="G59" s="28" t="s">
-        <v>527</v>
-      </c>
-      <c r="I59" s="28" t="s">
-        <v>531</v>
-      </c>
-      <c r="J59" s="28" t="s">
-        <v>532</v>
-      </c>
-      <c r="K59" s="28" t="s">
-        <v>533</v>
+        <v>346</v>
+      </c>
+      <c r="G59" s="25" t="s">
+        <v>505</v>
+      </c>
+      <c r="I59" s="25" t="s">
+        <v>509</v>
+      </c>
+      <c r="J59" s="25" t="s">
+        <v>510</v>
+      </c>
+      <c r="K59" s="25" t="s">
+        <v>511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added mapping of TV domain
</commit_message>
<xml_diff>
--- a/Maps/sdtm_mapping_paths.xlsx
+++ b/Maps/sdtm_mapping_paths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\SDTM_mapper\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A53CBE-1FD0-4B3E-9F43-5E2E37DB15F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE15098-C11F-4849-B0D7-8E3E1A74B54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20700" yWindow="-19200" windowWidth="19830" windowHeight="15225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20895" yWindow="-17145" windowWidth="39225" windowHeight="15225" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -42,25 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4294960377" uniqueCount="527">
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>Attribute</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>Condition Notes</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="495">
   <si>
     <t>Identifier</t>
   </si>
@@ -68,18 +50,6 @@
     <t>Timing</t>
   </si>
   <si>
-    <t>StudyArm</t>
-  </si>
-  <si>
-    <t>StudyIdentifier</t>
-  </si>
-  <si>
-    <t>TransitionRule</t>
-  </si>
-  <si>
-    <t>USDM</t>
-  </si>
-  <si>
     <t>Variable Name </t>
   </si>
   <si>
@@ -95,9 +65,6 @@
     <t>Core </t>
   </si>
   <si>
-    <t>v4.0 Change </t>
-  </si>
-  <si>
     <t>STUDYID </t>
   </si>
   <si>
@@ -191,58 +158,12 @@
     <t>Epoch </t>
   </si>
   <si>
-    <t>SDTM</t>
-  </si>
-  <si>
-    <t>Target Path</t>
-  </si>
-  <si>
-    <t>Condition Path</t>
-  </si>
-  <si>
-    <t>Target Notes</t>
-  </si>
-  <si>
-    <t>Mapping Category</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>StudyVersion/@studyIdentifiers/StudyIdentifier/@text</t>
-  </si>
-  <si>
-    <t>StudyRole/@code/Code/@code="C70793" | 
-StudyRole/@organizations | 
-StudyVersion/@studyIdentifiers/StudyIdentifier/@scope</t>
-  </si>
-  <si>
-    <t>Identifies the sponsor role | 
-Identifies the sponsor organization from the role | 
-Identifies the sponsor organization from the study identifier</t>
-  </si>
-  <si>
     <t>Sponsor Study Identifier</t>
   </si>
   <si>
     <t>Study Identifier</t>
   </si>
   <si>
-    <t>Mapped</t>
-  </si>
-  <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@arms/StudyArm/@label</t>
-  </si>
-  <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@arms/StudyArm/@description</t>
-  </si>
-  <si>
-    <t>next</t>
-  </si>
-  <si>
-    <t>Overall Notes</t>
-  </si>
-  <si>
     <t>Mapping Name</t>
   </si>
   <si>
@@ -354,33 +275,6 @@
     <t>Exp</t>
   </si>
   <si>
-    <t>Encounter</t>
-  </si>
-  <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@encounters/Encounter/@next</t>
-  </si>
-  <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@encounters/Encounter/@label</t>
-  </si>
-  <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@encounters /Encounter/@scheduledAt/Timing/@label</t>
-  </si>
-  <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@encounters /Encounter/@transitionEndRule /TransitionRule/@text</t>
-  </si>
-  <si>
-    <t>StudyVersion/@studyDesigns/StudyDesign/@encounters/Encounter/@transitionStartRule/TransitionRule/@text</t>
-  </si>
-  <si>
-    <t>Set to "TV"</t>
-  </si>
-  <si>
-    <t>Order encounters according to their next attributes (pointing to the next encounter) and apply the corresponding sponsor defined visit numbering logic to it.</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>IETESTCD</t>
   </si>
   <si>
@@ -1098,15 +992,9 @@
     <t>C Code</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Arm Name</t>
   </si>
   <si>
-    <t>Study Design</t>
-  </si>
-  <si>
     <t>Arm Description</t>
   </si>
   <si>
@@ -1132,9 +1020,6 @@
   </si>
   <si>
     <t>Element Duration</t>
-  </si>
-  <si>
-    <t>Study Timeline</t>
   </si>
   <si>
     <t>Adaptive Design Indicator</t>
@@ -1387,101 +1272,6 @@
     <t>study.versions.studyDesigns[studyType.code="C98388"].model.decode</t>
   </si>
   <si>
-    <r>
-      <t>$count</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>study</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>versions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>studyDesigns</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>arms</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>study.versions.studyDesigns.blindingSchema.standardCode.decode</t>
   </si>
   <si>
@@ -1864,6 +1654,24 @@
   </si>
   <si>
     <t>study.versions.studyDesigns.($EpochName := function($id) {(epochs[id=$id].label)}; studyCells.{armId: armId, elementIds[0]: $EpochName(epochId)})</t>
+  </si>
+  <si>
+    <t>$count(study.versions.studyDesigns.arms)</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.encounters.label</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.encounters .scheduledAt.label</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.encounters .transitionEndRule .text</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.encounters.transitionStartRule.text</t>
   </si>
 </sst>
 </file>
@@ -1954,7 +1762,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1984,20 +1792,8 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -2025,30 +1821,6 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -2105,12 +1877,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2139,10 +1924,10 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2170,28 +1955,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2199,13 +1965,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2220,29 +1980,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2563,67 +2336,67 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>382</v>
+        <v>345</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>391</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>386</v>
+        <v>349</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>390</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>388</v>
+        <v>351</v>
       </c>
       <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>387</v>
+        <v>350</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
-        <v>383</v>
+        <v>346</v>
       </c>
       <c r="B7" s="17"/>
     </row>
     <row r="9" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>510</v>
+        <v>472</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
-        <v>392</v>
+        <v>355</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>512</v>
+        <v>474</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
-        <v>511</v>
+        <v>473</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>513</v>
+        <v>475</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
-        <v>514</v>
+        <v>476</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>515</v>
+        <v>477</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -2644,24 +2417,24 @@
     </row>
     <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
-        <v>384</v>
+        <v>347</v>
       </c>
       <c r="B18" s="17"/>
     </row>
     <row r="20" spans="1:2" ht="62" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
-        <v>385</v>
+        <v>348</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>516</v>
+        <v>478</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>517</v>
-      </c>
-      <c r="B21" s="38" t="s">
-        <v>518</v>
+        <v>479</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -2674,93 +2447,93 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="17.81640625" customWidth="1"/>
     <col min="6" max="6" width="25.81640625" customWidth="1"/>
-    <col min="7" max="7" width="62.26953125" style="38" customWidth="1"/>
+    <col min="7" max="7" width="28" style="29" customWidth="1"/>
     <col min="8" max="8" width="18.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>392</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>412</v>
-      </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
+        <v>40</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>355</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>427</v>
-      </c>
-      <c r="H2" s="30"/>
+        <v>389</v>
+      </c>
+      <c r="H2" s="23"/>
       <c r="I2" s="16"/>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
     </row>
     <row r="3" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="6"/>
       <c r="H3" s="9" t="s">
-        <v>498</v>
+        <v>460</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
@@ -2768,178 +2541,178 @@
     </row>
     <row r="4" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>351</v>
+        <v>316</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>499</v>
+        <v>461</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>353</v>
+        <v>317</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>500</v>
+        <v>462</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>354</v>
+        <v>318</v>
       </c>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="118" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>355</v>
+        <v>319</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>524</v>
+        <v>486</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>356</v>
+        <v>320</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>525</v>
+        <v>487</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>357</v>
+        <v>321</v>
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="137.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>358</v>
+        <v>322</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>526</v>
+        <v>488</v>
       </c>
     </row>
   </sheetData>
@@ -2952,7 +2725,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2962,85 +2735,85 @@
     <col min="3" max="5" width="9.36328125" customWidth="1"/>
     <col min="6" max="6" width="25.81640625" customWidth="1"/>
     <col min="7" max="7" width="39.90625" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" style="38"/>
+    <col min="8" max="8" width="10.81640625" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="42" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>392</v>
-      </c>
-      <c r="H1" s="39" t="s">
-        <v>412</v>
-      </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
+        <v>40</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>355</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>374</v>
+      </c>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>427</v>
-      </c>
-      <c r="H2" s="36"/>
+        <v>38</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>389</v>
+      </c>
+      <c r="H2" s="27"/>
       <c r="I2" s="16"/>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F3" s="5"/>
-      <c r="G3" s="35"/>
+      <c r="G3" s="26"/>
       <c r="H3" s="9" t="s">
-        <v>519</v>
+        <v>481</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
@@ -3048,114 +2821,114 @@
     </row>
     <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>379</v>
-      </c>
-      <c r="G4" s="40" t="s">
-        <v>520</v>
+        <v>342</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>380</v>
-      </c>
-      <c r="G5" s="40" t="s">
-        <v>521</v>
+        <v>343</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>359</v>
-      </c>
-      <c r="G6" s="40" t="s">
-        <v>522</v>
+        <v>323</v>
+      </c>
+      <c r="G6" s="41" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>360</v>
-      </c>
-      <c r="G7" s="40" t="s">
-        <v>523</v>
+        <v>324</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>361</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -3165,520 +2938,260 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143561C3-5632-DF4D-A3FB-55321D75FDD5}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="18.6328125" customWidth="1"/>
     <col min="3" max="5" width="9.6328125" customWidth="1"/>
-    <col min="6" max="6" width="48.36328125" customWidth="1"/>
-    <col min="7" max="7" width="26" customWidth="1"/>
-    <col min="8" max="8" width="60.453125" customWidth="1"/>
-    <col min="9" max="13" width="26" customWidth="1"/>
-    <col min="14" max="15" width="19.453125" customWidth="1"/>
-    <col min="16" max="16" width="16.36328125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="47" customWidth="1"/>
+    <col min="8" max="8" width="19.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="43"/>
-    </row>
-    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="3" t="s">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>355</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="E2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>389</v>
+      </c>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>491</v>
+      </c>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="E6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>492</v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>461</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="E8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>462</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="P2" s="21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="87" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="L3" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="P3" s="23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="23"/>
-    </row>
-    <row r="5" spans="1:16" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="F9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="P5" s="23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="P6" s="23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>362</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="P7" s="23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>351</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="P8" s="23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>353</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="P9" s="23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>96</v>
-      </c>
       <c r="B10" s="6" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>4</v>
+        <v>494</v>
       </c>
       <c r="H10" s="6"/>
-      <c r="I10" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="P10" s="23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="58" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="P11" s="23" t="s">
-        <v>110</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F1:P1"/>
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="I5" r:id="rId1" display="StudyVersion/@studyDesigns/StudyDesign/@encounters/Encounter/@previous | @next" xr:uid="{36282C5C-665C-3D4E-9653-50792B2941FE}"/>
-    <hyperlink ref="I6" r:id="rId2" display="StudyVersion/@studyDesigns/StudyDesign/@encounters/Encounter/@previous | @next" xr:uid="{AB1C5F56-2F0F-5144-B8D5-546A5BC35C74}"/>
-    <hyperlink ref="I7" r:id="rId3" xr:uid="{D6963997-FDAE-BC4A-B4FD-4E8BFBDFABA4}"/>
-    <hyperlink ref="I10" r:id="rId4" display="StudyVersion/@studyDesigns/StudyDesign/@encounters /Encounter/@transitionEndRule" xr:uid="{4B5A0369-7BAB-B94C-9F43-BB126B7B6772}"/>
-    <hyperlink ref="I11" r:id="rId5" xr:uid="{8E6D39C8-5356-BC4E-8632-2BD160EB6C24}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3688,232 +3201,232 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K3" sqref="G1:K3"/>
+      <selection activeCell="G1" sqref="G1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="5" width="18.6328125" customWidth="1"/>
     <col min="6" max="6" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.6328125" style="37" customWidth="1"/>
+    <col min="7" max="7" width="26.6328125" style="28" customWidth="1"/>
     <col min="8" max="8" width="29.81640625" style="16" customWidth="1"/>
     <col min="9" max="11" width="8.6328125" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>392</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>412</v>
-      </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
+        <v>40</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>355</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>427</v>
-      </c>
-      <c r="H2" s="30"/>
+        <v>38</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>389</v>
+      </c>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="35"/>
+      <c r="G3" s="26"/>
       <c r="H3" s="9" t="s">
-        <v>490</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>491</v>
-      </c>
-      <c r="H4" s="30"/>
+        <v>78</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>453</v>
+      </c>
+      <c r="H4" s="23"/>
     </row>
     <row r="5" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G5" s="38" t="s">
-        <v>496</v>
-      </c>
-      <c r="H5" s="30"/>
+        <v>80</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>458</v>
+      </c>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G6" s="36" t="s">
-        <v>492</v>
-      </c>
-      <c r="H6" s="30"/>
+        <v>82</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>454</v>
+      </c>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G7" s="36" t="s">
-        <v>493</v>
-      </c>
-      <c r="H7" s="30"/>
+        <v>84</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>455</v>
+      </c>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="30"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G9" s="35" t="s">
-        <v>497</v>
-      </c>
-      <c r="H9" s="30"/>
+        <v>88</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>459</v>
+      </c>
+      <c r="H9" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3924,7 +3437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF8120D-B51B-094C-AABA-CA55EB26DD5D}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -3942,266 +3455,266 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>392</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>412</v>
-      </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
+        <v>355</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" ht="93" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>427</v>
-      </c>
-      <c r="H2" s="30"/>
+        <v>38</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>389</v>
+      </c>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F3" s="5"/>
-      <c r="G3" s="29"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="9" t="s">
-        <v>428</v>
+        <v>390</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="30"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="23"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F5" s="12"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="30"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F6" s="12"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="30"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="F7" s="12"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="30"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>134</v>
+        <v>100</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="F8" s="12"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>134</v>
+        <v>100</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F9" s="12"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="30"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>134</v>
+        <v>100</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="F10" s="12"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
     </row>
     <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>134</v>
+        <v>100</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>413</v>
-      </c>
-      <c r="H11" s="30"/>
+        <v>106</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>375</v>
+      </c>
+      <c r="H11" s="23"/>
     </row>
     <row r="12" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>141</v>
+        <v>107</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>134</v>
+        <v>100</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>381</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>414</v>
-      </c>
-      <c r="H12" s="30"/>
+        <v>344</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>376</v>
+      </c>
+      <c r="H12" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4212,19 +3725,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DEA66B-9A3B-A542-95A2-9E48A8B13E1D}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="A24" zoomScale="109" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.90625" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" customWidth="1"/>
     <col min="4" max="4" width="28.6328125" customWidth="1"/>
     <col min="5" max="5" width="33.81640625" customWidth="1"/>
-    <col min="6" max="6" width="32.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="85.54296875" customWidth="1"/>
+    <col min="6" max="6" width="32.453125" customWidth="1"/>
+    <col min="7" max="7" width="59.36328125" customWidth="1"/>
     <col min="8" max="8" width="27.7265625" customWidth="1"/>
     <col min="9" max="9" width="30.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="43.453125" customWidth="1"/>
@@ -4233,1358 +3746,1549 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>347</v>
+        <v>313</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>348</v>
+        <v>314</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>349</v>
+        <v>315</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>429</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>430</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>431</v>
-      </c>
-      <c r="J1" s="24" t="s">
-        <v>432</v>
-      </c>
-      <c r="K1" s="24" t="s">
-        <v>433</v>
+        <v>92</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>392</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>393</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>394</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="14" t="s">
-        <v>363</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>393</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>356</v>
+      </c>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
     </row>
     <row r="3" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>149</v>
+        <v>115</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="14" t="s">
-        <v>364</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>494</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>456</v>
+      </c>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
     </row>
     <row r="4" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="14" t="s">
-        <v>365</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>495</v>
-      </c>
-      <c r="H4" s="32" t="s">
-        <v>475</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>457</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>437</v>
+      </c>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
     </row>
     <row r="5" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>153</v>
+        <v>119</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>154</v>
+        <v>120</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>366</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>394</v>
-      </c>
+        <v>329</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>357</v>
+      </c>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
     </row>
     <row r="6" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>159</v>
+        <v>125</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>367</v>
-      </c>
-      <c r="G6" s="25" t="s">
-        <v>395</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>358</v>
+      </c>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
     </row>
     <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
       <c r="F7" s="14"/>
-      <c r="G7" s="25" t="s">
-        <v>426</v>
-      </c>
+      <c r="G7" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
     </row>
     <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>165</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
     </row>
     <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>169</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
     </row>
     <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>415</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>416</v>
-      </c>
+        <v>377</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>378</v>
+      </c>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
     </row>
     <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="G11" s="25" t="s">
-        <v>417</v>
-      </c>
+        <v>331</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>379</v>
+      </c>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
     </row>
     <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="G12" s="25" t="s">
-        <v>472</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>434</v>
+      </c>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
     </row>
     <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>369</v>
-      </c>
-      <c r="G13" s="25" t="s">
-        <v>423</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>385</v>
+      </c>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
     </row>
     <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>422</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="G14" s="33" t="s">
+        <v>384</v>
+      </c>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
     </row>
     <row r="15" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>190</v>
+        <v>156</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>191</v>
+        <v>157</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>192</v>
+        <v>158</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>370</v>
-      </c>
-      <c r="G15" s="25" t="s">
-        <v>425</v>
-      </c>
-      <c r="I15" s="25" t="s">
-        <v>436</v>
-      </c>
-      <c r="J15" s="25" t="s">
-        <v>437</v>
-      </c>
-      <c r="K15" s="25" t="s">
-        <v>438</v>
+        <v>333</v>
+      </c>
+      <c r="G15" s="33" t="s">
+        <v>387</v>
+      </c>
+      <c r="H15" s="32"/>
+      <c r="I15" s="33" t="s">
+        <v>398</v>
+      </c>
+      <c r="J15" s="33" t="s">
+        <v>399</v>
+      </c>
+      <c r="K15" s="33" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>194</v>
+        <v>160</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>195</v>
+        <v>161</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="G16" s="25" t="s">
-        <v>424</v>
-      </c>
-      <c r="I16" s="25" t="s">
-        <v>439</v>
-      </c>
-      <c r="J16" s="25" t="s">
-        <v>440</v>
-      </c>
-      <c r="K16" s="25" t="s">
-        <v>441</v>
+        <v>334</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>386</v>
+      </c>
+      <c r="H16" s="32"/>
+      <c r="I16" s="33" t="s">
+        <v>401</v>
+      </c>
+      <c r="J16" s="33" t="s">
+        <v>402</v>
+      </c>
+      <c r="K16" s="33" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="G17" s="33" t="s">
-        <v>474</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>436</v>
+      </c>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
     </row>
     <row r="18" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>201</v>
+        <v>167</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="14" t="s">
-        <v>199</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
     </row>
     <row r="19" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
-        <v>202</v>
+        <v>168</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>203</v>
+        <v>169</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>204</v>
+        <v>170</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="14" t="s">
-        <v>477</v>
-      </c>
-      <c r="G19" s="25" t="s">
-        <v>476</v>
-      </c>
+        <v>439</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>438</v>
+      </c>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
     </row>
     <row r="20" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
-        <v>205</v>
+        <v>171</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="14" t="s">
-        <v>372</v>
-      </c>
-      <c r="G20" s="25" t="s">
-        <v>509</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>471</v>
+      </c>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
     </row>
     <row r="21" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
-        <v>208</v>
+        <v>174</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>210</v>
+        <v>176</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="G21" s="26" t="s">
-        <v>398</v>
-      </c>
-      <c r="I21" s="26" t="s">
-        <v>442</v>
-      </c>
-      <c r="J21" s="26" t="s">
-        <v>443</v>
-      </c>
-      <c r="K21" s="26" t="s">
-        <v>444</v>
+        <v>174</v>
+      </c>
+      <c r="G21" s="36" t="s">
+        <v>361</v>
+      </c>
+      <c r="H21" s="32"/>
+      <c r="I21" s="36" t="s">
+        <v>404</v>
+      </c>
+      <c r="J21" s="36" t="s">
+        <v>405</v>
+      </c>
+      <c r="K21" s="36" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
-        <v>211</v>
+        <v>177</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>212</v>
+        <v>178</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>213</v>
+        <v>179</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="G22" s="25" t="s">
-        <v>419</v>
-      </c>
-      <c r="I22" s="25" t="s">
-        <v>445</v>
-      </c>
-      <c r="J22" s="25" t="s">
-        <v>446</v>
-      </c>
-      <c r="K22" s="25" t="s">
-        <v>447</v>
+        <v>177</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>381</v>
+      </c>
+      <c r="H22" s="32"/>
+      <c r="I22" s="33" t="s">
+        <v>407</v>
+      </c>
+      <c r="J22" s="33" t="s">
+        <v>408</v>
+      </c>
+      <c r="K22" s="33" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
-        <v>214</v>
+        <v>180</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>215</v>
+        <v>181</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>216</v>
+        <v>182</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="13" t="s">
-        <v>389</v>
-      </c>
-      <c r="G23" s="25" t="s">
-        <v>448</v>
-      </c>
-      <c r="H23" t="s">
-        <v>434</v>
-      </c>
+        <v>352</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>410</v>
+      </c>
+      <c r="H23" s="32" t="s">
+        <v>396</v>
+      </c>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
     </row>
     <row r="24" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
-        <v>217</v>
+        <v>183</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>218</v>
+        <v>184</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>219</v>
+        <v>185</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="14" t="s">
-        <v>373</v>
-      </c>
+        <v>336</v>
+      </c>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
     </row>
     <row r="25" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
-        <v>220</v>
+        <v>186</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>221</v>
+        <v>187</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>222</v>
+        <v>188</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
       <c r="F25" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="G25" s="25" t="s">
-        <v>399</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="G25" s="42" t="s">
+        <v>489</v>
+      </c>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
     </row>
     <row r="26" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
-        <v>224</v>
+        <v>190</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>226</v>
+        <v>192</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
       <c r="F26" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="G26" s="26" t="s">
-        <v>449</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="G26" s="36" t="s">
+        <v>411</v>
+      </c>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
     </row>
     <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
-        <v>227</v>
+        <v>193</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>228</v>
+        <v>194</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>229</v>
+        <v>195</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
       <c r="F27" s="14" t="s">
-        <v>227</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
     </row>
     <row r="28" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
-        <v>230</v>
+        <v>196</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>231</v>
+        <v>197</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>232</v>
+        <v>198</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>234</v>
+        <v>200</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>235</v>
+        <v>201</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="G28" s="25" t="s">
-        <v>408</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="G28" s="33" t="s">
+        <v>370</v>
+      </c>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
     </row>
     <row r="29" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
-        <v>236</v>
+        <v>202</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>238</v>
+        <v>204</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>234</v>
+        <v>200</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>235</v>
+        <v>201</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="G29" s="25" t="s">
-        <v>406</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>368</v>
+      </c>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
     </row>
     <row r="30" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
-        <v>240</v>
+        <v>206</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>241</v>
+        <v>207</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>242</v>
+        <v>208</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>234</v>
+        <v>200</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>235</v>
+        <v>201</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="G30" s="25" t="s">
-        <v>407</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="G30" s="33" t="s">
+        <v>369</v>
+      </c>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
     </row>
     <row r="31" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>245</v>
+        <v>211</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>246</v>
+        <v>212</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
       <c r="F31" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="G31" s="28" t="s">
-        <v>402</v>
-      </c>
-      <c r="I31" s="28" t="s">
-        <v>450</v>
-      </c>
-      <c r="J31" s="28" t="s">
-        <v>451</v>
-      </c>
-      <c r="K31" s="28" t="s">
-        <v>452</v>
+        <v>210</v>
+      </c>
+      <c r="G31" s="32" t="s">
+        <v>364</v>
+      </c>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32" t="s">
+        <v>412</v>
+      </c>
+      <c r="J31" s="32" t="s">
+        <v>413</v>
+      </c>
+      <c r="K31" s="32" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
-        <v>247</v>
+        <v>213</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>248</v>
+        <v>214</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>249</v>
+        <v>215</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
       <c r="F32" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="G32" s="26" t="s">
-        <v>403</v>
-      </c>
-      <c r="I32" s="26" t="s">
-        <v>453</v>
-      </c>
-      <c r="J32" s="26" t="s">
-        <v>454</v>
-      </c>
-      <c r="K32" s="26" t="s">
-        <v>455</v>
+        <v>213</v>
+      </c>
+      <c r="G32" s="36" t="s">
+        <v>365</v>
+      </c>
+      <c r="H32" s="32"/>
+      <c r="I32" s="36" t="s">
+        <v>415</v>
+      </c>
+      <c r="J32" s="36" t="s">
+        <v>416</v>
+      </c>
+      <c r="K32" s="36" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
-        <v>250</v>
+        <v>216</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>252</v>
+        <v>218</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
       <c r="F33" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="G33" s="26" t="s">
-        <v>404</v>
-      </c>
+        <v>337</v>
+      </c>
+      <c r="G33" s="36" t="s">
+        <v>366</v>
+      </c>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
     </row>
     <row r="34" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
-        <v>253</v>
+        <v>219</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>254</v>
+        <v>220</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>255</v>
+        <v>221</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
       <c r="F34" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="G34" s="26" t="s">
-        <v>405</v>
-      </c>
-      <c r="I34" s="26" t="s">
-        <v>456</v>
-      </c>
-      <c r="J34" s="26" t="s">
-        <v>457</v>
-      </c>
-      <c r="K34" s="26" t="s">
-        <v>458</v>
+        <v>219</v>
+      </c>
+      <c r="G34" s="36" t="s">
+        <v>367</v>
+      </c>
+      <c r="H34" s="32"/>
+      <c r="I34" s="36" t="s">
+        <v>418</v>
+      </c>
+      <c r="J34" s="36" t="s">
+        <v>419</v>
+      </c>
+      <c r="K34" s="36" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="15" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>259</v>
+        <v>225</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>260</v>
+        <v>226</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="G35" s="25" t="s">
-        <v>411</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>373</v>
+      </c>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="32"/>
     </row>
     <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="15" t="s">
-        <v>261</v>
+        <v>227</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>262</v>
+        <v>228</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>263</v>
+        <v>229</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>259</v>
+        <v>225</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>260</v>
+        <v>226</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="G36" s="25" t="s">
-        <v>409</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="G36" s="33" t="s">
+        <v>371</v>
+      </c>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="32"/>
     </row>
     <row r="37" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
-        <v>264</v>
+        <v>230</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>265</v>
+        <v>231</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>266</v>
+        <v>232</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>259</v>
+        <v>225</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>260</v>
+        <v>226</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="G37" s="25" t="s">
-        <v>410</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="G37" s="33" t="s">
+        <v>372</v>
+      </c>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="32"/>
     </row>
     <row r="38" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="15" t="s">
-        <v>267</v>
+        <v>233</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>268</v>
+        <v>234</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>269</v>
+        <v>235</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="15" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="G38" s="25" t="s">
-        <v>478</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="G38" s="33" t="s">
+        <v>440</v>
+      </c>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="32"/>
+      <c r="K38" s="32"/>
     </row>
     <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="15" t="s">
-        <v>270</v>
+        <v>236</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>271</v>
+        <v>237</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>272</v>
+        <v>238</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="20"/>
       <c r="F39" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="G39" s="25" t="s">
-        <v>479</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="G39" s="33" t="s">
+        <v>441</v>
+      </c>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="32"/>
     </row>
     <row r="40" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A40" s="15" t="s">
-        <v>273</v>
+        <v>239</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>274</v>
+        <v>240</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>275</v>
+        <v>241</v>
       </c>
       <c r="D40" s="20"/>
       <c r="E40" s="20"/>
       <c r="F40" s="14" t="s">
-        <v>375</v>
-      </c>
-      <c r="G40" s="25" t="s">
-        <v>401</v>
-      </c>
-      <c r="H40" t="s">
-        <v>434</v>
-      </c>
+        <v>338</v>
+      </c>
+      <c r="G40" s="33" t="s">
+        <v>363</v>
+      </c>
+      <c r="H40" s="32" t="s">
+        <v>396</v>
+      </c>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="32"/>
     </row>
     <row r="41" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="15" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>278</v>
+        <v>244</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="20" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>376</v>
-      </c>
-      <c r="G41" s="26" t="s">
-        <v>420</v>
-      </c>
-      <c r="H41" t="s">
-        <v>434</v>
-      </c>
+        <v>339</v>
+      </c>
+      <c r="G41" s="36" t="s">
+        <v>382</v>
+      </c>
+      <c r="H41" s="32" t="s">
+        <v>396</v>
+      </c>
+      <c r="I41" s="32"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="32"/>
     </row>
     <row r="42" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="15" t="s">
-        <v>279</v>
+        <v>245</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>280</v>
+        <v>246</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>281</v>
+        <v>247</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="20"/>
       <c r="F42" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="G42" s="25" t="s">
-        <v>480</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="G42" s="33" t="s">
+        <v>442</v>
+      </c>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="32"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
-        <v>283</v>
+        <v>249</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>284</v>
+        <v>250</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>285</v>
+        <v>251</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="20"/>
       <c r="F43" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="G43" s="26" t="s">
-        <v>481</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="G43" s="36" t="s">
+        <v>443</v>
+      </c>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="32"/>
     </row>
     <row r="44" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="15" t="s">
-        <v>287</v>
+        <v>253</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>288</v>
+        <v>254</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>289</v>
+        <v>255</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>290</v>
+        <v>256</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>287</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
+      <c r="J44" s="32"/>
+      <c r="K44" s="32"/>
     </row>
     <row r="45" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A45" s="15" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>294</v>
+        <v>260</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>292</v>
-      </c>
-      <c r="G45" s="25" t="s">
-        <v>468</v>
-      </c>
-      <c r="I45" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="J45" s="25" t="s">
-        <v>470</v>
-      </c>
-      <c r="K45" s="25" t="s">
-        <v>471</v>
+        <v>258</v>
+      </c>
+      <c r="G45" s="33" t="s">
+        <v>430</v>
+      </c>
+      <c r="H45" s="32"/>
+      <c r="I45" s="33" t="s">
+        <v>431</v>
+      </c>
+      <c r="J45" s="33" t="s">
+        <v>432</v>
+      </c>
+      <c r="K45" s="33" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A46" s="15" t="s">
-        <v>295</v>
+        <v>261</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>296</v>
+        <v>262</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>297</v>
+        <v>263</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>298</v>
+        <v>264</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>295</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
+      <c r="K46" s="32"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="15" t="s">
-        <v>299</v>
+        <v>265</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>300</v>
+        <v>266</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>301</v>
+        <v>267</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
       <c r="F47" s="14" t="s">
-        <v>299</v>
-      </c>
+        <v>265</v>
+      </c>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="32"/>
+      <c r="J47" s="32"/>
+      <c r="K47" s="32"/>
     </row>
     <row r="48" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="15" t="s">
-        <v>302</v>
+        <v>268</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>303</v>
+        <v>269</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>304</v>
+        <v>270</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="20"/>
       <c r="F48" s="19" t="s">
-        <v>377</v>
-      </c>
-      <c r="G48" s="25" t="s">
-        <v>473</v>
-      </c>
+        <v>340</v>
+      </c>
+      <c r="G48" s="33" t="s">
+        <v>435</v>
+      </c>
+      <c r="H48" s="32"/>
+      <c r="I48" s="32"/>
+      <c r="J48" s="32"/>
+      <c r="K48" s="32"/>
     </row>
     <row r="49" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="15" t="s">
-        <v>305</v>
+        <v>271</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>306</v>
+        <v>272</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>307</v>
+        <v>273</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>290</v>
+        <v>256</v>
       </c>
       <c r="E49" s="20"/>
       <c r="F49" s="14" t="s">
-        <v>305</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="32"/>
+      <c r="K49" s="32"/>
     </row>
     <row r="50" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="15" t="s">
-        <v>308</v>
+        <v>274</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>309</v>
+        <v>275</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>310</v>
+        <v>276</v>
       </c>
       <c r="D50" s="20"/>
       <c r="E50" s="20"/>
       <c r="F50" s="14" t="s">
-        <v>378</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="32"/>
+      <c r="J50" s="32"/>
+      <c r="K50" s="32"/>
     </row>
     <row r="51" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="15" t="s">
-        <v>311</v>
+        <v>277</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>312</v>
+        <v>278</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>313</v>
+        <v>279</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="20"/>
       <c r="F51" s="14" t="s">
-        <v>314</v>
-      </c>
-      <c r="G51" s="28" t="s">
-        <v>482</v>
-      </c>
-      <c r="I51" s="28" t="s">
-        <v>483</v>
-      </c>
-      <c r="J51" s="28" t="s">
-        <v>484</v>
-      </c>
-      <c r="K51" s="28" t="s">
-        <v>485</v>
+        <v>280</v>
+      </c>
+      <c r="G51" s="32" t="s">
+        <v>444</v>
+      </c>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32" t="s">
+        <v>445</v>
+      </c>
+      <c r="J51" s="32" t="s">
+        <v>446</v>
+      </c>
+      <c r="K51" s="32" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A52" s="15" t="s">
-        <v>315</v>
+        <v>281</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>316</v>
+        <v>282</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>317</v>
+        <v>283</v>
       </c>
       <c r="D52" s="20"/>
       <c r="E52" s="20"/>
       <c r="F52" s="14" t="s">
-        <v>318</v>
-      </c>
-      <c r="G52" s="25" t="s">
-        <v>400</v>
-      </c>
-      <c r="I52" s="25" t="s">
-        <v>459</v>
-      </c>
-      <c r="J52" s="25" t="s">
-        <v>460</v>
-      </c>
-      <c r="K52" s="25" t="s">
-        <v>461</v>
+        <v>284</v>
+      </c>
+      <c r="G52" s="33" t="s">
+        <v>362</v>
+      </c>
+      <c r="H52" s="32"/>
+      <c r="I52" s="33" t="s">
+        <v>421</v>
+      </c>
+      <c r="J52" s="33" t="s">
+        <v>422</v>
+      </c>
+      <c r="K52" s="33" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A53" s="15" t="s">
-        <v>319</v>
+        <v>285</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>320</v>
+        <v>286</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>321</v>
+        <v>287</v>
       </c>
       <c r="D53" s="15"/>
       <c r="E53" s="15"/>
       <c r="F53" s="14" t="s">
-        <v>322</v>
-      </c>
-      <c r="G53" s="26" t="s">
-        <v>421</v>
-      </c>
-      <c r="I53" s="26" t="s">
-        <v>462</v>
-      </c>
-      <c r="J53" s="26" t="s">
-        <v>463</v>
-      </c>
-      <c r="K53" s="26" t="s">
-        <v>464</v>
+        <v>288</v>
+      </c>
+      <c r="G53" s="36" t="s">
+        <v>383</v>
+      </c>
+      <c r="H53" s="32"/>
+      <c r="I53" s="36" t="s">
+        <v>424</v>
+      </c>
+      <c r="J53" s="36" t="s">
+        <v>425</v>
+      </c>
+      <c r="K53" s="36" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="15" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>324</v>
+        <v>290</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>325</v>
+        <v>291</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="15"/>
       <c r="F54" s="14" t="s">
-        <v>323</v>
-      </c>
-      <c r="G54" s="25" t="s">
-        <v>486</v>
-      </c>
-      <c r="I54" s="25" t="s">
-        <v>487</v>
-      </c>
-      <c r="J54" s="25" t="s">
-        <v>488</v>
-      </c>
-      <c r="K54" s="25" t="s">
-        <v>489</v>
+        <v>289</v>
+      </c>
+      <c r="G54" s="33" t="s">
+        <v>448</v>
+      </c>
+      <c r="H54" s="32"/>
+      <c r="I54" s="33" t="s">
+        <v>449</v>
+      </c>
+      <c r="J54" s="33" t="s">
+        <v>450</v>
+      </c>
+      <c r="K54" s="33" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="15" t="s">
-        <v>326</v>
+        <v>292</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>327</v>
+        <v>293</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>328</v>
+        <v>294</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>330</v>
+        <v>296</v>
       </c>
       <c r="E55" s="15"/>
       <c r="F55" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="G55" s="25" t="s">
-        <v>501</v>
-      </c>
-      <c r="I55" s="25" t="s">
-        <v>503</v>
-      </c>
-      <c r="J55" s="25" t="s">
-        <v>504</v>
-      </c>
-      <c r="K55" s="25" t="s">
-        <v>505</v>
+        <v>295</v>
+      </c>
+      <c r="G55" s="33" t="s">
+        <v>463</v>
+      </c>
+      <c r="H55" s="32"/>
+      <c r="I55" s="33" t="s">
+        <v>465</v>
+      </c>
+      <c r="J55" s="33" t="s">
+        <v>466</v>
+      </c>
+      <c r="K55" s="33" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="15" t="s">
-        <v>331</v>
+        <v>297</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>332</v>
+        <v>298</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>333</v>
+        <v>299</v>
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="15"/>
       <c r="F56" s="14" t="s">
-        <v>334</v>
-      </c>
-      <c r="G56" s="25" t="s">
+        <v>300</v>
+      </c>
+      <c r="G56" s="33" t="s">
+        <v>359</v>
+      </c>
+      <c r="H56" s="32"/>
+      <c r="I56" s="32"/>
+      <c r="J56" s="32"/>
+      <c r="K56" s="32"/>
+    </row>
+    <row r="57" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A57" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="B57" s="37" t="s">
+        <v>302</v>
+      </c>
+      <c r="C57" s="37" t="s">
+        <v>303</v>
+      </c>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="38" t="s">
+        <v>304</v>
+      </c>
+      <c r="G57" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="H57" s="34" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="15" t="s">
-        <v>335</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>336</v>
-      </c>
-      <c r="C57" s="15" t="s">
-        <v>337</v>
-      </c>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="14" t="s">
-        <v>338</v>
-      </c>
-      <c r="G57" s="28" t="s">
+      <c r="I57" s="32" t="s">
+        <v>427</v>
+      </c>
+      <c r="J57" s="32" t="s">
+        <v>428</v>
+      </c>
+      <c r="K57" s="32" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="G58" s="41" t="s">
+        <v>380</v>
+      </c>
+      <c r="H58" s="34" t="s">
         <v>397</v>
       </c>
-      <c r="H57" s="32" t="s">
-        <v>434</v>
-      </c>
-      <c r="I57" s="28" t="s">
-        <v>465</v>
-      </c>
-      <c r="J57" s="28" t="s">
-        <v>466</v>
-      </c>
-      <c r="K57" s="28" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="15" t="s">
-        <v>339</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>340</v>
-      </c>
-      <c r="C58" s="15" t="s">
-        <v>341</v>
-      </c>
-      <c r="D58" s="15" t="s">
-        <v>330</v>
-      </c>
-      <c r="E58" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="F58" s="14" t="s">
-        <v>342</v>
-      </c>
-      <c r="G58" s="25" t="s">
-        <v>418</v>
-      </c>
-      <c r="H58" s="32" t="s">
-        <v>435</v>
-      </c>
+      <c r="I58" s="32"/>
+      <c r="J58" s="32"/>
+      <c r="K58" s="32"/>
     </row>
     <row r="59" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="B59" s="15" t="s">
-        <v>344</v>
-      </c>
-      <c r="C59" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="G59" s="25" t="s">
-        <v>502</v>
-      </c>
-      <c r="I59" s="25" t="s">
-        <v>506</v>
-      </c>
-      <c r="J59" s="25" t="s">
-        <v>507</v>
-      </c>
-      <c r="K59" s="25" t="s">
-        <v>508</v>
+      <c r="A59" s="39" t="s">
+        <v>309</v>
+      </c>
+      <c r="B59" s="39" t="s">
+        <v>310</v>
+      </c>
+      <c r="C59" s="39" t="s">
+        <v>311</v>
+      </c>
+      <c r="D59" s="39"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="40" t="s">
+        <v>312</v>
+      </c>
+      <c r="G59" s="33" t="s">
+        <v>464</v>
+      </c>
+      <c r="H59" s="32"/>
+      <c r="I59" s="33" t="s">
+        <v>468</v>
+      </c>
+      <c r="J59" s="33" t="s">
+        <v>469</v>
+      </c>
+      <c r="K59" s="33" t="s">
+        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted TA mapping for better processing
</commit_message>
<xml_diff>
--- a/Maps/sdtm_mapping_paths.xlsx
+++ b/Maps/sdtm_mapping_paths.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\SDTM_mapper\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE15098-C11F-4849-B0D7-8E3E1A74B54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352201F3-0064-4BF4-A66C-E399969A2CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20895" yWindow="-17145" windowWidth="39225" windowHeight="15225" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19890" yWindow="-18810" windowWidth="25080" windowHeight="15225" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -1647,15 +1647,6 @@
     <t>study.versions.studyDesigns.elements.{id: transitionEndRule.text}</t>
   </si>
   <si>
-    <t>study.versions.studyDesigns.($ElementName := function($id) {(elements[id=$id].label)}; studyCells.{armId: armId, elementIds[0]:$ElementName(elementIds[0])})</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.($ElementName := function($id) {(elements[id=$id].description)}; studyCells.{armId: armId, elementIds[0]:$ElementName(elementIds[0])})</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.($EpochName := function($id) {(epochs[id=$id].label)}; studyCells.{armId: armId, elementIds[0]: $EpochName(epochId)})</t>
-  </si>
-  <si>
     <t>$count(study.versions.studyDesigns.arms)</t>
   </si>
   <si>
@@ -1672,6 +1663,15 @@
   </si>
   <si>
     <t>study.versions.studyDesigns.encounters.transitionStartRule.text</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.($ElementName := function($id) {(elements[id=$id].label)}; studyCells.{armId: elementIds[0], elementIds[0]:$ElementName(elementIds[0])})</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.($ElementName := function($id) {(elements[id=$id].description)}; studyCells.{armId: elementIds[0], elementIds[0]:$ElementName(elementIds[0])})</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.($EpochName := function($id) {(epochs[id=$id].label)}; studyCells.{armId: elementIds[0], elementIds[0]: $EpochName(epochId)})</t>
   </si>
 </sst>
 </file>
@@ -1895,7 +1895,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1983,20 +1983,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2011,10 +2007,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2446,7 +2439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CEFEB0-0887-1349-82EC-A63800D98F30}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="87" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -2487,7 +2480,7 @@
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -2626,10 +2619,10 @@
         <v>319</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>27</v>
       </c>
@@ -2649,7 +2642,7 @@
         <v>320</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
@@ -2712,7 +2705,7 @@
         <v>322</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
     </row>
   </sheetData>
@@ -2838,7 +2831,7 @@
       <c r="F4" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="13" t="s">
         <v>482</v>
       </c>
     </row>
@@ -2861,7 +2854,7 @@
       <c r="F5" s="12" t="s">
         <v>343</v>
       </c>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="13" t="s">
         <v>483</v>
       </c>
     </row>
@@ -2884,7 +2877,7 @@
       <c r="F6" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="13" t="s">
         <v>484</v>
       </c>
     </row>
@@ -2907,7 +2900,7 @@
       <c r="F7" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="G7" s="13" t="s">
         <v>485</v>
       </c>
     </row>
@@ -3022,7 +3015,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -3067,7 +3060,7 @@
         <v>64</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="H5" s="6"/>
     </row>
@@ -3091,7 +3084,7 @@
         <v>66</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -3114,7 +3107,7 @@
       <c r="F7" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="G7" s="13" t="s">
         <v>461</v>
       </c>
       <c r="H7" s="6"/>
@@ -3138,7 +3131,7 @@
       <c r="F8" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="G8" s="33" t="s">
+      <c r="G8" s="29" t="s">
         <v>462</v>
       </c>
       <c r="H8" s="6"/>
@@ -3163,7 +3156,7 @@
         <v>72</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="H9" s="6"/>
     </row>
@@ -3187,7 +3180,7 @@
         <v>74</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="H10" s="6"/>
     </row>
@@ -3797,10 +3790,6 @@
       <c r="G2" s="31" t="s">
         <v>356</v>
       </c>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
     </row>
     <row r="3" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
@@ -3817,13 +3806,9 @@
       <c r="F3" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="29" t="s">
         <v>456</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
     </row>
     <row r="4" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
@@ -3840,15 +3825,12 @@
       <c r="F4" s="14" t="s">
         <v>328</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="29" t="s">
         <v>457</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="32" t="s">
         <v>437</v>
       </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
     </row>
     <row r="5" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
@@ -3869,13 +3851,9 @@
       <c r="F5" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="29" t="s">
         <v>357</v>
       </c>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
     </row>
     <row r="6" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
@@ -3896,13 +3874,9 @@
       <c r="F6" s="14" t="s">
         <v>330</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="G6" s="29" t="s">
         <v>358</v>
       </c>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
     </row>
     <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
@@ -3921,13 +3895,9 @@
         <v>130</v>
       </c>
       <c r="F7" s="14"/>
-      <c r="G7" s="33" t="s">
+      <c r="G7" s="29" t="s">
         <v>388</v>
       </c>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
     </row>
     <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
@@ -3948,11 +3918,6 @@
       <c r="F8" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
     </row>
     <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
@@ -3973,11 +3938,6 @@
       <c r="F9" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
     </row>
     <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
@@ -3998,13 +3958,9 @@
       <c r="F10" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="G10" s="33" t="s">
+      <c r="G10" s="29" t="s">
         <v>378</v>
       </c>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
     </row>
     <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
@@ -4025,13 +3981,9 @@
       <c r="F11" s="14" t="s">
         <v>331</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="G11" s="29" t="s">
         <v>379</v>
       </c>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
     </row>
     <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
@@ -4048,13 +4000,9 @@
       <c r="F12" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="G12" s="33" t="s">
+      <c r="G12" s="29" t="s">
         <v>434</v>
       </c>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
     </row>
     <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
@@ -4075,13 +4023,9 @@
       <c r="F13" s="14" t="s">
         <v>332</v>
       </c>
-      <c r="G13" s="33" t="s">
+      <c r="G13" s="29" t="s">
         <v>385</v>
       </c>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
     </row>
     <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
@@ -4102,13 +4046,9 @@
       <c r="F14" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="29" t="s">
         <v>384</v>
       </c>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
     </row>
     <row r="15" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
@@ -4129,17 +4069,16 @@
       <c r="F15" s="14" t="s">
         <v>333</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="29" t="s">
         <v>387</v>
       </c>
-      <c r="H15" s="32"/>
-      <c r="I15" s="33" t="s">
+      <c r="I15" s="29" t="s">
         <v>398</v>
       </c>
-      <c r="J15" s="33" t="s">
+      <c r="J15" s="29" t="s">
         <v>399</v>
       </c>
-      <c r="K15" s="33" t="s">
+      <c r="K15" s="29" t="s">
         <v>400</v>
       </c>
     </row>
@@ -4162,17 +4101,16 @@
       <c r="F16" s="14" t="s">
         <v>334</v>
       </c>
-      <c r="G16" s="33" t="s">
+      <c r="G16" s="29" t="s">
         <v>386</v>
       </c>
-      <c r="H16" s="32"/>
-      <c r="I16" s="33" t="s">
+      <c r="I16" s="29" t="s">
         <v>401</v>
       </c>
-      <c r="J16" s="33" t="s">
+      <c r="J16" s="29" t="s">
         <v>402</v>
       </c>
-      <c r="K16" s="33" t="s">
+      <c r="K16" s="29" t="s">
         <v>403</v>
       </c>
     </row>
@@ -4191,13 +4129,9 @@
       <c r="F17" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="G17" s="35" t="s">
+      <c r="G17" s="33" t="s">
         <v>436</v>
       </c>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
     </row>
     <row r="18" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
@@ -4216,11 +4150,6 @@
       <c r="F18" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
     </row>
     <row r="19" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
@@ -4237,13 +4166,9 @@
       <c r="F19" s="14" t="s">
         <v>439</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="G19" s="29" t="s">
         <v>438</v>
       </c>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
     </row>
     <row r="20" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
@@ -4260,13 +4185,9 @@
       <c r="F20" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="G20" s="29" t="s">
         <v>471</v>
       </c>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
     </row>
     <row r="21" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
@@ -4283,17 +4204,16 @@
       <c r="F21" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="G21" s="36" t="s">
+      <c r="G21" s="34" t="s">
         <v>361</v>
       </c>
-      <c r="H21" s="32"/>
-      <c r="I21" s="36" t="s">
+      <c r="I21" s="34" t="s">
         <v>404</v>
       </c>
-      <c r="J21" s="36" t="s">
+      <c r="J21" s="34" t="s">
         <v>405</v>
       </c>
-      <c r="K21" s="36" t="s">
+      <c r="K21" s="34" t="s">
         <v>406</v>
       </c>
     </row>
@@ -4316,17 +4236,16 @@
       <c r="F22" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="G22" s="33" t="s">
+      <c r="G22" s="29" t="s">
         <v>381</v>
       </c>
-      <c r="H22" s="32"/>
-      <c r="I22" s="33" t="s">
+      <c r="I22" s="29" t="s">
         <v>407</v>
       </c>
-      <c r="J22" s="33" t="s">
+      <c r="J22" s="29" t="s">
         <v>408</v>
       </c>
-      <c r="K22" s="33" t="s">
+      <c r="K22" s="29" t="s">
         <v>409</v>
       </c>
     </row>
@@ -4345,15 +4264,12 @@
       <c r="F23" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="G23" s="33" t="s">
+      <c r="G23" s="29" t="s">
         <v>410</v>
       </c>
-      <c r="H23" s="32" t="s">
+      <c r="H23" t="s">
         <v>396</v>
       </c>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
     </row>
     <row r="24" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
@@ -4370,11 +4286,6 @@
       <c r="F24" s="14" t="s">
         <v>336</v>
       </c>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
     </row>
     <row r="25" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
@@ -4391,13 +4302,9 @@
       <c r="F25" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="G25" s="42" t="s">
-        <v>489</v>
-      </c>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
+      <c r="G25" s="39" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
@@ -4414,13 +4321,9 @@
       <c r="F26" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="G26" s="36" t="s">
+      <c r="G26" s="34" t="s">
         <v>411</v>
       </c>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
     </row>
     <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
@@ -4437,11 +4340,6 @@
       <c r="F27" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
     </row>
     <row r="28" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
@@ -4462,13 +4360,9 @@
       <c r="F28" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="G28" s="33" t="s">
+      <c r="G28" s="29" t="s">
         <v>370</v>
       </c>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="32"/>
     </row>
     <row r="29" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
@@ -4489,13 +4383,9 @@
       <c r="F29" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="G29" s="33" t="s">
+      <c r="G29" s="29" t="s">
         <v>368</v>
       </c>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
     </row>
     <row r="30" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
@@ -4516,13 +4406,9 @@
       <c r="F30" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="G30" s="33" t="s">
+      <c r="G30" s="29" t="s">
         <v>369</v>
       </c>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
     </row>
     <row r="31" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
@@ -4539,17 +4425,16 @@
       <c r="F31" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="G31" s="32" t="s">
+      <c r="G31" t="s">
         <v>364</v>
       </c>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32" t="s">
+      <c r="I31" t="s">
         <v>412</v>
       </c>
-      <c r="J31" s="32" t="s">
+      <c r="J31" t="s">
         <v>413</v>
       </c>
-      <c r="K31" s="32" t="s">
+      <c r="K31" t="s">
         <v>414</v>
       </c>
     </row>
@@ -4568,17 +4453,16 @@
       <c r="F32" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="G32" s="36" t="s">
+      <c r="G32" s="34" t="s">
         <v>365</v>
       </c>
-      <c r="H32" s="32"/>
-      <c r="I32" s="36" t="s">
+      <c r="I32" s="34" t="s">
         <v>415</v>
       </c>
-      <c r="J32" s="36" t="s">
+      <c r="J32" s="34" t="s">
         <v>416</v>
       </c>
-      <c r="K32" s="36" t="s">
+      <c r="K32" s="34" t="s">
         <v>417</v>
       </c>
     </row>
@@ -4597,13 +4481,9 @@
       <c r="F33" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="G33" s="36" t="s">
+      <c r="G33" s="34" t="s">
         <v>366</v>
       </c>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
     </row>
     <row r="34" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
@@ -4620,17 +4500,16 @@
       <c r="F34" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="G34" s="36" t="s">
+      <c r="G34" s="34" t="s">
         <v>367</v>
       </c>
-      <c r="H34" s="32"/>
-      <c r="I34" s="36" t="s">
+      <c r="I34" s="34" t="s">
         <v>418</v>
       </c>
-      <c r="J34" s="36" t="s">
+      <c r="J34" s="34" t="s">
         <v>419</v>
       </c>
-      <c r="K34" s="36" t="s">
+      <c r="K34" s="34" t="s">
         <v>420</v>
       </c>
     </row>
@@ -4653,13 +4532,9 @@
       <c r="F35" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="G35" s="33" t="s">
+      <c r="G35" s="29" t="s">
         <v>373</v>
       </c>
-      <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
     </row>
     <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="15" t="s">
@@ -4680,13 +4555,9 @@
       <c r="F36" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="G36" s="33" t="s">
+      <c r="G36" s="29" t="s">
         <v>371</v>
       </c>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
     </row>
     <row r="37" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
@@ -4707,13 +4578,9 @@
       <c r="F37" s="14" t="s">
         <v>230</v>
       </c>
-      <c r="G37" s="33" t="s">
+      <c r="G37" s="29" t="s">
         <v>372</v>
       </c>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
     </row>
     <row r="38" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="15" t="s">
@@ -4732,15 +4599,11 @@
       <c r="F38" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="G38" s="33" t="s">
+      <c r="G38" s="29" t="s">
         <v>440</v>
       </c>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-    </row>
-    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="15" t="s">
         <v>236</v>
       </c>
@@ -4755,15 +4618,11 @@
       <c r="F39" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="G39" s="33" t="s">
+      <c r="G39" s="29" t="s">
         <v>441</v>
       </c>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
-    </row>
-    <row r="40" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:11" ht="116" x14ac:dyDescent="0.35">
       <c r="A40" s="15" t="s">
         <v>239</v>
       </c>
@@ -4778,15 +4637,12 @@
       <c r="F40" s="14" t="s">
         <v>338</v>
       </c>
-      <c r="G40" s="33" t="s">
+      <c r="G40" s="29" t="s">
         <v>363</v>
       </c>
-      <c r="H40" s="32" t="s">
+      <c r="H40" t="s">
         <v>396</v>
       </c>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
     </row>
     <row r="41" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="15" t="s">
@@ -4805,17 +4661,14 @@
       <c r="F41" s="14" t="s">
         <v>339</v>
       </c>
-      <c r="G41" s="36" t="s">
+      <c r="G41" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="H41" s="32" t="s">
+      <c r="H41" t="s">
         <v>396</v>
       </c>
-      <c r="I41" s="32"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
-    </row>
-    <row r="42" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A42" s="15" t="s">
         <v>245</v>
       </c>
@@ -4830,15 +4683,11 @@
       <c r="F42" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="G42" s="33" t="s">
+      <c r="G42" s="29" t="s">
         <v>442</v>
       </c>
-      <c r="H42" s="32"/>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
-      <c r="K42" s="32"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
         <v>249</v>
       </c>
@@ -4853,13 +4702,9 @@
       <c r="F43" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="G43" s="36" t="s">
+      <c r="G43" s="34" t="s">
         <v>443</v>
       </c>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="32"/>
     </row>
     <row r="44" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="15" t="s">
@@ -4880,11 +4725,6 @@
       <c r="F44" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="G44" s="32"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="32"/>
-      <c r="K44" s="32"/>
     </row>
     <row r="45" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A45" s="15" t="s">
@@ -4905,17 +4745,16 @@
       <c r="F45" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="G45" s="33" t="s">
+      <c r="G45" s="29" t="s">
         <v>430</v>
       </c>
-      <c r="H45" s="32"/>
-      <c r="I45" s="33" t="s">
+      <c r="I45" s="29" t="s">
         <v>431</v>
       </c>
-      <c r="J45" s="33" t="s">
+      <c r="J45" s="29" t="s">
         <v>432</v>
       </c>
-      <c r="K45" s="33" t="s">
+      <c r="K45" s="29" t="s">
         <v>433</v>
       </c>
     </row>
@@ -4938,13 +4777,8 @@
       <c r="F46" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="G46" s="32"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32"/>
-      <c r="K46" s="32"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="15" t="s">
         <v>265</v>
       </c>
@@ -4959,13 +4793,8 @@
       <c r="F47" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
-    </row>
-    <row r="48" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A48" s="15" t="s">
         <v>268</v>
       </c>
@@ -4980,13 +4809,9 @@
       <c r="F48" s="19" t="s">
         <v>340</v>
       </c>
-      <c r="G48" s="33" t="s">
+      <c r="G48" s="29" t="s">
         <v>435</v>
       </c>
-      <c r="H48" s="32"/>
-      <c r="I48" s="32"/>
-      <c r="J48" s="32"/>
-      <c r="K48" s="32"/>
     </row>
     <row r="49" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="15" t="s">
@@ -5005,13 +4830,8 @@
       <c r="F49" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
-      <c r="I49" s="32"/>
-      <c r="J49" s="32"/>
-      <c r="K49" s="32"/>
-    </row>
-    <row r="50" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A50" s="15" t="s">
         <v>274</v>
       </c>
@@ -5026,13 +4846,8 @@
       <c r="F50" s="14" t="s">
         <v>341</v>
       </c>
-      <c r="G50" s="32"/>
-      <c r="H50" s="32"/>
-      <c r="I50" s="32"/>
-      <c r="J50" s="32"/>
-      <c r="K50" s="32"/>
-    </row>
-    <row r="51" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="15" t="s">
         <v>277</v>
       </c>
@@ -5047,21 +4862,20 @@
       <c r="F51" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="G51" s="32" t="s">
+      <c r="G51" t="s">
         <v>444</v>
       </c>
-      <c r="H51" s="32"/>
-      <c r="I51" s="32" t="s">
+      <c r="I51" t="s">
         <v>445</v>
       </c>
-      <c r="J51" s="32" t="s">
+      <c r="J51" t="s">
         <v>446</v>
       </c>
-      <c r="K51" s="32" t="s">
+      <c r="K51" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" ht="145" x14ac:dyDescent="0.35">
       <c r="A52" s="15" t="s">
         <v>281</v>
       </c>
@@ -5076,17 +4890,16 @@
       <c r="F52" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="G52" s="33" t="s">
+      <c r="G52" s="29" t="s">
         <v>362</v>
       </c>
-      <c r="H52" s="32"/>
-      <c r="I52" s="33" t="s">
+      <c r="I52" s="29" t="s">
         <v>421</v>
       </c>
-      <c r="J52" s="33" t="s">
+      <c r="J52" s="29" t="s">
         <v>422</v>
       </c>
-      <c r="K52" s="33" t="s">
+      <c r="K52" s="29" t="s">
         <v>423</v>
       </c>
     </row>
@@ -5105,17 +4918,16 @@
       <c r="F53" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="G53" s="36" t="s">
+      <c r="G53" s="34" t="s">
         <v>383</v>
       </c>
-      <c r="H53" s="32"/>
-      <c r="I53" s="36" t="s">
+      <c r="I53" s="34" t="s">
         <v>424</v>
       </c>
-      <c r="J53" s="36" t="s">
+      <c r="J53" s="34" t="s">
         <v>425</v>
       </c>
-      <c r="K53" s="36" t="s">
+      <c r="K53" s="34" t="s">
         <v>426</v>
       </c>
     </row>
@@ -5134,17 +4946,16 @@
       <c r="F54" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="G54" s="33" t="s">
+      <c r="G54" s="29" t="s">
         <v>448</v>
       </c>
-      <c r="H54" s="32"/>
-      <c r="I54" s="33" t="s">
+      <c r="I54" s="29" t="s">
         <v>449</v>
       </c>
-      <c r="J54" s="33" t="s">
+      <c r="J54" s="29" t="s">
         <v>450</v>
       </c>
-      <c r="K54" s="33" t="s">
+      <c r="K54" s="29" t="s">
         <v>451</v>
       </c>
     </row>
@@ -5165,21 +4976,20 @@
       <c r="F55" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="G55" s="33" t="s">
+      <c r="G55" s="29" t="s">
         <v>463</v>
       </c>
-      <c r="H55" s="32"/>
-      <c r="I55" s="33" t="s">
+      <c r="I55" s="29" t="s">
         <v>465</v>
       </c>
-      <c r="J55" s="33" t="s">
+      <c r="J55" s="29" t="s">
         <v>466</v>
       </c>
-      <c r="K55" s="33" t="s">
+      <c r="K55" s="29" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A56" s="15" t="s">
         <v>297</v>
       </c>
@@ -5194,42 +5004,38 @@
       <c r="F56" s="14" t="s">
         <v>300</v>
       </c>
-      <c r="G56" s="33" t="s">
+      <c r="G56" s="29" t="s">
         <v>359</v>
       </c>
-      <c r="H56" s="32"/>
-      <c r="I56" s="32"/>
-      <c r="J56" s="32"/>
-      <c r="K56" s="32"/>
-    </row>
-    <row r="57" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="37" t="s">
+    </row>
+    <row r="57" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="35" t="s">
         <v>301</v>
       </c>
-      <c r="B57" s="37" t="s">
+      <c r="B57" s="35" t="s">
         <v>302</v>
       </c>
-      <c r="C57" s="37" t="s">
+      <c r="C57" s="35" t="s">
         <v>303</v>
       </c>
-      <c r="D57" s="37"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="38" t="s">
+      <c r="D57" s="35"/>
+      <c r="E57" s="35"/>
+      <c r="F57" s="36" t="s">
         <v>304</v>
       </c>
-      <c r="G57" s="32" t="s">
+      <c r="G57" t="s">
         <v>360</v>
       </c>
-      <c r="H57" s="34" t="s">
+      <c r="H57" s="32" t="s">
         <v>396</v>
       </c>
-      <c r="I57" s="32" t="s">
+      <c r="I57" t="s">
         <v>427</v>
       </c>
-      <c r="J57" s="32" t="s">
+      <c r="J57" t="s">
         <v>428</v>
       </c>
-      <c r="K57" s="32" t="s">
+      <c r="K57" t="s">
         <v>429</v>
       </c>
     </row>
@@ -5252,42 +5058,38 @@
       <c r="F58" s="14" t="s">
         <v>308</v>
       </c>
-      <c r="G58" s="41" t="s">
+      <c r="G58" s="13" t="s">
         <v>380</v>
       </c>
-      <c r="H58" s="34" t="s">
+      <c r="H58" s="32" t="s">
         <v>397</v>
       </c>
-      <c r="I58" s="32"/>
-      <c r="J58" s="32"/>
-      <c r="K58" s="32"/>
     </row>
     <row r="59" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="39" t="s">
+      <c r="A59" s="37" t="s">
         <v>309</v>
       </c>
-      <c r="B59" s="39" t="s">
+      <c r="B59" s="37" t="s">
         <v>310</v>
       </c>
-      <c r="C59" s="39" t="s">
+      <c r="C59" s="37" t="s">
         <v>311</v>
       </c>
-      <c r="D59" s="39"/>
-      <c r="E59" s="39"/>
-      <c r="F59" s="40" t="s">
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="38" t="s">
         <v>312</v>
       </c>
-      <c r="G59" s="33" t="s">
+      <c r="G59" s="29" t="s">
         <v>464</v>
       </c>
-      <c r="H59" s="32"/>
-      <c r="I59" s="33" t="s">
+      <c r="I59" s="29" t="s">
         <v>468</v>
       </c>
-      <c r="J59" s="33" t="s">
+      <c r="J59" s="29" t="s">
         <v>469</v>
       </c>
-      <c r="K59" s="33" t="s">
+      <c r="K59" s="29" t="s">
         <v>470</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjusted VS jsonata mapping
</commit_message>
<xml_diff>
--- a/Maps/sdtm_mapping_paths.xlsx
+++ b/Maps/sdtm_mapping_paths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\SDTM_mapper\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352201F3-0064-4BF4-A66C-E399969A2CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3C77DA-A480-482A-ADAE-A90914173FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19890" yWindow="-18810" windowWidth="25080" windowHeight="15225" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -1653,18 +1653,6 @@
     <t>TV</t>
   </si>
   <si>
-    <t>study.versions.studyDesigns.encounters.label</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.encounters .scheduledAt.label</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.encounters .transitionEndRule .text</t>
-  </si>
-  <si>
-    <t>study.versions.studyDesigns.encounters.transitionStartRule.text</t>
-  </si>
-  <si>
     <t>study.versions.studyDesigns.($ElementName := function($id) {(elements[id=$id].label)}; studyCells.{armId: elementIds[0], elementIds[0]:$ElementName(elementIds[0])})</t>
   </si>
   <si>
@@ -1672,6 +1660,18 @@
   </si>
   <si>
     <t>study.versions.studyDesigns.($EpochName := function($id) {(epochs[id=$id].label)}; studyCells.{armId: elementIds[0], elementIds[0]: $EpochName(epochId)})</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.encounters.{id: label}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.encounters{id: scheduledAt.label}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.encounters{id: transitionEndRule .text}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.encounters{id: transitionStartRule.text}</t>
   </si>
 </sst>
 </file>
@@ -2439,8 +2439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CEFEB0-0887-1349-82EC-A63800D98F30}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="87" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="A2" zoomScale="87" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2619,7 +2619,7 @@
         <v>319</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
@@ -2642,7 +2642,7 @@
         <v>320</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
@@ -2705,7 +2705,7 @@
         <v>322</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -2933,8 +2933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143561C3-5632-DF4D-A3FB-55321D75FDD5}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3060,7 +3060,7 @@
         <v>64</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="H5" s="6"/>
     </row>
@@ -3084,7 +3084,7 @@
         <v>66</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -3156,7 +3156,7 @@
         <v>72</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="H9" s="6"/>
     </row>
@@ -3180,7 +3180,7 @@
         <v>74</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="H10" s="6"/>
     </row>
@@ -4466,7 +4466,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
         <v>216</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="15" t="s">
         <v>222</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="15" t="s">
         <v>227</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
         <v>230</v>
       </c>

</xml_diff>

<commit_message>
Added mapping for visitnum
</commit_message>
<xml_diff>
--- a/Maps/sdtm_mapping_paths.xlsx
+++ b/Maps/sdtm_mapping_paths.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\SDTM_mapper\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3C77DA-A480-482A-ADAE-A90914173FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414B724A-2AC2-4AC9-9A51-1C43F7DA565D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="496">
   <si>
     <t>Identifier</t>
   </si>
@@ -1672,6 +1672,9 @@
   </si>
   <si>
     <t>study.versions.studyDesigns.encounters{id: transitionStartRule.text}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.encounters{id: nextId}</t>
   </si>
 </sst>
 </file>
@@ -2934,7 +2937,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3037,7 +3040,9 @@
       <c r="F4" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="6"/>
+      <c r="G4" s="6" t="s">
+        <v>495</v>
+      </c>
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -3185,6 +3190,9 @@
       <c r="H10" s="6"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G4" r:id="rId1" display="StudyVersion/@studyDesigns/StudyDesign/@encounters/Encounter/@previous | @next" xr:uid="{9E71AD6D-8EE4-4E56-A308-8F4E2624D075}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added jsonata code for TA.taeord
</commit_message>
<xml_diff>
--- a/Maps/sdtm_mapping_paths.xlsx
+++ b/Maps/sdtm_mapping_paths.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\SDTM_mapper\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414B724A-2AC2-4AC9-9A51-1C43F7DA565D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5AAEA3-C4BA-464F-876B-592826C68F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10935" yWindow="-18585" windowWidth="25050" windowHeight="14370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="497">
   <si>
     <t>Identifier</t>
   </si>
@@ -1675,6 +1675,9 @@
   </si>
   <si>
     <t>study.versions.studyDesigns.encounters{id: nextId}</t>
+  </si>
+  <si>
+    <t>study.versions.studyDesigns.($Next := function($id) {(epochs[id=$id].nextId)}; studyCells.{armId: elementIds[0], elementIds[0]:$Next(EpochId)})</t>
   </si>
 </sst>
 </file>
@@ -2442,15 +2445,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CEFEB0-0887-1349-82EC-A63800D98F30}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="87" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="17.81640625" customWidth="1"/>
     <col min="6" max="6" width="25.81640625" customWidth="1"/>
-    <col min="7" max="7" width="28" style="29" customWidth="1"/>
+    <col min="7" max="7" width="83.6328125" style="29" customWidth="1"/>
     <col min="8" max="8" width="18.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2600,7 +2603,9 @@
       <c r="F6" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="13" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="118" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
@@ -2936,8 +2941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143561C3-5632-DF4D-A3FB-55321D75FDD5}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Simplified TI Code + resolving all tags now
</commit_message>
<xml_diff>
--- a/Maps/sdtm_mapping_paths.xlsx
+++ b/Maps/sdtm_mapping_paths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\USDM_SDTM_mapper\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E29AEE-7586-46FC-83C7-9578D4AC79B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7965E50-497D-4691-944B-F8AB1FC8FE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20115" yWindow="-18930" windowWidth="23295" windowHeight="15225" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -1774,18 +1774,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB7DEE8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1795,62 +1789,15 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1869,91 +1816,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1961,45 +1830,50 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2007,20 +1881,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2340,26 +2202,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="2" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="2" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -2367,70 +2229,70 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="B7" s="17"/>
+      <c r="B7" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="3" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="31" x14ac:dyDescent="0.35">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="3" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="31" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="3" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="31" x14ac:dyDescent="0.35">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="3" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
     </row>
     <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="B18" s="17"/>
+      <c r="B18" s="2"/>
     </row>
     <row r="20" spans="1:2" ht="62" x14ac:dyDescent="0.35">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="3" t="s">
         <v>477</v>
       </c>
     </row>
@@ -2438,7 +2300,7 @@
       <c r="A21" t="s">
         <v>478</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="5" t="s">
         <v>479</v>
       </c>
     </row>
@@ -2452,273 +2314,276 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="17.81640625" customWidth="1"/>
-    <col min="6" max="6" width="25.81640625" customWidth="1"/>
-    <col min="7" max="7" width="83.6328125" style="29" customWidth="1"/>
-    <col min="8" max="8" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" customWidth="1"/>
+    <col min="4" max="4" width="48.36328125" customWidth="1"/>
+    <col min="5" max="5" width="15.36328125" customWidth="1"/>
+    <col min="6" max="6" width="23.6328125" customWidth="1"/>
+    <col min="7" max="7" width="83.6328125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="43.6328125" customWidth="1"/>
+    <col min="9" max="9" width="43.453125" customWidth="1"/>
+    <col min="10" max="10" width="41.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" s="11" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="11" t="s">
         <v>355</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="11" t="s">
         <v>374</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="7" t="s">
         <v>496</v>
       </c>
-      <c r="H2" s="23"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="31" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="9" t="s">
         <v>459</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-    </row>
-    <row r="4" spans="1:11" ht="31" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="8" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="31" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="8" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="5" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="118" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="8" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="31" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="5" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="G10" s="6"/>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:11" ht="137.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="8" t="s">
         <v>495</v>
       </c>
     </row>
@@ -2732,47 +2597,46 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.36328125" customWidth="1"/>
     <col min="2" max="2" width="20.36328125" customWidth="1"/>
-    <col min="3" max="5" width="9.36328125" customWidth="1"/>
-    <col min="6" max="6" width="25.81640625" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" customWidth="1"/>
+    <col min="4" max="4" width="19.90625" customWidth="1"/>
+    <col min="5" max="5" width="31.36328125" customWidth="1"/>
+    <col min="6" max="6" width="30.7265625" customWidth="1"/>
     <col min="7" max="7" width="39.90625" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" style="29"/>
+    <col min="8" max="8" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="42" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:11" s="11" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="11" t="s">
         <v>355</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="11" t="s">
         <v>374</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
@@ -2790,16 +2654,16 @@
       <c r="E2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="7" t="s">
         <v>496</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
@@ -2817,14 +2681,14 @@
       <c r="E3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="26"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
@@ -2842,10 +2706,10 @@
       <c r="E4" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="5" t="s">
         <v>481</v>
       </c>
     </row>
@@ -2865,10 +2729,10 @@
       <c r="E5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="5" t="s">
         <v>482</v>
       </c>
     </row>
@@ -2888,10 +2752,10 @@
       <c r="E6" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="13" t="s">
         <v>323</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="5" t="s">
         <v>483</v>
       </c>
     </row>
@@ -2911,10 +2775,10 @@
       <c r="E7" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="13" t="s">
         <v>324</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="5" t="s">
         <v>484</v>
       </c>
     </row>
@@ -2934,7 +2798,7 @@
       <c r="E8" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="13" t="s">
         <v>325</v>
       </c>
     </row>
@@ -2948,257 +2812,260 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="18.6328125" customWidth="1"/>
-    <col min="3" max="5" width="9.6328125" customWidth="1"/>
-    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="4" max="4" width="20.36328125" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+    <col min="6" max="6" width="24.08984375" customWidth="1"/>
     <col min="7" max="7" width="47" customWidth="1"/>
-    <col min="8" max="8" width="19.453125" customWidth="1"/>
+    <col min="8" max="8" width="34.6328125" customWidth="1"/>
+    <col min="9" max="9" width="32.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" s="11" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="11" t="s">
         <v>355</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="11" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="7" t="s">
         <v>496</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6" t="s">
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8" t="s">
         <v>486</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="8" t="s">
         <v>491</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="5" t="s">
         <v>487</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="5" t="s">
         <v>488</v>
       </c>
-      <c r="H6" s="6"/>
+      <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="5" t="s">
         <v>460</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="5" t="s">
         <v>461</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="8" t="s">
         <v>489</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="8" t="s">
         <v>490</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3210,51 +3077,66 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A2D413-6E3B-5A40-9DE8-0245851A536D}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="18.6328125" customWidth="1"/>
+    <col min="1" max="2" width="18.6328125" customWidth="1"/>
+    <col min="3" max="3" width="14.36328125" customWidth="1"/>
+    <col min="4" max="4" width="22.90625" customWidth="1"/>
+    <col min="5" max="5" width="54.1796875" style="5" customWidth="1"/>
     <col min="6" max="6" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.6328125" style="28" customWidth="1"/>
-    <col min="8" max="8" width="29.81640625" style="16" customWidth="1"/>
-    <col min="9" max="11" width="8.6328125" style="16"/>
+    <col min="7" max="7" width="51.6328125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="36.26953125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="47.90625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="47.7265625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="56.08984375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="57.26953125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="63.7265625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="46.54296875" style="5" customWidth="1"/>
+    <col min="15" max="15" width="51.7265625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="10.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:16" s="11" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="15" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="11" t="s">
         <v>355</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="11" t="s">
         <v>374</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-    </row>
-    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+    </row>
+    <row r="2" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>41</v>
       </c>
@@ -3270,15 +3152,14 @@
       <c r="E2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="7" t="s">
         <v>496</v>
       </c>
-      <c r="H2" s="23"/>
-    </row>
-    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>44</v>
       </c>
@@ -3294,13 +3175,13 @@
       <c r="E3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="26"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="9" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>77</v>
       </c>
@@ -3316,15 +3197,14 @@
       <c r="E4" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="H4" s="23"/>
-    </row>
-    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>79</v>
       </c>
@@ -3340,15 +3220,14 @@
       <c r="E5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="5" t="s">
         <v>457</v>
       </c>
-      <c r="H5" s="23"/>
-    </row>
-    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>81</v>
       </c>
@@ -3364,15 +3243,14 @@
       <c r="E6" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="H6" s="23"/>
-    </row>
-    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>83</v>
       </c>
@@ -3388,15 +3266,14 @@
       <c r="E7" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="H7" s="23"/>
-    </row>
-    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>85</v>
       </c>
@@ -3412,11 +3289,10 @@
       <c r="E8" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="23"/>
-    </row>
-    <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="F8" s="14"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>87</v>
       </c>
@@ -3432,13 +3308,12 @@
       <c r="E9" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="8" t="s">
         <v>458</v>
       </c>
-      <c r="H9" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3447,54 +3322,59 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF8120D-B51B-094C-AABA-CA55EB26DD5D}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.6328125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="21.453125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="26.6328125" style="16" customWidth="1"/>
-    <col min="8" max="8" width="29.81640625" style="16" customWidth="1"/>
-    <col min="9" max="16384" width="8.6328125" style="16"/>
+    <col min="1" max="1" width="19.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.36328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="38.90625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="58.6328125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.6328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:16" s="11" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="11" t="s">
         <v>355</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="11" t="s">
         <v>374</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-    </row>
-    <row r="2" spans="1:11" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+    </row>
+    <row r="2" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>41</v>
       </c>
@@ -3510,15 +3390,14 @@
       <c r="E2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="7" t="s">
         <v>496</v>
       </c>
-      <c r="H2" s="23"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>44</v>
       </c>
@@ -3534,13 +3413,13 @@
       <c r="E3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="22"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="9" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>90</v>
       </c>
@@ -3556,11 +3435,10 @@
       <c r="E4" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F4" s="13"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>92</v>
       </c>
@@ -3576,11 +3454,10 @@
       <c r="E5" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="23"/>
-    </row>
-    <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F5" s="13"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>94</v>
       </c>
@@ -3596,11 +3473,10 @@
       <c r="E6" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="23"/>
-    </row>
-    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="F6" s="13"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>96</v>
       </c>
@@ -3616,11 +3492,10 @@
       <c r="E7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="23"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F7" s="13"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>98</v>
       </c>
@@ -3636,11 +3511,10 @@
       <c r="E8" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="23"/>
-    </row>
-    <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="F8" s="13"/>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>101</v>
       </c>
@@ -3656,11 +3530,10 @@
       <c r="E9" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="23"/>
-    </row>
-    <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="F9" s="13"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>103</v>
       </c>
@@ -3676,11 +3549,10 @@
       <c r="E10" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="23"/>
-    </row>
-    <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="F10" s="13"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>105</v>
       </c>
@@ -3696,15 +3568,14 @@
       <c r="E11" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="H11" s="23"/>
-    </row>
-    <row r="12" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>107</v>
       </c>
@@ -3720,13 +3591,12 @@
       <c r="E12" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="10" t="s">
         <v>376</v>
       </c>
-      <c r="H12" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3735,10 +3605,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DEA66B-9A3B-A542-95A2-9E48A8B13E1D}">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:P132"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScale="109" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3749,541 +3619,546 @@
     <col min="4" max="4" width="28.6328125" customWidth="1"/>
     <col min="5" max="5" width="33.81640625" customWidth="1"/>
     <col min="6" max="6" width="32.453125" customWidth="1"/>
-    <col min="7" max="7" width="59.36328125" customWidth="1"/>
+    <col min="7" max="7" width="68.6328125" customWidth="1"/>
     <col min="8" max="8" width="27.7265625" customWidth="1"/>
     <col min="9" max="9" width="30.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="43.453125" customWidth="1"/>
     <col min="11" max="11" width="35.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:16" s="11" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="11" t="s">
         <v>390</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="11" t="s">
         <v>391</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="11" t="s">
         <v>392</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="15" t="s">
         <v>393</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="15" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="14" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="17" t="s">
         <v>326</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="18" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="116" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:16" ht="116" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="14" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17" t="s">
         <v>327</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="5" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:16" ht="87" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="14" t="s">
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17" t="s">
         <v>328</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="H4" s="16" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="17" t="s">
         <v>329</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="5" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="17" t="s">
         <v>330</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="5" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="29" t="s">
+      <c r="F7" s="17"/>
+      <c r="G7" s="5" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="17" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="17" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="17" t="s">
         <v>377</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="5" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
+    <row r="11" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="17" t="s">
         <v>331</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="5" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+    <row r="12" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="14" t="s">
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="G12" s="29" t="s">
+      <c r="G12" s="5" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="17" t="s">
         <v>332</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="G13" s="5" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="5" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
+    <row r="15" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="17" t="s">
         <v>333</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="I15" s="29" t="s">
+      <c r="I15" s="5" t="s">
         <v>397</v>
       </c>
-      <c r="J15" s="29" t="s">
+      <c r="J15" s="5" t="s">
         <v>398</v>
       </c>
-      <c r="K15" s="29" t="s">
+      <c r="K15" s="5" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
+    <row r="16" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="A16" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="17" t="s">
         <v>334</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="I16" s="29" t="s">
+      <c r="I16" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="J16" s="29" t="s">
+      <c r="J16" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="K16" s="29" t="s">
+      <c r="K16" s="5" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="14" t="s">
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="G17" s="33" t="s">
+      <c r="G17" s="19" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="14" t="s">
+      <c r="E18" s="16"/>
+      <c r="F18" s="17" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="14" t="s">
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17" t="s">
         <v>438</v>
       </c>
-      <c r="G19" s="29" t="s">
+      <c r="G19" s="5" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="14" t="s">
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="17" t="s">
         <v>335</v>
       </c>
-      <c r="G20" s="29" t="s">
+      <c r="G20" s="5" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="14" t="s">
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="G21" s="34" t="s">
+      <c r="G21" s="20" t="s">
         <v>361</v>
       </c>
-      <c r="I21" s="34" t="s">
+      <c r="I21" s="20" t="s">
         <v>403</v>
       </c>
-      <c r="J21" s="34" t="s">
+      <c r="J21" s="20" t="s">
         <v>404</v>
       </c>
-      <c r="K21" s="34" t="s">
+      <c r="K21" s="20" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="G22" s="29" t="s">
+      <c r="G22" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="I22" s="29" t="s">
+      <c r="I22" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="J22" s="29" t="s">
+      <c r="J22" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="K22" s="29" t="s">
+      <c r="K22" s="5" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="13" t="s">
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="G23" s="29" t="s">
+      <c r="G23" s="5" t="s">
         <v>409</v>
       </c>
       <c r="H23" t="s">
@@ -4291,157 +4166,157 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="14" t="s">
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="17" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="14" t="s">
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="G25" s="39" t="s">
+      <c r="G25" s="20" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="14" t="s">
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="G26" s="34" t="s">
+      <c r="G26" s="20" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="14" t="s">
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="17" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="G28" s="29" t="s">
+      <c r="G28" s="5" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="G29" s="29" t="s">
+      <c r="G29" s="5" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="G30" s="29" t="s">
+      <c r="G30" s="5" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="14" t="s">
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="17" t="s">
         <v>210</v>
       </c>
       <c r="G31" t="s">
@@ -4458,205 +4333,205 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="14" t="s">
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="G32" s="34" t="s">
+      <c r="G32" s="20" t="s">
         <v>365</v>
       </c>
-      <c r="I32" s="34" t="s">
+      <c r="I32" s="20" t="s">
         <v>414</v>
       </c>
-      <c r="J32" s="34" t="s">
+      <c r="J32" s="20" t="s">
         <v>415</v>
       </c>
-      <c r="K32" s="34" t="s">
+      <c r="K32" s="20" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="14" t="s">
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="17" t="s">
         <v>337</v>
       </c>
-      <c r="G33" s="34" t="s">
+      <c r="G33" s="20" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="14" t="s">
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="G34" s="34" t="s">
+      <c r="G34" s="20" t="s">
         <v>367</v>
       </c>
-      <c r="I34" s="34" t="s">
+      <c r="I34" s="20" t="s">
         <v>417</v>
       </c>
-      <c r="J34" s="34" t="s">
+      <c r="J34" s="20" t="s">
         <v>418</v>
       </c>
-      <c r="K34" s="34" t="s">
+      <c r="K34" s="20" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="F35" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="G35" s="29" t="s">
+      <c r="G35" s="5" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="E36" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="G36" s="29" t="s">
+      <c r="G36" s="5" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="E37" s="15" t="s">
+      <c r="E37" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="F37" s="14" t="s">
+      <c r="F37" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="G37" s="29" t="s">
+      <c r="G37" s="5" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15" t="s">
+      <c r="D38" s="16"/>
+      <c r="E38" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="G38" s="29" t="s">
+      <c r="G38" s="5" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="14" t="s">
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="G39" s="29" t="s">
+      <c r="G39" s="5" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="116" x14ac:dyDescent="0.35">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="14" t="s">
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="17" t="s">
         <v>338</v>
       </c>
-      <c r="G40" s="29" t="s">
+      <c r="G40" s="5" t="s">
         <v>363</v>
       </c>
       <c r="H40" t="s">
@@ -4664,155 +4539,155 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20" t="s">
+      <c r="D41" s="16"/>
+      <c r="E41" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="F41" s="14" t="s">
+      <c r="F41" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="G41" s="34" t="s">
+      <c r="G41" s="20" t="s">
         <v>382</v>
       </c>
       <c r="H41" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A42" s="15" t="s">
+    <row r="42" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="14" t="s">
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="G42" s="29" t="s">
+      <c r="G42" s="5" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="14" t="s">
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="G43" s="34" t="s">
+      <c r="G43" s="20" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="E44" s="20" t="s">
+      <c r="E44" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="F44" s="14" t="s">
+      <c r="F44" s="17" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="D45" s="20" t="s">
+      <c r="D45" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E45" s="20" t="s">
+      <c r="E45" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="F45" s="14" t="s">
+      <c r="F45" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="G45" s="29" t="s">
+      <c r="G45" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="I45" s="29" t="s">
+      <c r="I45" s="5" t="s">
         <v>430</v>
       </c>
-      <c r="J45" s="29" t="s">
+      <c r="J45" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="K45" s="29" t="s">
+      <c r="K45" s="5" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="D46" s="20" t="s">
+      <c r="D46" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E46" s="20" t="s">
+      <c r="E46" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="F46" s="14" t="s">
+      <c r="F46" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="G46" s="29" t="s">
+      <c r="G46" s="5" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="16" t="s">
         <v>265</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="C47" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="14" t="s">
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="17" t="s">
         <v>265</v>
       </c>
       <c r="G47" t="s">
@@ -4820,71 +4695,71 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="16" t="s">
         <v>268</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="C48" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="19" t="s">
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="21" t="s">
         <v>340</v>
       </c>
-      <c r="G48" s="29" t="s">
+      <c r="G48" s="5" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="16" t="s">
         <v>272</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="C49" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="D49" s="20" t="s">
+      <c r="D49" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="E49" s="20"/>
-      <c r="F49" s="14" t="s">
+      <c r="E49" s="16"/>
+      <c r="F49" s="17" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="16" t="s">
         <v>274</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="14" t="s">
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="17" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="15" t="s">
+      <c r="A51" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="C51" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="14" t="s">
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="17" t="s">
         <v>280</v>
       </c>
       <c r="G51" t="s">
@@ -4901,157 +4776,157 @@
       </c>
     </row>
     <row r="52" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A52" s="15" t="s">
+      <c r="A52" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="14" t="s">
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="G52" s="29" t="s">
+      <c r="G52" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="I52" s="29" t="s">
+      <c r="I52" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="J52" s="29" t="s">
+      <c r="J52" s="5" t="s">
         <v>421</v>
       </c>
-      <c r="K52" s="29" t="s">
+      <c r="K52" s="5" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="C53" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="14" t="s">
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="17" t="s">
         <v>288</v>
       </c>
-      <c r="G53" s="34" t="s">
+      <c r="G53" s="20" t="s">
         <v>383</v>
       </c>
-      <c r="I53" s="34" t="s">
+      <c r="I53" s="20" t="s">
         <v>423</v>
       </c>
-      <c r="J53" s="34" t="s">
+      <c r="J53" s="20" t="s">
         <v>424</v>
       </c>
-      <c r="K53" s="34" t="s">
+      <c r="K53" s="20" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="16" t="s">
         <v>289</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="C54" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="14" t="s">
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="17" t="s">
         <v>289</v>
       </c>
-      <c r="G54" s="29" t="s">
+      <c r="G54" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="I54" s="29" t="s">
+      <c r="I54" s="5" t="s">
         <v>448</v>
       </c>
-      <c r="J54" s="29" t="s">
+      <c r="J54" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="K54" s="29" t="s">
+      <c r="K54" s="5" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="16" t="s">
         <v>293</v>
       </c>
-      <c r="C55" s="15" t="s">
+      <c r="C55" s="16" t="s">
         <v>294</v>
       </c>
-      <c r="D55" s="15" t="s">
+      <c r="D55" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="E55" s="15"/>
-      <c r="F55" s="14" t="s">
+      <c r="E55" s="16"/>
+      <c r="F55" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="G55" s="29" t="s">
+      <c r="G55" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="I55" s="29" t="s">
+      <c r="I55" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="J55" s="29" t="s">
+      <c r="J55" s="5" t="s">
         <v>465</v>
       </c>
-      <c r="K55" s="29" t="s">
+      <c r="K55" s="5" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="16" t="s">
         <v>297</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="C56" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="14" t="s">
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="17" t="s">
         <v>300</v>
       </c>
-      <c r="G56" s="29" t="s">
+      <c r="G56" s="5" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="B57" s="35" t="s">
+      <c r="B57" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="C57" s="35" t="s">
+      <c r="C57" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="36" t="s">
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="17" t="s">
         <v>304</v>
       </c>
       <c r="G57" t="s">
         <v>360</v>
       </c>
-      <c r="H57" s="32" t="s">
+      <c r="H57" s="16" t="s">
         <v>395</v>
       </c>
       <c r="I57" t="s">
@@ -5065,59 +4940,127 @@
       </c>
     </row>
     <row r="58" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="15" t="s">
+      <c r="A58" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B58" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C58" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="D58" s="15" t="s">
+      <c r="D58" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="E58" s="15" t="s">
+      <c r="E58" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="F58" s="14" t="s">
+      <c r="F58" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="G58" s="13" t="s">
+      <c r="G58" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="H58" s="32" t="s">
+      <c r="H58" s="16" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="37" t="s">
+      <c r="A59" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="B59" s="37" t="s">
+      <c r="B59" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="C59" s="37" t="s">
+      <c r="C59" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="38" t="s">
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="G59" s="29" t="s">
+      <c r="G59" s="5" t="s">
         <v>463</v>
       </c>
-      <c r="I59" s="29" t="s">
+      <c r="I59" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="J59" s="29" t="s">
+      <c r="J59" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="K59" s="29" t="s">
+      <c r="K59" s="5" t="s">
         <v>469</v>
       </c>
     </row>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="82" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="83" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="84" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="85" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="86" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="87" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="88" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="89" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="90" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="91" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="92" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="93" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="94" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="95" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="96" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="97" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="98" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="99" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="100" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="101" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="102" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="103" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="104" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="105" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="106" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="107" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="108" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="109" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="110" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="111" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="112" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="113" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="114" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="115" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="116" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="117" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="118" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="119" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="120" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="121" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="122" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="123" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="124" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="125" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="126" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="127" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="128" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="129" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="130" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="131" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="132" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <autoFilter ref="A1:G59" xr:uid="{A2DEA66B-9A3B-A542-95A2-9E48A8B13E1D}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>